<commit_message>
sanitized database to prevent parsing errors
Issues were caused by " and ; symbols occurring within the database entries as well as "Sp." entries, which were replaced by values retrieved from https://www.wikifit.de/kalorientabelle
</commit_message>
<xml_diff>
--- a/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
+++ b/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\NutriLearnVR\NutriLearnVR\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB7F80C8-3700-4D99-B62D-618CEA3B8057}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310871BC-CA58-4354-BFE5-D3C4A194A888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8C58FACA-B588-4A2F-A614-585794A6AB4A}"/>
   </bookViews>
@@ -29,7 +29,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="773" uniqueCount="342">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="340">
   <si>
     <t>ID</t>
   </si>
@@ -115,9 +115,6 @@
     <t>Früchte/Früchte gekocht (inkl. Konserven)</t>
   </si>
   <si>
-    <t>Sp.</t>
-  </si>
-  <si>
     <t>Ananas, roh</t>
   </si>
   <si>
@@ -136,9 +133,6 @@
     <t>Apfel, roh</t>
   </si>
   <si>
-    <t>Süssigkeiten/Kuchen, Torten und Cake;Gerichte/Kuchen und Gratins</t>
-  </si>
-  <si>
     <t>Apfelmus, gezuckert (Konserve)</t>
   </si>
   <si>
@@ -148,9 +142,6 @@
     <t>Apfelsaft</t>
   </si>
   <si>
-    <t>Früchte/Fruchtsäfte;Alkoholfreie Getränke/Frucht- und Gemüsesäfte</t>
-  </si>
-  <si>
     <t>Milch und Milchprodukte/Hartkäse</t>
   </si>
   <si>
@@ -178,24 +169,15 @@
     <t>Avocado, roh</t>
   </si>
   <si>
-    <t>Gemüse/Gemüse frisch;Nüsse, Samen und Ölfrüchte</t>
-  </si>
-  <si>
     <t>Bäckerhefe, gepresst</t>
   </si>
   <si>
-    <t>Verschiedenes/Hefe;Verschiedenes/Backzutaten</t>
-  </si>
-  <si>
     <t>Balsamicoessig</t>
   </si>
   <si>
     <t>Verschiedenes/Salz, Gewürze und Aromen</t>
   </si>
   <si>
-    <t>&lt;0.6</t>
-  </si>
-  <si>
     <t>Bami Goreng, zubereitet</t>
   </si>
   <si>
@@ -277,9 +259,6 @@
     <t>Bratbutter</t>
   </si>
   <si>
-    <t>Fette und Öle/Fette;Milch und Milchprodukte/Rahm und Butter</t>
-  </si>
-  <si>
     <t>Milch und Milchprodukte/Weichkäse</t>
   </si>
   <si>
@@ -331,9 +310,6 @@
     <t>Cannelloni mit Spinat-Ricotta-Füllung, zubereitet</t>
   </si>
   <si>
-    <t>Milch und Milchprodukte/Milch- und Joghurtgetränke;Alkoholfreie Getränke/Kaffee</t>
-  </si>
-  <si>
     <t>Cashewnuss</t>
   </si>
   <si>
@@ -400,9 +376,6 @@
     <t>Gerichte/Sandwiches</t>
   </si>
   <si>
-    <t>Fette und Öle/Rahm;Milch und Milchprodukte/Rahm und Butter</t>
-  </si>
-  <si>
     <t>Fisch/Meeresfische</t>
   </si>
   <si>
@@ -481,9 +454,6 @@
     <t xml:space="preserve">Fleisch (Durchschnitt exkl. Innereien), roh </t>
   </si>
   <si>
-    <t>Fleisch und Innereien/Kalb;Fleisch und Innereien/Geflügel;Fleisch und Innereien/Lamm, Schaf;Fleisch und Innereien/Rind;Fleisch und Innereien/Schwein;Fleisch und Innereien/Wild</t>
-  </si>
-  <si>
     <t>Fleischlasagne, zubereitet</t>
   </si>
   <si>
@@ -523,9 +493,6 @@
     <t>Gehacktes (Durchschnitt aus Rind, Kalb, Schwein, Poulet), roh</t>
   </si>
   <si>
-    <t>Fleisch und Innereien/Kalb;Fleisch und Innereien/Rind;Fleisch und Innereien/Schwein;Fleisch und Innereien/Geflügel</t>
-  </si>
-  <si>
     <t>Gemüselasagne, zubereitet</t>
   </si>
   <si>
@@ -700,9 +667,6 @@
     <t>Margarine, 35 - 40 % Fett</t>
   </si>
   <si>
-    <t>Fette und Öle/Fette;Fette und Öle/Fette</t>
-  </si>
-  <si>
     <t>Marmorkuchen</t>
   </si>
   <si>
@@ -736,9 +700,6 @@
     <t>Mozzarella</t>
   </si>
   <si>
-    <t>Milch und Milchprodukte/Weichkäse;Milch und Milchprodukte/Frischkäse und Quark</t>
-  </si>
-  <si>
     <t xml:space="preserve">Müeslimischung, Getreideflocken mit Früchten und Nüssen, gezuckert </t>
   </si>
   <si>
@@ -841,15 +802,9 @@
     <t>Reis unpoliert, gekocht in Salzwasser (unjodiert)</t>
   </si>
   <si>
-    <t>Rind, Entrecôte, "medium" gebraten (ohne Zusatz von Fett und Salz)</t>
-  </si>
-  <si>
     <t>Rind, Entrecôte, roh</t>
   </si>
   <si>
-    <t>Rind, Filet, "medium" gebraten (ohne Zustatz von Fett und Salz)</t>
-  </si>
-  <si>
     <t>Rind, Filet, roh</t>
   </si>
   <si>
@@ -1055,6 +1010,45 @@
   </si>
   <si>
     <t>Rinderhack, roh</t>
+  </si>
+  <si>
+    <t>Gemüse/Gemüse frisch/Nüsse, Samen und Ölfrüchte</t>
+  </si>
+  <si>
+    <t>Früchte/Fruchtsäfte/Alkoholfreie Getränke/Frucht- und Gemüsesäfte</t>
+  </si>
+  <si>
+    <t>Verschiedenes/Hefe/Verschiedenes/Backzutaten</t>
+  </si>
+  <si>
+    <t>Fette und Öle/Fette/Milch und Milchprodukte/Rahm und Butter</t>
+  </si>
+  <si>
+    <t>Süssigkeiten/Kuchen, Torten und Cake/Gerichte/Kuchen und Gratins</t>
+  </si>
+  <si>
+    <t>Milch und Milchprodukte/Milch- und Joghurtgetränke/Alkoholfreie Getränke/Kaffee</t>
+  </si>
+  <si>
+    <t>Fette und Öle/Fette/Fette und Öle/Fette</t>
+  </si>
+  <si>
+    <t>Milch und Milchprodukte/Weichkäse/Milch und Milchprodukte/Frischkäse und Quark</t>
+  </si>
+  <si>
+    <t>Fette und Öle/Rahm/Milch und Milchprodukte/Rahm und Butter</t>
+  </si>
+  <si>
+    <t>Fleisch und Innereien/Kalb/Fleisch und Innereien/Geflügel/Fleisch und Innereien/Lamm, Schaf/Fleisch und Innereien/Rind/Fleisch und Innereien/Schwein/Fleisch und Innereien/Wild</t>
+  </si>
+  <si>
+    <t>Fleisch und Innereien/Kalb/Fleisch und Innereien/Rind/Fleisch und Innereien/Schwein/Fleisch und Innereien/Geflügel</t>
+  </si>
+  <si>
+    <t>Rind, Entrecôte, medium gebraten (ohne Zusatz von Fett und Salz)</t>
+  </si>
+  <si>
+    <t>Rind, Filet, medium gebraten (ohne Zustatz von Fett und Salz)</t>
   </si>
 </sst>
 </file>
@@ -1444,8 +1438,8 @@
   <dimension ref="A1:I238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft"/>
+      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E152" sqref="E152"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1572,7 +1566,7 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C5">
         <v>52</v>
@@ -1590,7 +1584,7 @@
         <v>15</v>
       </c>
       <c r="H5" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
@@ -1598,7 +1592,7 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C6">
         <v>51</v>
@@ -1616,7 +1610,7 @@
         <v>15</v>
       </c>
       <c r="H6" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="I6">
         <v>1.05</v>
@@ -1627,7 +1621,7 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C7">
         <v>52</v>
@@ -1645,7 +1639,7 @@
         <v>15</v>
       </c>
       <c r="H7" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
@@ -1653,7 +1647,7 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="C8">
         <v>89</v>
@@ -1679,7 +1673,7 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C9">
         <v>55</v>
@@ -1705,7 +1699,7 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C10">
         <v>50</v>
@@ -1723,7 +1717,7 @@
         <v>21</v>
       </c>
       <c r="H10" t="s">
-        <v>39</v>
+        <v>328</v>
       </c>
       <c r="I10">
         <v>1.04</v>
@@ -1734,7 +1728,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="C11">
         <v>44</v>
@@ -1752,7 +1746,7 @@
         <v>15</v>
       </c>
       <c r="H11" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
@@ -1760,7 +1754,7 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="C12">
         <v>21</v>
@@ -1778,7 +1772,7 @@
         <v>15</v>
       </c>
       <c r="H12" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -1786,7 +1780,7 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>45</v>
+        <v>42</v>
       </c>
       <c r="C13">
         <v>136</v>
@@ -1812,7 +1806,7 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>46</v>
+        <v>43</v>
       </c>
       <c r="C14">
         <v>276</v>
@@ -1830,7 +1824,7 @@
         <v>15</v>
       </c>
       <c r="H14" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
@@ -1838,7 +1832,7 @@
         <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>48</v>
+        <v>45</v>
       </c>
       <c r="C15">
         <v>158</v>
@@ -1856,7 +1850,7 @@
         <v>15</v>
       </c>
       <c r="H15" t="s">
-        <v>49</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1864,7 +1858,7 @@
         <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>50</v>
+        <v>46</v>
       </c>
       <c r="C16">
         <v>96</v>
@@ -1882,7 +1876,7 @@
         <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>51</v>
+        <v>329</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -1890,13 +1884,13 @@
         <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>52</v>
+        <v>47</v>
       </c>
       <c r="C17">
         <v>128</v>
       </c>
-      <c r="D17" t="s">
-        <v>54</v>
+      <c r="D17">
+        <v>0.6</v>
       </c>
       <c r="E17">
         <v>25.8</v>
@@ -1908,7 +1902,7 @@
         <v>15</v>
       </c>
       <c r="H17" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
@@ -1916,7 +1910,7 @@
         <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>57</v>
+        <v>51</v>
       </c>
       <c r="C18">
         <v>89</v>
@@ -1934,7 +1928,7 @@
         <v>15</v>
       </c>
       <c r="H18" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
@@ -1942,7 +1936,7 @@
         <v>18</v>
       </c>
       <c r="B19" t="s">
-        <v>58</v>
+        <v>52</v>
       </c>
       <c r="C19">
         <v>46</v>
@@ -1960,7 +1954,7 @@
         <v>15</v>
       </c>
       <c r="H19" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
@@ -1968,7 +1962,7 @@
         <v>19</v>
       </c>
       <c r="B20" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="C20">
         <v>241</v>
@@ -1986,7 +1980,7 @@
         <v>15</v>
       </c>
       <c r="H20" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
@@ -1994,7 +1988,7 @@
         <v>20</v>
       </c>
       <c r="B21" t="s">
-        <v>66</v>
+        <v>60</v>
       </c>
       <c r="C21">
         <v>40</v>
@@ -2012,7 +2006,7 @@
         <v>15</v>
       </c>
       <c r="H21" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
@@ -2020,7 +2014,7 @@
         <v>21</v>
       </c>
       <c r="B22" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="C22">
         <v>54</v>
@@ -2038,7 +2032,7 @@
         <v>15</v>
       </c>
       <c r="H22" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
@@ -2046,7 +2040,7 @@
         <v>22</v>
       </c>
       <c r="B23" t="s">
-        <v>71</v>
+        <v>65</v>
       </c>
       <c r="C23">
         <v>52</v>
@@ -2064,7 +2058,7 @@
         <v>21</v>
       </c>
       <c r="H23" t="s">
-        <v>39</v>
+        <v>328</v>
       </c>
       <c r="I23">
         <v>1.04</v>
@@ -2075,7 +2069,7 @@
         <v>23</v>
       </c>
       <c r="B24" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C24">
         <v>19</v>
@@ -2093,7 +2087,7 @@
         <v>15</v>
       </c>
       <c r="H24" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
@@ -2101,7 +2095,7 @@
         <v>24</v>
       </c>
       <c r="B25" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C25">
         <v>360</v>
@@ -2119,7 +2113,7 @@
         <v>15</v>
       </c>
       <c r="H25" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
@@ -2127,7 +2121,7 @@
         <v>25</v>
       </c>
       <c r="B26" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C26">
         <v>26</v>
@@ -2145,7 +2139,7 @@
         <v>15</v>
       </c>
       <c r="H26" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
@@ -2153,7 +2147,7 @@
         <v>26</v>
       </c>
       <c r="B27" t="s">
-        <v>78</v>
+        <v>72</v>
       </c>
       <c r="C27">
         <v>32</v>
@@ -2171,7 +2165,7 @@
         <v>15</v>
       </c>
       <c r="H27" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
@@ -2179,7 +2173,7 @@
         <v>27</v>
       </c>
       <c r="B28" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C28">
         <v>885</v>
@@ -2197,7 +2191,7 @@
         <v>15</v>
       </c>
       <c r="H28" t="s">
-        <v>82</v>
+        <v>330</v>
       </c>
       <c r="I28">
         <v>0.9</v>
@@ -2208,7 +2202,7 @@
         <v>28</v>
       </c>
       <c r="B29" t="s">
-        <v>84</v>
+        <v>77</v>
       </c>
       <c r="C29">
         <v>39</v>
@@ -2226,7 +2220,7 @@
         <v>15</v>
       </c>
       <c r="H29" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
@@ -2234,7 +2228,7 @@
         <v>29</v>
       </c>
       <c r="B30" t="s">
-        <v>85</v>
+        <v>78</v>
       </c>
       <c r="C30">
         <v>47</v>
@@ -2252,7 +2246,7 @@
         <v>15</v>
       </c>
       <c r="H30" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
@@ -2260,7 +2254,7 @@
         <v>30</v>
       </c>
       <c r="B31" t="s">
-        <v>86</v>
+        <v>79</v>
       </c>
       <c r="C31">
         <v>264</v>
@@ -2278,7 +2272,7 @@
         <v>15</v>
       </c>
       <c r="H31" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
@@ -2286,7 +2280,7 @@
         <v>31</v>
       </c>
       <c r="B32" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C32">
         <v>348</v>
@@ -2304,7 +2298,7 @@
         <v>15</v>
       </c>
       <c r="H32" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
@@ -2312,7 +2306,7 @@
         <v>32</v>
       </c>
       <c r="B33" t="s">
-        <v>92</v>
+        <v>85</v>
       </c>
       <c r="C33">
         <v>34</v>
@@ -2330,7 +2324,7 @@
         <v>21</v>
       </c>
       <c r="H33" t="s">
-        <v>93</v>
+        <v>86</v>
       </c>
       <c r="I33">
         <v>1</v>
@@ -2341,7 +2335,7 @@
         <v>33</v>
       </c>
       <c r="B34" t="s">
-        <v>94</v>
+        <v>87</v>
       </c>
       <c r="C34">
         <v>325</v>
@@ -2359,7 +2353,7 @@
         <v>15</v>
       </c>
       <c r="H34" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
@@ -2367,7 +2361,7 @@
         <v>34</v>
       </c>
       <c r="B35" t="s">
-        <v>96</v>
+        <v>89</v>
       </c>
       <c r="C35">
         <v>355</v>
@@ -2385,7 +2379,7 @@
         <v>15</v>
       </c>
       <c r="H35" t="s">
-        <v>83</v>
+        <v>76</v>
       </c>
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
@@ -2393,7 +2387,7 @@
         <v>35</v>
       </c>
       <c r="B36" t="s">
-        <v>97</v>
+        <v>90</v>
       </c>
       <c r="C36">
         <v>177</v>
@@ -2411,7 +2405,7 @@
         <v>15</v>
       </c>
       <c r="H36" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
@@ -2419,7 +2413,7 @@
         <v>36</v>
       </c>
       <c r="B37" t="s">
-        <v>99</v>
+        <v>92</v>
       </c>
       <c r="C37">
         <v>221</v>
@@ -2437,7 +2431,7 @@
         <v>15</v>
       </c>
       <c r="H37" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
@@ -2445,7 +2439,7 @@
         <v>37</v>
       </c>
       <c r="B38" t="s">
-        <v>101</v>
+        <v>93</v>
       </c>
       <c r="C38">
         <v>619</v>
@@ -2463,7 +2457,7 @@
         <v>15</v>
       </c>
       <c r="H38" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
@@ -2471,7 +2465,7 @@
         <v>38</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>94</v>
       </c>
       <c r="C39">
         <v>19</v>
@@ -2489,7 +2483,7 @@
         <v>15</v>
       </c>
       <c r="H39" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
@@ -2497,7 +2491,7 @@
         <v>39</v>
       </c>
       <c r="B40" t="s">
-        <v>104</v>
+        <v>96</v>
       </c>
       <c r="C40">
         <v>25</v>
@@ -2515,7 +2509,7 @@
         <v>15</v>
       </c>
       <c r="H40" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
@@ -2523,7 +2517,7 @@
         <v>40</v>
       </c>
       <c r="B41" t="s">
-        <v>105</v>
+        <v>97</v>
       </c>
       <c r="C41">
         <v>281</v>
@@ -2541,7 +2535,7 @@
         <v>15</v>
       </c>
       <c r="H41" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
@@ -2549,7 +2543,7 @@
         <v>41</v>
       </c>
       <c r="B42" t="s">
-        <v>106</v>
+        <v>98</v>
       </c>
       <c r="C42">
         <v>20</v>
@@ -2567,7 +2561,7 @@
         <v>15</v>
       </c>
       <c r="H42" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
@@ -2575,7 +2569,7 @@
         <v>42</v>
       </c>
       <c r="B43" t="s">
-        <v>107</v>
+        <v>99</v>
       </c>
       <c r="C43">
         <v>115</v>
@@ -2593,7 +2587,7 @@
         <v>15</v>
       </c>
       <c r="H43" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
@@ -2601,7 +2595,7 @@
         <v>43</v>
       </c>
       <c r="B44" t="s">
-        <v>108</v>
+        <v>100</v>
       </c>
       <c r="C44">
         <v>696</v>
@@ -2619,7 +2613,7 @@
         <v>15</v>
       </c>
       <c r="H44" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
@@ -2627,7 +2621,7 @@
         <v>44</v>
       </c>
       <c r="B45" t="s">
-        <v>111</v>
+        <v>103</v>
       </c>
       <c r="C45">
         <v>241</v>
@@ -2645,7 +2639,7 @@
         <v>15</v>
       </c>
       <c r="H45" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
@@ -2653,7 +2647,7 @@
         <v>45</v>
       </c>
       <c r="B46" t="s">
-        <v>113</v>
+        <v>105</v>
       </c>
       <c r="C46">
         <v>363</v>
@@ -2671,7 +2665,7 @@
         <v>15</v>
       </c>
       <c r="H46" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
@@ -2679,7 +2673,7 @@
         <v>46</v>
       </c>
       <c r="B47" t="s">
-        <v>115</v>
+        <v>107</v>
       </c>
       <c r="C47">
         <v>449</v>
@@ -2697,7 +2691,7 @@
         <v>15</v>
       </c>
       <c r="H47" t="s">
-        <v>116</v>
+        <v>108</v>
       </c>
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
@@ -2705,7 +2699,7 @@
         <v>47</v>
       </c>
       <c r="B48" t="s">
-        <v>117</v>
+        <v>109</v>
       </c>
       <c r="C48">
         <v>378</v>
@@ -2723,7 +2717,7 @@
         <v>15</v>
       </c>
       <c r="H48" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
@@ -2731,7 +2725,7 @@
         <v>48</v>
       </c>
       <c r="B49" t="s">
-        <v>119</v>
+        <v>111</v>
       </c>
       <c r="C49">
         <v>193</v>
@@ -2757,7 +2751,7 @@
         <v>49</v>
       </c>
       <c r="B50" t="s">
-        <v>120</v>
+        <v>112</v>
       </c>
       <c r="C50">
         <v>254</v>
@@ -2775,7 +2769,7 @@
         <v>15</v>
       </c>
       <c r="H50" t="s">
-        <v>118</v>
+        <v>110</v>
       </c>
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
@@ -2783,7 +2777,7 @@
         <v>50</v>
       </c>
       <c r="B51" t="s">
-        <v>121</v>
+        <v>113</v>
       </c>
       <c r="C51">
         <v>234</v>
@@ -2809,7 +2803,7 @@
         <v>51</v>
       </c>
       <c r="B52" t="s">
-        <v>333</v>
+        <v>318</v>
       </c>
       <c r="C52">
         <v>76</v>
@@ -2827,7 +2821,7 @@
         <v>15</v>
       </c>
       <c r="H52" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
@@ -2835,7 +2829,7 @@
         <v>52</v>
       </c>
       <c r="B53" t="s">
-        <v>334</v>
+        <v>319</v>
       </c>
       <c r="C53">
         <v>192</v>
@@ -2861,7 +2855,7 @@
         <v>53</v>
       </c>
       <c r="B54" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="C54">
         <v>16</v>
@@ -2879,7 +2873,7 @@
         <v>15</v>
       </c>
       <c r="H54" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
@@ -2887,7 +2881,7 @@
         <v>54</v>
       </c>
       <c r="B55" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C55">
         <v>408</v>
@@ -2905,7 +2899,7 @@
         <v>15</v>
       </c>
       <c r="H55" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
@@ -2913,7 +2907,7 @@
         <v>55</v>
       </c>
       <c r="B56" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="C56">
         <v>44</v>
@@ -2931,7 +2925,7 @@
         <v>21</v>
       </c>
       <c r="H56" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
       <c r="I56">
         <v>1</v>
@@ -2942,7 +2936,7 @@
         <v>56</v>
       </c>
       <c r="B57" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C57">
         <v>87</v>
@@ -2960,7 +2954,7 @@
         <v>15</v>
       </c>
       <c r="H57" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
@@ -2968,7 +2962,7 @@
         <v>57</v>
       </c>
       <c r="B58" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="C58">
         <v>89</v>
@@ -2986,7 +2980,7 @@
         <v>15</v>
       </c>
       <c r="H58" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
@@ -2994,7 +2988,7 @@
         <v>58</v>
       </c>
       <c r="B59" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C59">
         <v>69</v>
@@ -3012,7 +3006,7 @@
         <v>15</v>
       </c>
       <c r="H59" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
@@ -3020,7 +3014,7 @@
         <v>59</v>
       </c>
       <c r="B60" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="C60">
         <v>70</v>
@@ -3038,7 +3032,7 @@
         <v>15</v>
       </c>
       <c r="H60" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
@@ -3046,7 +3040,7 @@
         <v>60</v>
       </c>
       <c r="B61" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="C61">
         <v>39</v>
@@ -3064,7 +3058,7 @@
         <v>15</v>
       </c>
       <c r="H61" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
@@ -3072,7 +3066,7 @@
         <v>61</v>
       </c>
       <c r="B62" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C62">
         <v>507</v>
@@ -3090,7 +3084,7 @@
         <v>15</v>
       </c>
       <c r="H62" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
@@ -3098,7 +3092,7 @@
         <v>62</v>
       </c>
       <c r="B63" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C63">
         <v>631</v>
@@ -3116,7 +3110,7 @@
         <v>15</v>
       </c>
       <c r="H63" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
@@ -3124,7 +3118,7 @@
         <v>63</v>
       </c>
       <c r="B64" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C64">
         <v>636</v>
@@ -3142,7 +3136,7 @@
         <v>15</v>
       </c>
       <c r="H64" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
@@ -3150,7 +3144,7 @@
         <v>64</v>
       </c>
       <c r="B65" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C65">
         <v>222</v>
@@ -3168,7 +3162,7 @@
         <v>15</v>
       </c>
       <c r="H65" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
@@ -3176,7 +3170,7 @@
         <v>65</v>
       </c>
       <c r="B66" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C66">
         <v>71</v>
@@ -3194,7 +3188,7 @@
         <v>15</v>
       </c>
       <c r="H66" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
@@ -3202,7 +3196,7 @@
         <v>66</v>
       </c>
       <c r="B67" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="C67">
         <v>146</v>
@@ -3220,7 +3214,7 @@
         <v>15</v>
       </c>
       <c r="H67" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
@@ -3228,7 +3222,7 @@
         <v>67</v>
       </c>
       <c r="B68" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="C68">
         <v>300</v>
@@ -3246,7 +3240,7 @@
         <v>15</v>
       </c>
       <c r="H68" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
@@ -3254,7 +3248,7 @@
         <v>68</v>
       </c>
       <c r="B69" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C69">
         <v>230</v>
@@ -3272,7 +3266,7 @@
         <v>15</v>
       </c>
       <c r="H69" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
@@ -3280,7 +3274,7 @@
         <v>69</v>
       </c>
       <c r="B70" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C70">
         <v>146</v>
@@ -3298,7 +3292,7 @@
         <v>15</v>
       </c>
       <c r="H70" t="s">
-        <v>150</v>
+        <v>336</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3306,7 +3300,7 @@
         <v>70</v>
       </c>
       <c r="B71" t="s">
-        <v>151</v>
+        <v>141</v>
       </c>
       <c r="C71">
         <v>141</v>
@@ -3324,7 +3318,7 @@
         <v>15</v>
       </c>
       <c r="H71" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
@@ -3332,7 +3326,7 @@
         <v>71</v>
       </c>
       <c r="B72" t="s">
-        <v>152</v>
+        <v>142</v>
       </c>
       <c r="C72">
         <v>127</v>
@@ -3350,7 +3344,7 @@
         <v>15</v>
       </c>
       <c r="H72" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
@@ -3358,7 +3352,7 @@
         <v>72</v>
       </c>
       <c r="B73" t="s">
-        <v>153</v>
+        <v>143</v>
       </c>
       <c r="C73">
         <v>351</v>
@@ -3376,7 +3370,7 @@
         <v>15</v>
       </c>
       <c r="H73" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
@@ -3384,7 +3378,7 @@
         <v>73</v>
       </c>
       <c r="B74" t="s">
-        <v>154</v>
+        <v>144</v>
       </c>
       <c r="C74">
         <v>31</v>
@@ -3402,7 +3396,7 @@
         <v>21</v>
       </c>
       <c r="H74" t="s">
-        <v>155</v>
+        <v>145</v>
       </c>
       <c r="I74">
         <v>1</v>
@@ -3413,7 +3407,7 @@
         <v>74</v>
       </c>
       <c r="B75" t="s">
-        <v>156</v>
+        <v>146</v>
       </c>
       <c r="C75">
         <v>52</v>
@@ -3431,7 +3425,7 @@
         <v>21</v>
       </c>
       <c r="H75" t="s">
-        <v>39</v>
+        <v>328</v>
       </c>
       <c r="I75">
         <v>1</v>
@@ -3442,7 +3436,7 @@
         <v>75</v>
       </c>
       <c r="B76" t="s">
-        <v>157</v>
+        <v>147</v>
       </c>
       <c r="C76">
         <v>224</v>
@@ -3460,7 +3454,7 @@
         <v>15</v>
       </c>
       <c r="H76" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
@@ -3468,7 +3462,7 @@
         <v>76</v>
       </c>
       <c r="B77" t="s">
-        <v>158</v>
+        <v>148</v>
       </c>
       <c r="C77">
         <v>46</v>
@@ -3486,7 +3480,7 @@
         <v>15</v>
       </c>
       <c r="H77" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
@@ -3494,7 +3488,7 @@
         <v>77</v>
       </c>
       <c r="B78" t="s">
-        <v>160</v>
+        <v>150</v>
       </c>
       <c r="C78">
         <v>56</v>
@@ -3512,7 +3506,7 @@
         <v>15</v>
       </c>
       <c r="H78" t="s">
-        <v>159</v>
+        <v>149</v>
       </c>
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
@@ -3520,7 +3514,7 @@
         <v>78</v>
       </c>
       <c r="B79" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C79">
         <v>134</v>
@@ -3538,7 +3532,7 @@
         <v>15</v>
       </c>
       <c r="H79" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
@@ -3546,7 +3540,7 @@
         <v>79</v>
       </c>
       <c r="B80" t="s">
-        <v>163</v>
+        <v>153</v>
       </c>
       <c r="C80">
         <v>143</v>
@@ -3564,7 +3558,7 @@
         <v>15</v>
       </c>
       <c r="H80" t="s">
-        <v>164</v>
+        <v>337</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -3572,7 +3566,7 @@
         <v>80</v>
       </c>
       <c r="B81" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="C81">
         <v>133</v>
@@ -3590,7 +3584,7 @@
         <v>15</v>
       </c>
       <c r="H81" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
@@ -3598,7 +3592,7 @@
         <v>81</v>
       </c>
       <c r="B82" t="s">
-        <v>167</v>
+        <v>156</v>
       </c>
       <c r="C82">
         <v>459</v>
@@ -3616,7 +3610,7 @@
         <v>15</v>
       </c>
       <c r="H82" t="s">
-        <v>168</v>
+        <v>157</v>
       </c>
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
@@ -3624,7 +3618,7 @@
         <v>82</v>
       </c>
       <c r="B83" t="s">
-        <v>169</v>
+        <v>158</v>
       </c>
       <c r="C83">
         <v>341</v>
@@ -3642,7 +3636,7 @@
         <v>15</v>
       </c>
       <c r="H83" t="s">
-        <v>170</v>
+        <v>159</v>
       </c>
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
@@ -3650,7 +3644,7 @@
         <v>83</v>
       </c>
       <c r="B84" t="s">
-        <v>171</v>
+        <v>160</v>
       </c>
       <c r="C84">
         <v>14</v>
@@ -3668,7 +3662,7 @@
         <v>15</v>
       </c>
       <c r="H84" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
@@ -3676,7 +3670,7 @@
         <v>84</v>
       </c>
       <c r="B85" t="s">
-        <v>173</v>
+        <v>162</v>
       </c>
       <c r="C85">
         <v>381</v>
@@ -3694,7 +3688,7 @@
         <v>15</v>
       </c>
       <c r="H85" t="s">
-        <v>166</v>
+        <v>155</v>
       </c>
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
@@ -3702,7 +3696,7 @@
         <v>85</v>
       </c>
       <c r="B86" t="s">
-        <v>175</v>
+        <v>164</v>
       </c>
       <c r="C86">
         <v>258</v>
@@ -3720,7 +3714,7 @@
         <v>15</v>
       </c>
       <c r="H86" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
@@ -3728,7 +3722,7 @@
         <v>86</v>
       </c>
       <c r="B87" t="s">
-        <v>176</v>
+        <v>165</v>
       </c>
       <c r="C87">
         <v>661</v>
@@ -3746,7 +3740,7 @@
         <v>15</v>
       </c>
       <c r="H87" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
@@ -3754,7 +3748,7 @@
         <v>87</v>
       </c>
       <c r="B88" t="s">
-        <v>177</v>
+        <v>166</v>
       </c>
       <c r="C88">
         <v>551</v>
@@ -3772,7 +3766,7 @@
         <v>15</v>
       </c>
       <c r="H88" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="I88">
         <v>1.3</v>
@@ -3783,7 +3777,7 @@
         <v>88</v>
       </c>
       <c r="B89" t="s">
-        <v>178</v>
+        <v>167</v>
       </c>
       <c r="C89">
         <v>52</v>
@@ -3801,7 +3795,7 @@
         <v>15</v>
       </c>
       <c r="H89" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
@@ -3809,7 +3803,7 @@
         <v>89</v>
       </c>
       <c r="B90" t="s">
-        <v>179</v>
+        <v>168</v>
       </c>
       <c r="C90">
         <v>44</v>
@@ -3827,7 +3821,7 @@
         <v>15</v>
       </c>
       <c r="H90" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
@@ -3835,7 +3829,7 @@
         <v>90</v>
       </c>
       <c r="B91" t="s">
-        <v>180</v>
+        <v>169</v>
       </c>
       <c r="C91">
         <v>104</v>
@@ -3853,7 +3847,7 @@
         <v>15</v>
       </c>
       <c r="H91" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
@@ -3861,7 +3855,7 @@
         <v>91</v>
       </c>
       <c r="B92" t="s">
-        <v>181</v>
+        <v>170</v>
       </c>
       <c r="C92">
         <v>212</v>
@@ -3879,7 +3873,7 @@
         <v>15</v>
       </c>
       <c r="H92" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
@@ -3887,7 +3881,7 @@
         <v>92</v>
       </c>
       <c r="B93" t="s">
-        <v>182</v>
+        <v>171</v>
       </c>
       <c r="C93">
         <v>306</v>
@@ -3905,7 +3899,7 @@
         <v>15</v>
       </c>
       <c r="H93" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="I93">
         <v>1.4</v>
@@ -3916,7 +3910,7 @@
         <v>93</v>
       </c>
       <c r="B94" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="C94">
         <v>216</v>
@@ -3942,7 +3936,7 @@
         <v>94</v>
       </c>
       <c r="B95" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="C95">
         <v>156</v>
@@ -3960,7 +3954,7 @@
         <v>15</v>
       </c>
       <c r="H95" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
@@ -3968,7 +3962,7 @@
         <v>95</v>
       </c>
       <c r="B96" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="C96">
         <v>140</v>
@@ -3986,7 +3980,7 @@
         <v>15</v>
       </c>
       <c r="H96" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
@@ -3994,7 +3988,7 @@
         <v>96</v>
       </c>
       <c r="B97" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="C97">
         <v>204</v>
@@ -4012,7 +4006,7 @@
         <v>15</v>
       </c>
       <c r="H97" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
@@ -4020,7 +4014,7 @@
         <v>97</v>
       </c>
       <c r="B98" t="s">
-        <v>327</v>
+        <v>312</v>
       </c>
       <c r="C98">
         <v>117</v>
@@ -4038,7 +4032,7 @@
         <v>15</v>
       </c>
       <c r="H98" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
@@ -4046,7 +4040,7 @@
         <v>98</v>
       </c>
       <c r="B99" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="C99">
         <v>64</v>
@@ -4064,7 +4058,7 @@
         <v>21</v>
       </c>
       <c r="H99" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="I99">
         <v>1.1000000000000001</v>
@@ -4075,7 +4069,7 @@
         <v>99</v>
       </c>
       <c r="B100" t="s">
-        <v>191</v>
+        <v>180</v>
       </c>
       <c r="C100">
         <v>101</v>
@@ -4093,7 +4087,7 @@
         <v>15</v>
       </c>
       <c r="H100" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="I100">
         <v>1.1000000000000001</v>
@@ -4104,7 +4098,7 @@
         <v>100</v>
       </c>
       <c r="B101" t="s">
-        <v>192</v>
+        <v>181</v>
       </c>
       <c r="C101">
         <v>66</v>
@@ -4122,7 +4116,7 @@
         <v>15</v>
       </c>
       <c r="H101" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="I101">
         <v>1.1000000000000001</v>
@@ -4133,7 +4127,7 @@
         <v>101</v>
       </c>
       <c r="B102" t="s">
-        <v>193</v>
+        <v>182</v>
       </c>
       <c r="C102">
         <v>98</v>
@@ -4151,7 +4145,7 @@
         <v>15</v>
       </c>
       <c r="H102" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="I102">
         <v>1.1000000000000001</v>
@@ -4162,7 +4156,7 @@
         <v>102</v>
       </c>
       <c r="B103" t="s">
-        <v>194</v>
+        <v>183</v>
       </c>
       <c r="C103">
         <v>71</v>
@@ -4180,7 +4174,7 @@
         <v>15</v>
       </c>
       <c r="H103" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
@@ -4188,7 +4182,7 @@
         <v>103</v>
       </c>
       <c r="B104" t="s">
-        <v>195</v>
+        <v>184</v>
       </c>
       <c r="C104">
         <v>216</v>
@@ -4206,7 +4200,7 @@
         <v>15</v>
       </c>
       <c r="H104" t="s">
-        <v>35</v>
+        <v>331</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -4214,7 +4208,7 @@
         <v>104</v>
       </c>
       <c r="B105" t="s">
-        <v>196</v>
+        <v>185</v>
       </c>
       <c r="C105">
         <v>128</v>
@@ -4232,7 +4226,7 @@
         <v>15</v>
       </c>
       <c r="H105" t="s">
-        <v>110</v>
+        <v>102</v>
       </c>
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
@@ -4240,7 +4234,7 @@
         <v>105</v>
       </c>
       <c r="B106" t="s">
-        <v>335</v>
+        <v>320</v>
       </c>
       <c r="C106">
         <v>42</v>
@@ -4258,7 +4252,7 @@
         <v>15</v>
       </c>
       <c r="H106" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
@@ -4266,7 +4260,7 @@
         <v>106</v>
       </c>
       <c r="B107" t="s">
-        <v>197</v>
+        <v>186</v>
       </c>
       <c r="C107">
         <v>303</v>
@@ -4284,7 +4278,7 @@
         <v>15</v>
       </c>
       <c r="H107" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -4292,7 +4286,7 @@
         <v>107</v>
       </c>
       <c r="B108" t="s">
-        <v>198</v>
+        <v>187</v>
       </c>
       <c r="C108">
         <v>117</v>
@@ -4310,7 +4304,7 @@
         <v>15</v>
       </c>
       <c r="H108" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I108">
         <v>1.1399999999999999</v>
@@ -4321,7 +4315,7 @@
         <v>108</v>
       </c>
       <c r="B109" t="s">
-        <v>199</v>
+        <v>188</v>
       </c>
       <c r="C109">
         <v>62</v>
@@ -4339,7 +4333,7 @@
         <v>15</v>
       </c>
       <c r="H109" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4347,7 +4341,7 @@
         <v>109</v>
       </c>
       <c r="B110" t="s">
-        <v>200</v>
+        <v>189</v>
       </c>
       <c r="C110">
         <v>332</v>
@@ -4365,7 +4359,7 @@
         <v>15</v>
       </c>
       <c r="H110" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -4373,7 +4367,7 @@
         <v>110</v>
       </c>
       <c r="B111" t="s">
-        <v>202</v>
+        <v>191</v>
       </c>
       <c r="C111">
         <v>137</v>
@@ -4391,7 +4385,7 @@
         <v>15</v>
       </c>
       <c r="H111" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4399,7 +4393,7 @@
         <v>111</v>
       </c>
       <c r="B112" t="s">
-        <v>203</v>
+        <v>192</v>
       </c>
       <c r="C112">
         <v>442</v>
@@ -4417,7 +4411,7 @@
         <v>15</v>
       </c>
       <c r="H112" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -4425,7 +4419,7 @@
         <v>112</v>
       </c>
       <c r="B113" t="s">
-        <v>204</v>
+        <v>193</v>
       </c>
       <c r="C113">
         <v>223</v>
@@ -4443,7 +4437,7 @@
         <v>15</v>
       </c>
       <c r="H113" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -4451,7 +4445,7 @@
         <v>113</v>
       </c>
       <c r="B114" t="s">
-        <v>205</v>
+        <v>194</v>
       </c>
       <c r="C114">
         <v>214</v>
@@ -4469,7 +4463,7 @@
         <v>15</v>
       </c>
       <c r="H114" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -4477,7 +4471,7 @@
         <v>114</v>
       </c>
       <c r="B115" t="s">
-        <v>206</v>
+        <v>195</v>
       </c>
       <c r="C115">
         <v>246</v>
@@ -4495,7 +4489,7 @@
         <v>15</v>
       </c>
       <c r="H115" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="I115">
         <v>1.4</v>
@@ -4506,7 +4500,7 @@
         <v>115</v>
       </c>
       <c r="B116" t="s">
-        <v>207</v>
+        <v>196</v>
       </c>
       <c r="C116">
         <v>14</v>
@@ -4524,7 +4518,7 @@
         <v>15</v>
       </c>
       <c r="H116" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -4532,7 +4526,7 @@
         <v>116</v>
       </c>
       <c r="B117" t="s">
-        <v>208</v>
+        <v>197</v>
       </c>
       <c r="C117">
         <v>28</v>
@@ -4550,7 +4544,7 @@
         <v>15</v>
       </c>
       <c r="H117" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
@@ -4558,7 +4552,7 @@
         <v>117</v>
       </c>
       <c r="B118" t="s">
-        <v>209</v>
+        <v>198</v>
       </c>
       <c r="C118">
         <v>615</v>
@@ -4576,7 +4570,7 @@
         <v>15</v>
       </c>
       <c r="H118" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -4584,7 +4578,7 @@
         <v>118</v>
       </c>
       <c r="B119" t="s">
-        <v>210</v>
+        <v>199</v>
       </c>
       <c r="C119">
         <v>167</v>
@@ -4602,7 +4596,7 @@
         <v>15</v>
       </c>
       <c r="H119" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -4610,7 +4604,7 @@
         <v>119</v>
       </c>
       <c r="B120" t="s">
-        <v>211</v>
+        <v>200</v>
       </c>
       <c r="C120">
         <v>47</v>
@@ -4628,7 +4622,7 @@
         <v>21</v>
       </c>
       <c r="H120" t="s">
-        <v>100</v>
+        <v>332</v>
       </c>
       <c r="I120">
         <v>0.88</v>
@@ -4639,7 +4633,7 @@
         <v>120</v>
       </c>
       <c r="B121" t="s">
-        <v>212</v>
+        <v>201</v>
       </c>
       <c r="C121">
         <v>444</v>
@@ -4657,7 +4651,7 @@
         <v>15</v>
       </c>
       <c r="H121" t="s">
-        <v>67</v>
+        <v>61</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -4665,7 +4659,7 @@
         <v>121</v>
       </c>
       <c r="B122" t="s">
-        <v>214</v>
+        <v>203</v>
       </c>
       <c r="C122">
         <v>134</v>
@@ -4683,7 +4677,7 @@
         <v>15</v>
       </c>
       <c r="H122" t="s">
-        <v>77</v>
+        <v>71</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -4691,7 +4685,7 @@
         <v>122</v>
       </c>
       <c r="B123" t="s">
-        <v>215</v>
+        <v>204</v>
       </c>
       <c r="C123">
         <v>244</v>
@@ -4709,7 +4703,7 @@
         <v>15</v>
       </c>
       <c r="H123" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -4717,7 +4711,7 @@
         <v>123</v>
       </c>
       <c r="B124" t="s">
-        <v>216</v>
+        <v>205</v>
       </c>
       <c r="C124">
         <v>93</v>
@@ -4735,7 +4729,7 @@
         <v>15</v>
       </c>
       <c r="H124" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -4743,7 +4737,7 @@
         <v>124</v>
       </c>
       <c r="B125" t="s">
-        <v>217</v>
+        <v>206</v>
       </c>
       <c r="C125">
         <v>47</v>
@@ -4761,7 +4755,7 @@
         <v>15</v>
       </c>
       <c r="H125" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -4769,7 +4763,7 @@
         <v>125</v>
       </c>
       <c r="B126" t="s">
-        <v>218</v>
+        <v>207</v>
       </c>
       <c r="C126">
         <v>624</v>
@@ -4787,7 +4781,7 @@
         <v>15</v>
       </c>
       <c r="H126" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -4795,7 +4789,7 @@
         <v>126</v>
       </c>
       <c r="B127" t="s">
-        <v>219</v>
+        <v>208</v>
       </c>
       <c r="C127">
         <v>649</v>
@@ -4813,7 +4807,7 @@
         <v>15</v>
       </c>
       <c r="H127" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -4821,7 +4815,7 @@
         <v>127</v>
       </c>
       <c r="B128" t="s">
-        <v>220</v>
+        <v>209</v>
       </c>
       <c r="C128">
         <v>68</v>
@@ -4839,7 +4833,7 @@
         <v>15</v>
       </c>
       <c r="H128" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -4847,7 +4841,7 @@
         <v>128</v>
       </c>
       <c r="B129" t="s">
-        <v>221</v>
+        <v>210</v>
       </c>
       <c r="C129">
         <v>23</v>
@@ -4865,7 +4859,7 @@
         <v>15</v>
       </c>
       <c r="H129" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -4873,7 +4867,7 @@
         <v>129</v>
       </c>
       <c r="B130" t="s">
-        <v>222</v>
+        <v>211</v>
       </c>
       <c r="C130">
         <v>357</v>
@@ -4891,7 +4885,7 @@
         <v>15</v>
       </c>
       <c r="H130" t="s">
-        <v>223</v>
+        <v>333</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -4899,7 +4893,7 @@
         <v>130</v>
       </c>
       <c r="B131" t="s">
-        <v>224</v>
+        <v>212</v>
       </c>
       <c r="C131">
         <v>356</v>
@@ -4917,7 +4911,7 @@
         <v>15</v>
       </c>
       <c r="H131" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -4925,7 +4919,7 @@
         <v>131</v>
       </c>
       <c r="B132" t="s">
-        <v>225</v>
+        <v>213</v>
       </c>
       <c r="C132">
         <v>474</v>
@@ -4943,7 +4937,7 @@
         <v>15</v>
       </c>
       <c r="H132" t="s">
-        <v>226</v>
+        <v>214</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -4951,7 +4945,7 @@
         <v>132</v>
       </c>
       <c r="B133" t="s">
-        <v>227</v>
+        <v>215</v>
       </c>
       <c r="C133">
         <v>742</v>
@@ -4969,7 +4963,7 @@
         <v>15</v>
       </c>
       <c r="H133" t="s">
-        <v>228</v>
+        <v>216</v>
       </c>
       <c r="I133">
         <v>0.9</v>
@@ -4980,7 +4974,7 @@
         <v>133</v>
       </c>
       <c r="B134" t="s">
-        <v>229</v>
+        <v>217</v>
       </c>
       <c r="C134">
         <v>343</v>
@@ -4998,7 +4992,7 @@
         <v>15</v>
       </c>
       <c r="H134" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -5006,7 +5000,7 @@
         <v>134</v>
       </c>
       <c r="B135" t="s">
-        <v>230</v>
+        <v>218</v>
       </c>
       <c r="C135">
         <v>59</v>
@@ -5024,7 +5018,7 @@
         <v>21</v>
       </c>
       <c r="H135" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="I135">
         <v>1</v>
@@ -5035,7 +5029,7 @@
         <v>135</v>
       </c>
       <c r="B136" t="s">
-        <v>231</v>
+        <v>219</v>
       </c>
       <c r="C136">
         <v>537</v>
@@ -5053,7 +5047,7 @@
         <v>15</v>
       </c>
       <c r="H136" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -5061,7 +5055,7 @@
         <v>136</v>
       </c>
       <c r="B137" t="s">
-        <v>232</v>
+        <v>220</v>
       </c>
       <c r="C137">
         <v>570</v>
@@ -5079,7 +5073,7 @@
         <v>15</v>
       </c>
       <c r="H137" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
@@ -5087,7 +5081,7 @@
         <v>137</v>
       </c>
       <c r="B138" t="s">
-        <v>329</v>
+        <v>314</v>
       </c>
       <c r="C138">
         <v>0</v>
@@ -5105,7 +5099,7 @@
         <v>21</v>
       </c>
       <c r="H138" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="I138">
         <v>1</v>
@@ -5116,7 +5110,7 @@
         <v>138</v>
       </c>
       <c r="B139" t="s">
-        <v>330</v>
+        <v>315</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -5134,7 +5128,7 @@
         <v>21</v>
       </c>
       <c r="H139" t="s">
-        <v>328</v>
+        <v>313</v>
       </c>
       <c r="I139">
         <v>1</v>
@@ -5145,7 +5139,7 @@
         <v>139</v>
       </c>
       <c r="B140" t="s">
-        <v>233</v>
+        <v>221</v>
       </c>
       <c r="C140">
         <v>314</v>
@@ -5163,7 +5157,7 @@
         <v>15</v>
       </c>
       <c r="H140" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
@@ -5171,7 +5165,7 @@
         <v>140</v>
       </c>
       <c r="B141" t="s">
-        <v>234</v>
+        <v>222</v>
       </c>
       <c r="C141">
         <v>256</v>
@@ -5189,7 +5183,7 @@
         <v>15</v>
       </c>
       <c r="H141" t="s">
-        <v>235</v>
+        <v>334</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -5197,7 +5191,7 @@
         <v>141</v>
       </c>
       <c r="B142" t="s">
-        <v>236</v>
+        <v>223</v>
       </c>
       <c r="C142">
         <v>365</v>
@@ -5215,7 +5209,7 @@
         <v>15</v>
       </c>
       <c r="H142" t="s">
-        <v>114</v>
+        <v>106</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
@@ -5223,7 +5217,7 @@
         <v>142</v>
       </c>
       <c r="B143" t="s">
-        <v>237</v>
+        <v>224</v>
       </c>
       <c r="C143">
         <v>125</v>
@@ -5241,7 +5235,7 @@
         <v>15</v>
       </c>
       <c r="H143" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -5249,7 +5243,7 @@
         <v>143</v>
       </c>
       <c r="B144" t="s">
-        <v>238</v>
+        <v>225</v>
       </c>
       <c r="C144">
         <v>55</v>
@@ -5267,7 +5261,7 @@
         <v>15</v>
       </c>
       <c r="H144" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -5275,7 +5269,7 @@
         <v>144</v>
       </c>
       <c r="B145" t="s">
-        <v>336</v>
+        <v>321</v>
       </c>
       <c r="C145">
         <v>127</v>
@@ -5293,7 +5287,7 @@
         <v>15</v>
       </c>
       <c r="H145" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -5301,7 +5295,7 @@
         <v>145</v>
       </c>
       <c r="B146" t="s">
-        <v>239</v>
+        <v>226</v>
       </c>
       <c r="C146">
         <v>176</v>
@@ -5319,7 +5313,7 @@
         <v>15</v>
       </c>
       <c r="H146" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -5327,7 +5321,7 @@
         <v>146</v>
       </c>
       <c r="B147" t="s">
-        <v>240</v>
+        <v>227</v>
       </c>
       <c r="C147">
         <v>810</v>
@@ -5345,7 +5339,7 @@
         <v>21</v>
       </c>
       <c r="H147" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I147">
         <v>0.9</v>
@@ -5356,7 +5350,7 @@
         <v>147</v>
       </c>
       <c r="B148" t="s">
-        <v>241</v>
+        <v>228</v>
       </c>
       <c r="C148">
         <v>45</v>
@@ -5374,7 +5368,7 @@
         <v>15</v>
       </c>
       <c r="H148" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -5382,7 +5376,7 @@
         <v>148</v>
       </c>
       <c r="B149" t="s">
-        <v>242</v>
+        <v>229</v>
       </c>
       <c r="C149">
         <v>44</v>
@@ -5400,7 +5394,7 @@
         <v>21</v>
       </c>
       <c r="H149" t="s">
-        <v>39</v>
+        <v>328</v>
       </c>
       <c r="I149">
         <v>1.04</v>
@@ -5411,7 +5405,7 @@
         <v>149</v>
       </c>
       <c r="B150" t="s">
-        <v>243</v>
+        <v>230</v>
       </c>
       <c r="C150">
         <v>358</v>
@@ -5429,7 +5423,7 @@
         <v>15</v>
       </c>
       <c r="H150" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -5437,7 +5431,7 @@
         <v>150</v>
       </c>
       <c r="B151" t="s">
-        <v>244</v>
+        <v>231</v>
       </c>
       <c r="C151">
         <v>698</v>
@@ -5455,7 +5449,7 @@
         <v>15</v>
       </c>
       <c r="H151" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -5463,7 +5457,7 @@
         <v>151</v>
       </c>
       <c r="B152" t="s">
-        <v>245</v>
+        <v>232</v>
       </c>
       <c r="C152">
         <v>401</v>
@@ -5471,8 +5465,8 @@
       <c r="D152">
         <v>31</v>
       </c>
-      <c r="E152" t="s">
-        <v>28</v>
+      <c r="E152">
+        <v>0.3</v>
       </c>
       <c r="F152">
         <v>30.5</v>
@@ -5481,7 +5475,7 @@
         <v>15</v>
       </c>
       <c r="H152" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -5489,7 +5483,7 @@
         <v>152</v>
       </c>
       <c r="B153" t="s">
-        <v>246</v>
+        <v>233</v>
       </c>
       <c r="C153">
         <v>430</v>
@@ -5507,7 +5501,7 @@
         <v>15</v>
       </c>
       <c r="H153" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -5515,7 +5509,7 @@
         <v>153</v>
       </c>
       <c r="B154" t="s">
-        <v>247</v>
+        <v>234</v>
       </c>
       <c r="C154">
         <v>398</v>
@@ -5533,7 +5527,7 @@
         <v>15</v>
       </c>
       <c r="H154" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
@@ -5541,7 +5535,7 @@
         <v>154</v>
       </c>
       <c r="B155" t="s">
-        <v>248</v>
+        <v>235</v>
       </c>
       <c r="C155">
         <v>58</v>
@@ -5559,7 +5553,7 @@
         <v>15</v>
       </c>
       <c r="H155" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -5567,7 +5561,7 @@
         <v>155</v>
       </c>
       <c r="B156" t="s">
-        <v>249</v>
+        <v>236</v>
       </c>
       <c r="C156">
         <v>43</v>
@@ -5585,7 +5579,7 @@
         <v>15</v>
       </c>
       <c r="H156" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -5593,7 +5587,7 @@
         <v>156</v>
       </c>
       <c r="B157" t="s">
-        <v>250</v>
+        <v>237</v>
       </c>
       <c r="C157">
         <v>48</v>
@@ -5611,7 +5605,7 @@
         <v>15</v>
       </c>
       <c r="H157" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
@@ -5619,7 +5613,7 @@
         <v>157</v>
       </c>
       <c r="B158" t="s">
-        <v>251</v>
+        <v>238</v>
       </c>
       <c r="C158">
         <v>29</v>
@@ -5637,7 +5631,7 @@
         <v>15</v>
       </c>
       <c r="H158" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -5645,7 +5639,7 @@
         <v>158</v>
       </c>
       <c r="B159" t="s">
-        <v>252</v>
+        <v>239</v>
       </c>
       <c r="C159">
         <v>594</v>
@@ -5663,7 +5657,7 @@
         <v>15</v>
       </c>
       <c r="H159" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -5671,7 +5665,7 @@
         <v>159</v>
       </c>
       <c r="B160" t="s">
-        <v>253</v>
+        <v>240</v>
       </c>
       <c r="C160">
         <v>226</v>
@@ -5689,7 +5683,7 @@
         <v>15</v>
       </c>
       <c r="H160" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -5697,7 +5691,7 @@
         <v>160</v>
       </c>
       <c r="B161" t="s">
-        <v>254</v>
+        <v>241</v>
       </c>
       <c r="C161">
         <v>195</v>
@@ -5715,7 +5709,7 @@
         <v>15</v>
       </c>
       <c r="H161" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
@@ -5723,7 +5717,7 @@
         <v>161</v>
       </c>
       <c r="B162" t="s">
-        <v>255</v>
+        <v>242</v>
       </c>
       <c r="C162">
         <v>238</v>
@@ -5741,7 +5735,7 @@
         <v>15</v>
       </c>
       <c r="H162" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
@@ -5749,7 +5743,7 @@
         <v>162</v>
       </c>
       <c r="B163" t="s">
-        <v>256</v>
+        <v>243</v>
       </c>
       <c r="C163">
         <v>204</v>
@@ -5767,7 +5761,7 @@
         <v>15</v>
       </c>
       <c r="H163" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
@@ -5775,7 +5769,7 @@
         <v>163</v>
       </c>
       <c r="B164" t="s">
-        <v>257</v>
+        <v>244</v>
       </c>
       <c r="C164">
         <v>218</v>
@@ -5793,7 +5787,7 @@
         <v>15</v>
       </c>
       <c r="H164" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
@@ -5801,7 +5795,7 @@
         <v>164</v>
       </c>
       <c r="B165" t="s">
-        <v>258</v>
+        <v>245</v>
       </c>
       <c r="C165">
         <v>297</v>
@@ -5819,7 +5813,7 @@
         <v>15</v>
       </c>
       <c r="H165" t="s">
-        <v>98</v>
+        <v>91</v>
       </c>
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
@@ -5827,7 +5821,7 @@
         <v>165</v>
       </c>
       <c r="B166" t="s">
-        <v>259</v>
+        <v>246</v>
       </c>
       <c r="C166">
         <v>232</v>
@@ -5845,7 +5839,7 @@
         <v>15</v>
       </c>
       <c r="H166" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -5853,7 +5847,7 @@
         <v>166</v>
       </c>
       <c r="B167" t="s">
-        <v>260</v>
+        <v>247</v>
       </c>
       <c r="C167">
         <v>286</v>
@@ -5871,7 +5865,7 @@
         <v>15</v>
       </c>
       <c r="H167" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
@@ -5879,7 +5873,7 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>261</v>
+        <v>248</v>
       </c>
       <c r="C168">
         <v>367</v>
@@ -5897,7 +5891,7 @@
         <v>15</v>
       </c>
       <c r="H168" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -5905,7 +5899,7 @@
         <v>168</v>
       </c>
       <c r="B169" t="s">
-        <v>337</v>
+        <v>322</v>
       </c>
       <c r="C169">
         <v>107</v>
@@ -5923,7 +5917,7 @@
         <v>15</v>
       </c>
       <c r="H169" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -5931,7 +5925,7 @@
         <v>169</v>
       </c>
       <c r="B170" t="s">
-        <v>338</v>
+        <v>323</v>
       </c>
       <c r="C170">
         <v>128</v>
@@ -5949,7 +5943,7 @@
         <v>15</v>
       </c>
       <c r="H170" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
@@ -5957,7 +5951,7 @@
         <v>170</v>
       </c>
       <c r="B171" t="s">
-        <v>339</v>
+        <v>324</v>
       </c>
       <c r="C171">
         <v>163</v>
@@ -5975,7 +5969,7 @@
         <v>15</v>
       </c>
       <c r="H171" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
@@ -5983,7 +5977,7 @@
         <v>171</v>
       </c>
       <c r="B172" t="s">
-        <v>262</v>
+        <v>249</v>
       </c>
       <c r="C172">
         <v>102</v>
@@ -6001,7 +5995,7 @@
         <v>15</v>
       </c>
       <c r="H172" t="s">
-        <v>213</v>
+        <v>202</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -6009,7 +6003,7 @@
         <v>172</v>
       </c>
       <c r="B173" t="s">
-        <v>263</v>
+        <v>250</v>
       </c>
       <c r="C173">
         <v>61</v>
@@ -6027,7 +6021,7 @@
         <v>15</v>
       </c>
       <c r="H173" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -6035,7 +6029,7 @@
         <v>173</v>
       </c>
       <c r="B174" t="s">
-        <v>264</v>
+        <v>251</v>
       </c>
       <c r="C174">
         <v>17</v>
@@ -6053,7 +6047,7 @@
         <v>15</v>
       </c>
       <c r="H174" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -6061,7 +6055,7 @@
         <v>174</v>
       </c>
       <c r="B175" t="s">
-        <v>265</v>
+        <v>252</v>
       </c>
       <c r="C175">
         <v>810</v>
@@ -6079,7 +6073,7 @@
         <v>21</v>
       </c>
       <c r="H175" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I175">
         <v>0.9</v>
@@ -6090,7 +6084,7 @@
         <v>175</v>
       </c>
       <c r="B176" t="s">
-        <v>266</v>
+        <v>253</v>
       </c>
       <c r="C176">
         <v>45</v>
@@ -6108,7 +6102,7 @@
         <v>15</v>
       </c>
       <c r="H176" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
@@ -6116,7 +6110,7 @@
         <v>176</v>
       </c>
       <c r="B177" t="s">
-        <v>267</v>
+        <v>254</v>
       </c>
       <c r="C177">
         <v>406</v>
@@ -6134,7 +6128,7 @@
         <v>15</v>
       </c>
       <c r="H177" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
@@ -6142,7 +6136,7 @@
         <v>177</v>
       </c>
       <c r="B178" t="s">
-        <v>269</v>
+        <v>256</v>
       </c>
       <c r="C178">
         <v>126</v>
@@ -6160,7 +6154,7 @@
         <v>15</v>
       </c>
       <c r="H178" t="s">
-        <v>268</v>
+        <v>255</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
@@ -6168,7 +6162,7 @@
         <v>178</v>
       </c>
       <c r="B179" t="s">
-        <v>270</v>
+        <v>338</v>
       </c>
       <c r="C179">
         <v>162</v>
@@ -6186,7 +6180,7 @@
         <v>15</v>
       </c>
       <c r="H179" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
@@ -6194,7 +6188,7 @@
         <v>179</v>
       </c>
       <c r="B180" t="s">
-        <v>271</v>
+        <v>257</v>
       </c>
       <c r="C180">
         <v>133</v>
@@ -6212,7 +6206,7 @@
         <v>15</v>
       </c>
       <c r="H180" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
@@ -6220,7 +6214,7 @@
         <v>180</v>
       </c>
       <c r="B181" t="s">
-        <v>272</v>
+        <v>339</v>
       </c>
       <c r="C181">
         <v>128</v>
@@ -6238,7 +6232,7 @@
         <v>15</v>
       </c>
       <c r="H181" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
@@ -6246,7 +6240,7 @@
         <v>181</v>
       </c>
       <c r="B182" t="s">
-        <v>273</v>
+        <v>258</v>
       </c>
       <c r="C182">
         <v>105</v>
@@ -6264,7 +6258,7 @@
         <v>15</v>
       </c>
       <c r="H182" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
@@ -6272,7 +6266,7 @@
         <v>182</v>
       </c>
       <c r="B183" t="s">
-        <v>340</v>
+        <v>325</v>
       </c>
       <c r="C183">
         <v>211</v>
@@ -6290,7 +6284,7 @@
         <v>15</v>
       </c>
       <c r="H183" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
@@ -6298,7 +6292,7 @@
         <v>183</v>
       </c>
       <c r="B184" t="s">
-        <v>341</v>
+        <v>326</v>
       </c>
       <c r="C184">
         <v>154</v>
@@ -6316,7 +6310,7 @@
         <v>15</v>
       </c>
       <c r="H184" t="s">
-        <v>172</v>
+        <v>161</v>
       </c>
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
@@ -6324,7 +6318,7 @@
         <v>184</v>
       </c>
       <c r="B185" t="s">
-        <v>274</v>
+        <v>259</v>
       </c>
       <c r="C185">
         <v>321</v>
@@ -6342,7 +6336,7 @@
         <v>15</v>
       </c>
       <c r="H185" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
@@ -6350,7 +6344,7 @@
         <v>185</v>
       </c>
       <c r="B186" t="s">
-        <v>275</v>
+        <v>260</v>
       </c>
       <c r="C186">
         <v>150</v>
@@ -6368,7 +6362,7 @@
         <v>15</v>
       </c>
       <c r="H186" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
@@ -6376,7 +6370,7 @@
         <v>186</v>
       </c>
       <c r="B187" t="s">
-        <v>276</v>
+        <v>261</v>
       </c>
       <c r="C187">
         <v>28</v>
@@ -6394,7 +6388,7 @@
         <v>15</v>
       </c>
       <c r="H187" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
@@ -6402,7 +6396,7 @@
         <v>187</v>
       </c>
       <c r="B188" t="s">
-        <v>277</v>
+        <v>262</v>
       </c>
       <c r="C188">
         <v>147</v>
@@ -6428,7 +6422,7 @@
         <v>188</v>
       </c>
       <c r="B189" t="s">
-        <v>278</v>
+        <v>263</v>
       </c>
       <c r="C189">
         <v>422</v>
@@ -6436,8 +6430,8 @@
       <c r="D189">
         <v>37.1</v>
       </c>
-      <c r="E189" t="s">
-        <v>28</v>
+      <c r="E189">
+        <v>3</v>
       </c>
       <c r="F189">
         <v>22</v>
@@ -6446,7 +6440,7 @@
         <v>15</v>
       </c>
       <c r="H189" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
@@ -6454,7 +6448,7 @@
         <v>189</v>
       </c>
       <c r="B190" t="s">
-        <v>279</v>
+        <v>264</v>
       </c>
       <c r="C190">
         <v>464</v>
@@ -6472,7 +6466,7 @@
         <v>21</v>
       </c>
       <c r="H190" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="I190">
         <v>1.1000000000000001</v>
@@ -6483,7 +6477,7 @@
         <v>190</v>
       </c>
       <c r="B191" t="s">
-        <v>280</v>
+        <v>265</v>
       </c>
       <c r="C191">
         <v>309</v>
@@ -6501,7 +6495,7 @@
         <v>15</v>
       </c>
       <c r="H191" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="I191">
         <v>1.1000000000000001</v>
@@ -6512,7 +6506,7 @@
         <v>191</v>
       </c>
       <c r="B192" t="s">
-        <v>281</v>
+        <v>266</v>
       </c>
       <c r="C192">
         <v>0</v>
@@ -6530,7 +6524,7 @@
         <v>15</v>
       </c>
       <c r="H192" t="s">
-        <v>53</v>
+        <v>48</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
@@ -6538,7 +6532,7 @@
         <v>192</v>
       </c>
       <c r="B193" t="s">
-        <v>282</v>
+        <v>267</v>
       </c>
       <c r="C193">
         <v>163</v>
@@ -6556,7 +6550,7 @@
         <v>15</v>
       </c>
       <c r="H193" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
@@ -6564,7 +6558,7 @@
         <v>193</v>
       </c>
       <c r="B194" t="s">
-        <v>283</v>
+        <v>268</v>
       </c>
       <c r="C194">
         <v>131</v>
@@ -6582,7 +6576,7 @@
         <v>15</v>
       </c>
       <c r="H194" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
@@ -6590,7 +6584,7 @@
         <v>194</v>
       </c>
       <c r="B195" t="s">
-        <v>284</v>
+        <v>269</v>
       </c>
       <c r="C195">
         <v>19</v>
@@ -6608,7 +6602,7 @@
         <v>15</v>
       </c>
       <c r="H195" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
@@ -6616,7 +6610,7 @@
         <v>195</v>
       </c>
       <c r="B196" t="s">
-        <v>285</v>
+        <v>270</v>
       </c>
       <c r="C196">
         <v>336</v>
@@ -6634,7 +6628,7 @@
         <v>15</v>
       </c>
       <c r="H196" t="s">
-        <v>123</v>
+        <v>335</v>
       </c>
       <c r="I196">
         <v>1</v>
@@ -6645,7 +6639,7 @@
         <v>196</v>
       </c>
       <c r="B197" t="s">
-        <v>286</v>
+        <v>271</v>
       </c>
       <c r="C197">
         <v>30</v>
@@ -6663,7 +6657,7 @@
         <v>15</v>
       </c>
       <c r="H197" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
@@ -6671,7 +6665,7 @@
         <v>197</v>
       </c>
       <c r="B198" t="s">
-        <v>287</v>
+        <v>272</v>
       </c>
       <c r="C198">
         <v>262</v>
@@ -6689,7 +6683,7 @@
         <v>15</v>
       </c>
       <c r="H198" t="s">
-        <v>122</v>
+        <v>114</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
@@ -6697,7 +6691,7 @@
         <v>198</v>
       </c>
       <c r="B199" t="s">
-        <v>288</v>
+        <v>273</v>
       </c>
       <c r="C199">
         <v>537</v>
@@ -6715,7 +6709,7 @@
         <v>15</v>
       </c>
       <c r="H199" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
@@ -6723,7 +6717,7 @@
         <v>199</v>
       </c>
       <c r="B200" t="s">
-        <v>289</v>
+        <v>274</v>
       </c>
       <c r="C200">
         <v>567</v>
@@ -6741,7 +6735,7 @@
         <v>15</v>
       </c>
       <c r="H200" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
@@ -6749,7 +6743,7 @@
         <v>200</v>
       </c>
       <c r="B201" t="s">
-        <v>290</v>
+        <v>275</v>
       </c>
       <c r="C201">
         <v>153</v>
@@ -6767,7 +6761,7 @@
         <v>15</v>
       </c>
       <c r="H201" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
@@ -6775,7 +6769,7 @@
         <v>201</v>
       </c>
       <c r="B202" t="s">
-        <v>291</v>
+        <v>276</v>
       </c>
       <c r="C202">
         <v>121</v>
@@ -6793,7 +6787,7 @@
         <v>15</v>
       </c>
       <c r="H202" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
@@ -6801,7 +6795,7 @@
         <v>202</v>
       </c>
       <c r="B203" t="s">
-        <v>292</v>
+        <v>277</v>
       </c>
       <c r="C203">
         <v>159</v>
@@ -6819,7 +6813,7 @@
         <v>15</v>
       </c>
       <c r="H203" t="s">
-        <v>112</v>
+        <v>104</v>
       </c>
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
@@ -6827,7 +6821,7 @@
         <v>203</v>
       </c>
       <c r="B204" t="s">
-        <v>293</v>
+        <v>278</v>
       </c>
       <c r="C204">
         <v>236</v>
@@ -6845,7 +6839,7 @@
         <v>15</v>
       </c>
       <c r="H204" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
@@ -6853,7 +6847,7 @@
         <v>204</v>
       </c>
       <c r="B205" t="s">
-        <v>294</v>
+        <v>279</v>
       </c>
       <c r="C205">
         <v>283</v>
@@ -6871,7 +6865,7 @@
         <v>15</v>
       </c>
       <c r="H205" t="s">
-        <v>62</v>
+        <v>56</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
@@ -6879,7 +6873,7 @@
         <v>205</v>
       </c>
       <c r="B206" t="s">
-        <v>295</v>
+        <v>280</v>
       </c>
       <c r="C206">
         <v>80</v>
@@ -6897,7 +6891,7 @@
         <v>15</v>
       </c>
       <c r="H206" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
@@ -6905,7 +6899,7 @@
         <v>206</v>
       </c>
       <c r="B207" t="s">
-        <v>296</v>
+        <v>281</v>
       </c>
       <c r="C207">
         <v>85</v>
@@ -6923,7 +6917,7 @@
         <v>15</v>
       </c>
       <c r="H207" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
@@ -6931,7 +6925,7 @@
         <v>207</v>
       </c>
       <c r="B208" t="s">
-        <v>298</v>
+        <v>283</v>
       </c>
       <c r="C208">
         <v>124</v>
@@ -6949,7 +6943,7 @@
         <v>15</v>
       </c>
       <c r="H208" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
@@ -6957,7 +6951,7 @@
         <v>208</v>
       </c>
       <c r="B209" t="s">
-        <v>299</v>
+        <v>284</v>
       </c>
       <c r="C209">
         <v>621</v>
@@ -6975,7 +6969,7 @@
         <v>15</v>
       </c>
       <c r="H209" t="s">
-        <v>63</v>
+        <v>57</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
@@ -6983,7 +6977,7 @@
         <v>209</v>
       </c>
       <c r="B210" t="s">
-        <v>300</v>
+        <v>285</v>
       </c>
       <c r="C210">
         <v>810</v>
@@ -7001,7 +6995,7 @@
         <v>21</v>
       </c>
       <c r="H210" t="s">
-        <v>64</v>
+        <v>58</v>
       </c>
       <c r="I210">
         <v>0.9</v>
@@ -7012,7 +7006,7 @@
         <v>210</v>
       </c>
       <c r="B211" t="s">
-        <v>301</v>
+        <v>286</v>
       </c>
       <c r="C211">
         <v>26</v>
@@ -7030,7 +7024,7 @@
         <v>15</v>
       </c>
       <c r="H211" t="s">
-        <v>42</v>
+        <v>39</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
@@ -7038,7 +7032,7 @@
         <v>211</v>
       </c>
       <c r="B212" t="s">
-        <v>302</v>
+        <v>287</v>
       </c>
       <c r="C212">
         <v>27</v>
@@ -7056,7 +7050,7 @@
         <v>15</v>
       </c>
       <c r="H212" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
@@ -7064,7 +7058,7 @@
         <v>212</v>
       </c>
       <c r="B213" t="s">
-        <v>303</v>
+        <v>288</v>
       </c>
       <c r="C213">
         <v>46</v>
@@ -7082,7 +7076,7 @@
         <v>15</v>
       </c>
       <c r="H213" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
@@ -7090,7 +7084,7 @@
         <v>213</v>
       </c>
       <c r="B214" t="s">
-        <v>304</v>
+        <v>289</v>
       </c>
       <c r="C214">
         <v>39</v>
@@ -7108,7 +7102,7 @@
         <v>15</v>
       </c>
       <c r="H214" t="s">
-        <v>103</v>
+        <v>95</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
@@ -7116,7 +7110,7 @@
         <v>214</v>
       </c>
       <c r="B215" t="s">
-        <v>305</v>
+        <v>290</v>
       </c>
       <c r="C215">
         <v>81</v>
@@ -7134,7 +7128,7 @@
         <v>15</v>
       </c>
       <c r="H215" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
@@ -7142,7 +7136,7 @@
         <v>215</v>
       </c>
       <c r="B216" t="s">
-        <v>306</v>
+        <v>291</v>
       </c>
       <c r="C216">
         <v>81</v>
@@ -7160,7 +7154,7 @@
         <v>15</v>
       </c>
       <c r="H216" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
@@ -7168,7 +7162,7 @@
         <v>216</v>
       </c>
       <c r="B217" t="s">
-        <v>307</v>
+        <v>292</v>
       </c>
       <c r="C217">
         <v>149</v>
@@ -7186,7 +7180,7 @@
         <v>15</v>
       </c>
       <c r="H217" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
@@ -7194,7 +7188,7 @@
         <v>217</v>
       </c>
       <c r="B218" t="s">
-        <v>308</v>
+        <v>293</v>
       </c>
       <c r="C218">
         <v>316</v>
@@ -7212,7 +7206,7 @@
         <v>15</v>
       </c>
       <c r="H218" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
@@ -7220,7 +7214,7 @@
         <v>218</v>
       </c>
       <c r="B219" t="s">
-        <v>309</v>
+        <v>294</v>
       </c>
       <c r="C219">
         <v>271</v>
@@ -7238,7 +7232,7 @@
         <v>15</v>
       </c>
       <c r="H219" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
@@ -7246,7 +7240,7 @@
         <v>219</v>
       </c>
       <c r="B220" t="s">
-        <v>310</v>
+        <v>295</v>
       </c>
       <c r="C220">
         <v>21</v>
@@ -7264,7 +7258,7 @@
         <v>15</v>
       </c>
       <c r="H220" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
@@ -7272,7 +7266,7 @@
         <v>220</v>
       </c>
       <c r="B221" t="s">
-        <v>311</v>
+        <v>296</v>
       </c>
       <c r="C221">
         <v>69</v>
@@ -7290,7 +7284,7 @@
         <v>15</v>
       </c>
       <c r="H221" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
@@ -7298,7 +7292,7 @@
         <v>221</v>
       </c>
       <c r="B222" t="s">
-        <v>312</v>
+        <v>297</v>
       </c>
       <c r="C222">
         <v>42</v>
@@ -7316,7 +7310,7 @@
         <v>15</v>
       </c>
       <c r="H222" t="s">
-        <v>79</v>
+        <v>73</v>
       </c>
       <c r="I222">
         <v>1</v>
@@ -7327,7 +7321,7 @@
         <v>222</v>
       </c>
       <c r="B223" t="s">
-        <v>331</v>
+        <v>316</v>
       </c>
       <c r="C223">
         <v>391</v>
@@ -7353,7 +7347,7 @@
         <v>223</v>
       </c>
       <c r="B224" t="s">
-        <v>313</v>
+        <v>298</v>
       </c>
       <c r="C224">
         <v>92</v>
@@ -7371,7 +7365,7 @@
         <v>15</v>
       </c>
       <c r="H224" t="s">
-        <v>297</v>
+        <v>282</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
@@ -7379,7 +7373,7 @@
         <v>224</v>
       </c>
       <c r="B225" t="s">
-        <v>314</v>
+        <v>299</v>
       </c>
       <c r="C225">
         <v>255</v>
@@ -7397,7 +7391,7 @@
         <v>21</v>
       </c>
       <c r="H225" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="I225">
         <v>1.1000000000000001</v>
@@ -7408,7 +7402,7 @@
         <v>225</v>
       </c>
       <c r="B226" t="s">
-        <v>315</v>
+        <v>300</v>
       </c>
       <c r="C226">
         <v>68</v>
@@ -7426,7 +7420,7 @@
         <v>21</v>
       </c>
       <c r="H226" t="s">
-        <v>174</v>
+        <v>163</v>
       </c>
       <c r="I226">
         <v>1</v>
@@ -7437,13 +7431,13 @@
         <v>226</v>
       </c>
       <c r="B227" t="s">
-        <v>316</v>
+        <v>301</v>
       </c>
       <c r="C227">
         <v>37</v>
       </c>
-      <c r="D227" t="s">
-        <v>28</v>
+      <c r="D227">
+        <v>0.2</v>
       </c>
       <c r="E227">
         <v>8.3000000000000007</v>
@@ -7455,7 +7449,7 @@
         <v>15</v>
       </c>
       <c r="H227" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
@@ -7463,7 +7457,7 @@
         <v>227</v>
       </c>
       <c r="B228" t="s">
-        <v>317</v>
+        <v>302</v>
       </c>
       <c r="C228">
         <v>242</v>
@@ -7481,7 +7475,7 @@
         <v>15</v>
       </c>
       <c r="H228" t="s">
-        <v>61</v>
+        <v>55</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
@@ -7489,7 +7483,7 @@
         <v>228</v>
       </c>
       <c r="B229" t="s">
-        <v>318</v>
+        <v>303</v>
       </c>
       <c r="C229">
         <v>242</v>
@@ -7507,7 +7501,7 @@
         <v>15</v>
       </c>
       <c r="H229" t="s">
-        <v>47</v>
+        <v>44</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
@@ -7515,7 +7509,7 @@
         <v>229</v>
       </c>
       <c r="B230" t="s">
-        <v>332</v>
+        <v>317</v>
       </c>
       <c r="C230">
         <v>96</v>
@@ -7533,7 +7527,7 @@
         <v>21</v>
       </c>
       <c r="H230" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="I230">
         <v>1</v>
@@ -7544,7 +7538,7 @@
         <v>230</v>
       </c>
       <c r="B231" t="s">
-        <v>319</v>
+        <v>304</v>
       </c>
       <c r="C231">
         <v>505</v>
@@ -7570,7 +7564,7 @@
         <v>231</v>
       </c>
       <c r="B232" t="s">
-        <v>320</v>
+        <v>305</v>
       </c>
       <c r="C232">
         <v>23</v>
@@ -7588,7 +7582,7 @@
         <v>15</v>
       </c>
       <c r="H232" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
@@ -7596,7 +7590,7 @@
         <v>232</v>
       </c>
       <c r="B233" t="s">
-        <v>321</v>
+        <v>306</v>
       </c>
       <c r="C233">
         <v>28</v>
@@ -7614,7 +7608,7 @@
         <v>21</v>
       </c>
       <c r="H233" t="s">
-        <v>39</v>
+        <v>328</v>
       </c>
       <c r="I233">
         <v>1</v>
@@ -7625,7 +7619,7 @@
         <v>233</v>
       </c>
       <c r="B234" t="s">
-        <v>322</v>
+        <v>307</v>
       </c>
       <c r="C234">
         <v>390</v>
@@ -7651,7 +7645,7 @@
         <v>234</v>
       </c>
       <c r="B235" t="s">
-        <v>323</v>
+        <v>308</v>
       </c>
       <c r="C235">
         <v>400</v>
@@ -7677,7 +7671,7 @@
         <v>235</v>
       </c>
       <c r="B236" t="s">
-        <v>324</v>
+        <v>309</v>
       </c>
       <c r="C236">
         <v>421</v>
@@ -7695,7 +7689,7 @@
         <v>15</v>
       </c>
       <c r="H236" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
@@ -7703,7 +7697,7 @@
         <v>236</v>
       </c>
       <c r="B237" t="s">
-        <v>325</v>
+        <v>310</v>
       </c>
       <c r="C237">
         <v>413</v>
@@ -7721,7 +7715,7 @@
         <v>15</v>
       </c>
       <c r="H237" t="s">
-        <v>201</v>
+        <v>190</v>
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
@@ -7729,7 +7723,7 @@
         <v>237</v>
       </c>
       <c r="B238" t="s">
-        <v>326</v>
+        <v>311</v>
       </c>
       <c r="C238">
         <v>39</v>
@@ -7747,7 +7741,7 @@
         <v>15</v>
       </c>
       <c r="H238" t="s">
-        <v>44</v>
+        <v>41</v>
       </c>
     </row>
   </sheetData>
@@ -7841,10 +7835,10 @@
         <v>1577</v>
       </c>
       <c r="D4" t="s">
-        <v>55</v>
+        <v>49</v>
       </c>
       <c r="F4" t="s">
-        <v>56</v>
+        <v>50</v>
       </c>
       <c r="H4" t="s">
         <v>15</v>
@@ -7882,10 +7876,10 @@
         <v>4714</v>
       </c>
       <c r="D5" t="s">
-        <v>68</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
-        <v>69</v>
+        <v>63</v>
       </c>
       <c r="H5" t="s">
         <v>15</v>
@@ -7920,10 +7914,10 @@
         <v>13461</v>
       </c>
       <c r="D6" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="F6" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="H6" t="s">
         <v>15</v>
@@ -7967,10 +7961,10 @@
         <v>13460</v>
       </c>
       <c r="D7" t="s">
-        <v>91</v>
+        <v>84</v>
       </c>
       <c r="F7" t="s">
-        <v>90</v>
+        <v>83</v>
       </c>
       <c r="H7" t="s">
         <v>15</v>

</xml_diff>

<commit_message>
made database IDs start from 0
</commit_message>
<xml_diff>
--- a/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
+++ b/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\NutriLearnVR\NutriLearnVR\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{310871BC-CA58-4354-BFE5-D3C4A194A888}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F8A298-CF03-4B76-80A5-64AF050B8226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8C58FACA-B588-4A2F-A614-585794A6AB4A}"/>
   </bookViews>
@@ -1438,8 +1438,8 @@
   <dimension ref="A1:I238"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A130" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E152" sqref="E152"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1482,7 +1482,7 @@
     </row>
     <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>18</v>
@@ -1508,7 +1508,7 @@
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>20</v>
@@ -1537,7 +1537,7 @@
     </row>
     <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>22</v>
@@ -1563,7 +1563,7 @@
     </row>
     <row r="5" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>28</v>
@@ -1589,7 +1589,7 @@
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>30</v>
@@ -1618,7 +1618,7 @@
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>33</v>
@@ -1644,7 +1644,7 @@
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>34</v>
@@ -1670,7 +1670,7 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>35</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>36</v>
@@ -1725,7 +1725,7 @@
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B11" t="s">
         <v>38</v>
@@ -1751,7 +1751,7 @@
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B12" t="s">
         <v>40</v>
@@ -1777,7 +1777,7 @@
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B13" t="s">
         <v>42</v>
@@ -1803,7 +1803,7 @@
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
         <v>43</v>
@@ -1829,7 +1829,7 @@
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B15" t="s">
         <v>45</v>
@@ -1855,7 +1855,7 @@
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B16" t="s">
         <v>46</v>
@@ -1881,7 +1881,7 @@
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B17" t="s">
         <v>47</v>
@@ -1907,7 +1907,7 @@
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B18" t="s">
         <v>51</v>
@@ -1933,7 +1933,7 @@
     </row>
     <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B19" t="s">
         <v>52</v>
@@ -1959,7 +1959,7 @@
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B20" t="s">
         <v>54</v>
@@ -1985,7 +1985,7 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B21" t="s">
         <v>60</v>
@@ -2011,7 +2011,7 @@
     </row>
     <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" t="s">
         <v>64</v>
@@ -2037,7 +2037,7 @@
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B23" t="s">
         <v>65</v>
@@ -2066,7 +2066,7 @@
     </row>
     <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B24" t="s">
         <v>67</v>
@@ -2092,7 +2092,7 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B25" t="s">
         <v>68</v>
@@ -2118,7 +2118,7 @@
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B26" t="s">
         <v>69</v>
@@ -2144,7 +2144,7 @@
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B27" t="s">
         <v>72</v>
@@ -2170,7 +2170,7 @@
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B28" t="s">
         <v>75</v>
@@ -2199,7 +2199,7 @@
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B29" t="s">
         <v>77</v>
@@ -2225,7 +2225,7 @@
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A30">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B30" t="s">
         <v>78</v>
@@ -2251,7 +2251,7 @@
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B31" t="s">
         <v>79</v>
@@ -2277,7 +2277,7 @@
     </row>
     <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B32" t="s">
         <v>80</v>
@@ -2303,7 +2303,7 @@
     </row>
     <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B33" t="s">
         <v>85</v>
@@ -2332,7 +2332,7 @@
     </row>
     <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="B34" t="s">
         <v>87</v>
@@ -2358,7 +2358,7 @@
     </row>
     <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="B35" t="s">
         <v>89</v>
@@ -2384,7 +2384,7 @@
     </row>
     <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B36" t="s">
         <v>90</v>
@@ -2410,7 +2410,7 @@
     </row>
     <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B37" t="s">
         <v>92</v>
@@ -2436,7 +2436,7 @@
     </row>
     <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B38" t="s">
         <v>93</v>
@@ -2462,7 +2462,7 @@
     </row>
     <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B39" t="s">
         <v>94</v>
@@ -2488,7 +2488,7 @@
     </row>
     <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B40" t="s">
         <v>96</v>
@@ -2514,7 +2514,7 @@
     </row>
     <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B41" t="s">
         <v>97</v>
@@ -2540,7 +2540,7 @@
     </row>
     <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="B42" t="s">
         <v>98</v>
@@ -2566,7 +2566,7 @@
     </row>
     <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B43" t="s">
         <v>99</v>
@@ -2592,7 +2592,7 @@
     </row>
     <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
         <v>100</v>
@@ -2618,7 +2618,7 @@
     </row>
     <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
         <v>103</v>
@@ -2644,7 +2644,7 @@
     </row>
     <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
         <v>105</v>
@@ -2670,7 +2670,7 @@
     </row>
     <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
         <v>107</v>
@@ -2696,7 +2696,7 @@
     </row>
     <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="B48" t="s">
         <v>109</v>
@@ -2722,7 +2722,7 @@
     </row>
     <row r="49" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A49">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="B49" t="s">
         <v>111</v>
@@ -2748,7 +2748,7 @@
     </row>
     <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="B50" t="s">
         <v>112</v>
@@ -2774,7 +2774,7 @@
     </row>
     <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="B51" t="s">
         <v>113</v>
@@ -2800,7 +2800,7 @@
     </row>
     <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="B52" t="s">
         <v>318</v>
@@ -2826,7 +2826,7 @@
     </row>
     <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="B53" t="s">
         <v>319</v>
@@ -2852,7 +2852,7 @@
     </row>
     <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="B54" t="s">
         <v>118</v>
@@ -2878,7 +2878,7 @@
     </row>
     <row r="55" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A55">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="B55" t="s">
         <v>119</v>
@@ -2904,7 +2904,7 @@
     </row>
     <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="B56" t="s">
         <v>120</v>
@@ -2933,7 +2933,7 @@
     </row>
     <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="B57" t="s">
         <v>121</v>
@@ -2959,7 +2959,7 @@
     </row>
     <row r="58" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A58">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="B58" t="s">
         <v>122</v>
@@ -2985,7 +2985,7 @@
     </row>
     <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="B59" t="s">
         <v>123</v>
@@ -3011,7 +3011,7 @@
     </row>
     <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="B60" t="s">
         <v>124</v>
@@ -3037,7 +3037,7 @@
     </row>
     <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="B61" t="s">
         <v>125</v>
@@ -3063,7 +3063,7 @@
     </row>
     <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="B62" t="s">
         <v>126</v>
@@ -3089,7 +3089,7 @@
     </row>
     <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="B63" t="s">
         <v>128</v>
@@ -3115,7 +3115,7 @@
     </row>
     <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="B64" t="s">
         <v>130</v>
@@ -3141,7 +3141,7 @@
     </row>
     <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="B65" t="s">
         <v>132</v>
@@ -3167,7 +3167,7 @@
     </row>
     <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="B66" t="s">
         <v>134</v>
@@ -3193,7 +3193,7 @@
     </row>
     <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="B67" t="s">
         <v>135</v>
@@ -3219,7 +3219,7 @@
     </row>
     <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B68" t="s">
         <v>137</v>
@@ -3245,7 +3245,7 @@
     </row>
     <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="B69" t="s">
         <v>138</v>
@@ -3271,7 +3271,7 @@
     </row>
     <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B70" t="s">
         <v>140</v>
@@ -3297,7 +3297,7 @@
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="B71" t="s">
         <v>141</v>
@@ -3323,7 +3323,7 @@
     </row>
     <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="B72" t="s">
         <v>142</v>
@@ -3349,7 +3349,7 @@
     </row>
     <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="B73" t="s">
         <v>143</v>
@@ -3375,7 +3375,7 @@
     </row>
     <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="B74" t="s">
         <v>144</v>
@@ -3404,7 +3404,7 @@
     </row>
     <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A75">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="B75" t="s">
         <v>146</v>
@@ -3433,7 +3433,7 @@
     </row>
     <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="B76" t="s">
         <v>147</v>
@@ -3459,7 +3459,7 @@
     </row>
     <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="B77" t="s">
         <v>148</v>
@@ -3485,7 +3485,7 @@
     </row>
     <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="B78" t="s">
         <v>150</v>
@@ -3511,7 +3511,7 @@
     </row>
     <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B79" t="s">
         <v>151</v>
@@ -3537,7 +3537,7 @@
     </row>
     <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A80">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="B80" t="s">
         <v>153</v>
@@ -3563,7 +3563,7 @@
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81">
-        <v>80</v>
+        <v>79</v>
       </c>
       <c r="B81" t="s">
         <v>154</v>
@@ -3589,7 +3589,7 @@
     </row>
     <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A82">
-        <v>81</v>
+        <v>80</v>
       </c>
       <c r="B82" t="s">
         <v>156</v>
@@ -3615,7 +3615,7 @@
     </row>
     <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83">
-        <v>82</v>
+        <v>81</v>
       </c>
       <c r="B83" t="s">
         <v>158</v>
@@ -3641,7 +3641,7 @@
     </row>
     <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84">
-        <v>83</v>
+        <v>82</v>
       </c>
       <c r="B84" t="s">
         <v>160</v>
@@ -3667,7 +3667,7 @@
     </row>
     <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85">
-        <v>84</v>
+        <v>83</v>
       </c>
       <c r="B85" t="s">
         <v>162</v>
@@ -3693,7 +3693,7 @@
     </row>
     <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86">
-        <v>85</v>
+        <v>84</v>
       </c>
       <c r="B86" t="s">
         <v>164</v>
@@ -3719,7 +3719,7 @@
     </row>
     <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87">
-        <v>86</v>
+        <v>85</v>
       </c>
       <c r="B87" t="s">
         <v>165</v>
@@ -3745,7 +3745,7 @@
     </row>
     <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A88">
-        <v>87</v>
+        <v>86</v>
       </c>
       <c r="B88" t="s">
         <v>166</v>
@@ -3774,7 +3774,7 @@
     </row>
     <row r="89" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A89">
-        <v>88</v>
+        <v>87</v>
       </c>
       <c r="B89" t="s">
         <v>167</v>
@@ -3800,7 +3800,7 @@
     </row>
     <row r="90" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A90">
-        <v>89</v>
+        <v>88</v>
       </c>
       <c r="B90" t="s">
         <v>168</v>
@@ -3826,7 +3826,7 @@
     </row>
     <row r="91" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A91">
-        <v>90</v>
+        <v>89</v>
       </c>
       <c r="B91" t="s">
         <v>169</v>
@@ -3852,7 +3852,7 @@
     </row>
     <row r="92" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A92">
-        <v>91</v>
+        <v>90</v>
       </c>
       <c r="B92" t="s">
         <v>170</v>
@@ -3878,7 +3878,7 @@
     </row>
     <row r="93" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A93">
-        <v>92</v>
+        <v>91</v>
       </c>
       <c r="B93" t="s">
         <v>171</v>
@@ -3907,7 +3907,7 @@
     </row>
     <row r="94" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A94">
-        <v>93</v>
+        <v>92</v>
       </c>
       <c r="B94" t="s">
         <v>172</v>
@@ -3933,7 +3933,7 @@
     </row>
     <row r="95" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A95">
-        <v>94</v>
+        <v>93</v>
       </c>
       <c r="B95" t="s">
         <v>173</v>
@@ -3959,7 +3959,7 @@
     </row>
     <row r="96" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A96">
-        <v>95</v>
+        <v>94</v>
       </c>
       <c r="B96" t="s">
         <v>175</v>
@@ -3985,7 +3985,7 @@
     </row>
     <row r="97" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A97">
-        <v>96</v>
+        <v>95</v>
       </c>
       <c r="B97" t="s">
         <v>176</v>
@@ -4011,7 +4011,7 @@
     </row>
     <row r="98" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A98">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B98" t="s">
         <v>312</v>
@@ -4037,7 +4037,7 @@
     </row>
     <row r="99" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A99">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="B99" t="s">
         <v>178</v>
@@ -4066,7 +4066,7 @@
     </row>
     <row r="100" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A100">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B100" t="s">
         <v>180</v>
@@ -4095,7 +4095,7 @@
     </row>
     <row r="101" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A101">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B101" t="s">
         <v>181</v>
@@ -4124,7 +4124,7 @@
     </row>
     <row r="102" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A102">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B102" t="s">
         <v>182</v>
@@ -4153,7 +4153,7 @@
     </row>
     <row r="103" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A103">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="B103" t="s">
         <v>183</v>
@@ -4179,7 +4179,7 @@
     </row>
     <row r="104" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A104">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B104" t="s">
         <v>184</v>
@@ -4205,7 +4205,7 @@
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A105">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="B105" t="s">
         <v>185</v>
@@ -4231,7 +4231,7 @@
     </row>
     <row r="106" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A106">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B106" t="s">
         <v>320</v>
@@ -4257,7 +4257,7 @@
     </row>
     <row r="107" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A107">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="B107" t="s">
         <v>186</v>
@@ -4283,7 +4283,7 @@
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A108">
-        <v>107</v>
+        <v>106</v>
       </c>
       <c r="B108" t="s">
         <v>187</v>
@@ -4312,7 +4312,7 @@
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A109">
-        <v>108</v>
+        <v>107</v>
       </c>
       <c r="B109" t="s">
         <v>188</v>
@@ -4338,7 +4338,7 @@
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A110">
-        <v>109</v>
+        <v>108</v>
       </c>
       <c r="B110" t="s">
         <v>189</v>
@@ -4364,7 +4364,7 @@
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A111">
-        <v>110</v>
+        <v>109</v>
       </c>
       <c r="B111" t="s">
         <v>191</v>
@@ -4390,7 +4390,7 @@
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A112">
-        <v>111</v>
+        <v>110</v>
       </c>
       <c r="B112" t="s">
         <v>192</v>
@@ -4416,7 +4416,7 @@
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A113">
-        <v>112</v>
+        <v>111</v>
       </c>
       <c r="B113" t="s">
         <v>193</v>
@@ -4442,7 +4442,7 @@
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A114">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="B114" t="s">
         <v>194</v>
@@ -4468,7 +4468,7 @@
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A115">
-        <v>114</v>
+        <v>113</v>
       </c>
       <c r="B115" t="s">
         <v>195</v>
@@ -4497,7 +4497,7 @@
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A116">
-        <v>115</v>
+        <v>114</v>
       </c>
       <c r="B116" t="s">
         <v>196</v>
@@ -4523,7 +4523,7 @@
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A117">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="B117" t="s">
         <v>197</v>
@@ -4549,7 +4549,7 @@
     </row>
     <row r="118" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A118">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="B118" t="s">
         <v>198</v>
@@ -4575,7 +4575,7 @@
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A119">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="B119" t="s">
         <v>199</v>
@@ -4601,7 +4601,7 @@
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A120">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="B120" t="s">
         <v>200</v>
@@ -4630,7 +4630,7 @@
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A121">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="B121" t="s">
         <v>201</v>
@@ -4656,7 +4656,7 @@
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A122">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="B122" t="s">
         <v>203</v>
@@ -4682,7 +4682,7 @@
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A123">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="B123" t="s">
         <v>204</v>
@@ -4708,7 +4708,7 @@
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A124">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="B124" t="s">
         <v>205</v>
@@ -4734,7 +4734,7 @@
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A125">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="B125" t="s">
         <v>206</v>
@@ -4760,7 +4760,7 @@
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A126">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B126" t="s">
         <v>207</v>
@@ -4786,7 +4786,7 @@
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A127">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="B127" t="s">
         <v>208</v>
@@ -4812,7 +4812,7 @@
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A128">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="B128" t="s">
         <v>209</v>
@@ -4838,7 +4838,7 @@
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A129">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="B129" t="s">
         <v>210</v>
@@ -4864,7 +4864,7 @@
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A130">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="B130" t="s">
         <v>211</v>
@@ -4890,7 +4890,7 @@
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A131">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="B131" t="s">
         <v>212</v>
@@ -4916,7 +4916,7 @@
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A132">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="B132" t="s">
         <v>213</v>
@@ -4942,7 +4942,7 @@
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A133">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="B133" t="s">
         <v>215</v>
@@ -4971,7 +4971,7 @@
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A134">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B134" t="s">
         <v>217</v>
@@ -4997,7 +4997,7 @@
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A135">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B135" t="s">
         <v>218</v>
@@ -5026,7 +5026,7 @@
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A136">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B136" t="s">
         <v>219</v>
@@ -5052,7 +5052,7 @@
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A137">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B137" t="s">
         <v>220</v>
@@ -5078,7 +5078,7 @@
     </row>
     <row r="138" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A138">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B138" t="s">
         <v>314</v>
@@ -5107,7 +5107,7 @@
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A139">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B139" t="s">
         <v>315</v>
@@ -5136,7 +5136,7 @@
     </row>
     <row r="140" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A140">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B140" t="s">
         <v>221</v>
@@ -5162,7 +5162,7 @@
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A141">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B141" t="s">
         <v>222</v>
@@ -5188,7 +5188,7 @@
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A142">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B142" t="s">
         <v>223</v>
@@ -5214,7 +5214,7 @@
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A143">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B143" t="s">
         <v>224</v>
@@ -5240,7 +5240,7 @@
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A144">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B144" t="s">
         <v>225</v>
@@ -5266,7 +5266,7 @@
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A145">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B145" t="s">
         <v>321</v>
@@ -5292,7 +5292,7 @@
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A146">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B146" t="s">
         <v>226</v>
@@ -5318,7 +5318,7 @@
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A147">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B147" t="s">
         <v>227</v>
@@ -5347,7 +5347,7 @@
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A148">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B148" t="s">
         <v>228</v>
@@ -5373,7 +5373,7 @@
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A149">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B149" t="s">
         <v>229</v>
@@ -5402,7 +5402,7 @@
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A150">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B150" t="s">
         <v>230</v>
@@ -5428,7 +5428,7 @@
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A151">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B151" t="s">
         <v>231</v>
@@ -5454,7 +5454,7 @@
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A152">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B152" t="s">
         <v>232</v>
@@ -5480,7 +5480,7 @@
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A153">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B153" t="s">
         <v>233</v>
@@ -5506,7 +5506,7 @@
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A154">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B154" t="s">
         <v>234</v>
@@ -5532,7 +5532,7 @@
     </row>
     <row r="155" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A155">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B155" t="s">
         <v>235</v>
@@ -5558,7 +5558,7 @@
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A156">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B156" t="s">
         <v>236</v>
@@ -5584,7 +5584,7 @@
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A157">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B157" t="s">
         <v>237</v>
@@ -5610,7 +5610,7 @@
     </row>
     <row r="158" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A158">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B158" t="s">
         <v>238</v>
@@ -5636,7 +5636,7 @@
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A159">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B159" t="s">
         <v>239</v>
@@ -5662,7 +5662,7 @@
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A160">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B160" t="s">
         <v>240</v>
@@ -5688,7 +5688,7 @@
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A161">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B161" t="s">
         <v>241</v>
@@ -5714,7 +5714,7 @@
     </row>
     <row r="162" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A162">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B162" t="s">
         <v>242</v>
@@ -5740,7 +5740,7 @@
     </row>
     <row r="163" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A163">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B163" t="s">
         <v>243</v>
@@ -5766,7 +5766,7 @@
     </row>
     <row r="164" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A164">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B164" t="s">
         <v>244</v>
@@ -5792,7 +5792,7 @@
     </row>
     <row r="165" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A165">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B165" t="s">
         <v>245</v>
@@ -5818,7 +5818,7 @@
     </row>
     <row r="166" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A166">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B166" t="s">
         <v>246</v>
@@ -5844,7 +5844,7 @@
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A167">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B167" t="s">
         <v>247</v>
@@ -5870,7 +5870,7 @@
     </row>
     <row r="168" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A168">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B168" t="s">
         <v>248</v>
@@ -5896,7 +5896,7 @@
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A169">
-        <v>168</v>
+        <v>167</v>
       </c>
       <c r="B169" t="s">
         <v>322</v>
@@ -5922,7 +5922,7 @@
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A170">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="B170" t="s">
         <v>323</v>
@@ -5948,7 +5948,7 @@
     </row>
     <row r="171" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A171">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="B171" t="s">
         <v>324</v>
@@ -5974,7 +5974,7 @@
     </row>
     <row r="172" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A172">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="B172" t="s">
         <v>249</v>
@@ -6000,7 +6000,7 @@
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A173">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="B173" t="s">
         <v>250</v>
@@ -6026,7 +6026,7 @@
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A174">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="B174" t="s">
         <v>251</v>
@@ -6052,7 +6052,7 @@
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A175">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B175" t="s">
         <v>252</v>
@@ -6081,7 +6081,7 @@
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A176">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B176" t="s">
         <v>253</v>
@@ -6107,7 +6107,7 @@
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A177">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="B177" t="s">
         <v>254</v>
@@ -6133,7 +6133,7 @@
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A178">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="B178" t="s">
         <v>256</v>
@@ -6159,7 +6159,7 @@
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A179">
-        <v>178</v>
+        <v>177</v>
       </c>
       <c r="B179" t="s">
         <v>338</v>
@@ -6185,7 +6185,7 @@
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A180">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="B180" t="s">
         <v>257</v>
@@ -6211,7 +6211,7 @@
     </row>
     <row r="181" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A181">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="B181" t="s">
         <v>339</v>
@@ -6237,7 +6237,7 @@
     </row>
     <row r="182" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A182">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="B182" t="s">
         <v>258</v>
@@ -6263,7 +6263,7 @@
     </row>
     <row r="183" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A183">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="B183" t="s">
         <v>325</v>
@@ -6289,7 +6289,7 @@
     </row>
     <row r="184" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A184">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B184" t="s">
         <v>326</v>
@@ -6315,7 +6315,7 @@
     </row>
     <row r="185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A185">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B185" t="s">
         <v>259</v>
@@ -6341,7 +6341,7 @@
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A186">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B186" t="s">
         <v>260</v>
@@ -6367,7 +6367,7 @@
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A187">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B187" t="s">
         <v>261</v>
@@ -6393,7 +6393,7 @@
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A188">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="B188" t="s">
         <v>262</v>
@@ -6419,7 +6419,7 @@
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A189">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="B189" t="s">
         <v>263</v>
@@ -6445,7 +6445,7 @@
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A190">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B190" t="s">
         <v>264</v>
@@ -6474,7 +6474,7 @@
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A191">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B191" t="s">
         <v>265</v>
@@ -6503,7 +6503,7 @@
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A192">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="B192" t="s">
         <v>266</v>
@@ -6529,7 +6529,7 @@
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A193">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="B193" t="s">
         <v>267</v>
@@ -6555,7 +6555,7 @@
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A194">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B194" t="s">
         <v>268</v>
@@ -6581,7 +6581,7 @@
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A195">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B195" t="s">
         <v>269</v>
@@ -6607,7 +6607,7 @@
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A196">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B196" t="s">
         <v>270</v>
@@ -6636,7 +6636,7 @@
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A197">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B197" t="s">
         <v>271</v>
@@ -6662,7 +6662,7 @@
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A198">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B198" t="s">
         <v>272</v>
@@ -6688,7 +6688,7 @@
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A199">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B199" t="s">
         <v>273</v>
@@ -6714,7 +6714,7 @@
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A200">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B200" t="s">
         <v>274</v>
@@ -6740,7 +6740,7 @@
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A201">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B201" t="s">
         <v>275</v>
@@ -6766,7 +6766,7 @@
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A202">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B202" t="s">
         <v>276</v>
@@ -6792,7 +6792,7 @@
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A203">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B203" t="s">
         <v>277</v>
@@ -6818,7 +6818,7 @@
     </row>
     <row r="204" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A204">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B204" t="s">
         <v>278</v>
@@ -6844,7 +6844,7 @@
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A205">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B205" t="s">
         <v>279</v>
@@ -6870,7 +6870,7 @@
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A206">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B206" t="s">
         <v>280</v>
@@ -6896,7 +6896,7 @@
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A207">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B207" t="s">
         <v>281</v>
@@ -6922,7 +6922,7 @@
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A208">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B208" t="s">
         <v>283</v>
@@ -6948,7 +6948,7 @@
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A209">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="B209" t="s">
         <v>284</v>
@@ -6974,7 +6974,7 @@
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A210">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B210" t="s">
         <v>285</v>
@@ -7003,7 +7003,7 @@
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A211">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B211" t="s">
         <v>286</v>
@@ -7029,7 +7029,7 @@
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A212">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B212" t="s">
         <v>287</v>
@@ -7055,7 +7055,7 @@
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A213">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B213" t="s">
         <v>288</v>
@@ -7081,7 +7081,7 @@
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A214">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="B214" t="s">
         <v>289</v>
@@ -7107,7 +7107,7 @@
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A215">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="B215" t="s">
         <v>290</v>
@@ -7133,7 +7133,7 @@
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A216">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B216" t="s">
         <v>291</v>
@@ -7159,7 +7159,7 @@
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A217">
-        <v>216</v>
+        <v>215</v>
       </c>
       <c r="B217" t="s">
         <v>292</v>
@@ -7185,7 +7185,7 @@
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A218">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B218" t="s">
         <v>293</v>
@@ -7211,7 +7211,7 @@
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A219">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B219" t="s">
         <v>294</v>
@@ -7237,7 +7237,7 @@
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A220">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B220" t="s">
         <v>295</v>
@@ -7263,7 +7263,7 @@
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A221">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B221" t="s">
         <v>296</v>
@@ -7289,7 +7289,7 @@
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A222">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B222" t="s">
         <v>297</v>
@@ -7318,7 +7318,7 @@
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A223">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B223" t="s">
         <v>316</v>
@@ -7344,7 +7344,7 @@
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A224">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B224" t="s">
         <v>298</v>
@@ -7370,7 +7370,7 @@
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A225">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B225" t="s">
         <v>299</v>
@@ -7399,7 +7399,7 @@
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A226">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B226" t="s">
         <v>300</v>
@@ -7428,7 +7428,7 @@
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A227">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B227" t="s">
         <v>301</v>
@@ -7454,7 +7454,7 @@
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A228">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B228" t="s">
         <v>302</v>
@@ -7480,7 +7480,7 @@
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A229">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B229" t="s">
         <v>303</v>
@@ -7506,7 +7506,7 @@
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A230">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B230" t="s">
         <v>317</v>
@@ -7535,7 +7535,7 @@
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A231">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B231" t="s">
         <v>304</v>
@@ -7561,7 +7561,7 @@
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A232">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B232" t="s">
         <v>305</v>
@@ -7587,7 +7587,7 @@
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A233">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B233" t="s">
         <v>306</v>
@@ -7616,7 +7616,7 @@
     </row>
     <row r="234" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A234">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B234" t="s">
         <v>307</v>
@@ -7642,7 +7642,7 @@
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A235">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B235" t="s">
         <v>308</v>
@@ -7668,7 +7668,7 @@
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A236">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B236" t="s">
         <v>309</v>
@@ -7694,7 +7694,7 @@
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A237">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B237" t="s">
         <v>310</v>
@@ -7720,7 +7720,7 @@
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A238">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B238" t="s">
         <v>311</v>

</xml_diff>

<commit_message>
small additions to database
</commit_message>
<xml_diff>
--- a/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
+++ b/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26827"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\NutriLearnVR\NutriLearnVR\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{21F8A298-CF03-4B76-80A5-64AF050B8226}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE1BC114-FF7E-4CC6-AA1E-459C7AA802C8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8C58FACA-B588-4A2F-A614-585794A6AB4A}"/>
   </bookViews>
@@ -19,17 +19,28 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Generische Lebensmittel'!#REF!</definedName>
   </definedNames>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+        <xcalcf:feature name="microsoft.com:ARRAYTEXT_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="769" uniqueCount="340">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="781" uniqueCount="344">
   <si>
     <t>ID</t>
   </si>
@@ -940,9 +951,6 @@
     <t>Weissbrot</t>
   </si>
   <si>
-    <t>Wienerli</t>
-  </si>
-  <si>
     <t>Zimtstern</t>
   </si>
   <si>
@@ -1049,6 +1057,21 @@
   </si>
   <si>
     <t>Rind, Filet, medium gebraten (ohne Zustatz von Fett und Salz)</t>
+  </si>
+  <si>
+    <t>Wiener Würstchen</t>
+  </si>
+  <si>
+    <t>Zucchini, roh</t>
+  </si>
+  <si>
+    <t>rote Zwiebel, roh</t>
+  </si>
+  <si>
+    <t>Kartoffel, roh</t>
+  </si>
+  <si>
+    <t>Walnuss Kerne</t>
   </si>
 </sst>
 </file>
@@ -1435,11 +1458,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB881A-4068-4DEA-B356-9AC1A56CFC86}">
-  <dimension ref="A1:I238"/>
+  <dimension ref="A1:I242"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
+      <pane ySplit="1" topLeftCell="A205" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A229" sqref="A229:H229"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1717,7 +1740,7 @@
         <v>21</v>
       </c>
       <c r="H10" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I10">
         <v>1.04</v>
@@ -1850,7 +1873,7 @@
         <v>15</v>
       </c>
       <c r="H15" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.25">
@@ -1876,7 +1899,7 @@
         <v>15</v>
       </c>
       <c r="H16" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
     </row>
     <row r="17" spans="1:9" x14ac:dyDescent="0.25">
@@ -2058,7 +2081,7 @@
         <v>21</v>
       </c>
       <c r="H23" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I23">
         <v>1.04</v>
@@ -2191,7 +2214,7 @@
         <v>15</v>
       </c>
       <c r="H28" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="I28">
         <v>0.9</v>
@@ -2803,7 +2826,7 @@
         <v>50</v>
       </c>
       <c r="B52" t="s">
-        <v>318</v>
+        <v>317</v>
       </c>
       <c r="C52">
         <v>76</v>
@@ -2829,7 +2852,7 @@
         <v>51</v>
       </c>
       <c r="B53" t="s">
-        <v>319</v>
+        <v>318</v>
       </c>
       <c r="C53">
         <v>192</v>
@@ -3292,7 +3315,7 @@
         <v>15</v>
       </c>
       <c r="H70" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
     </row>
     <row r="71" spans="1:9" x14ac:dyDescent="0.25">
@@ -3425,7 +3448,7 @@
         <v>21</v>
       </c>
       <c r="H75" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="I75">
         <v>1</v>
@@ -3558,7 +3581,7 @@
         <v>15</v>
       </c>
       <c r="H80" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
     </row>
     <row r="81" spans="1:9" x14ac:dyDescent="0.25">
@@ -4014,7 +4037,7 @@
         <v>96</v>
       </c>
       <c r="B98" t="s">
-        <v>312</v>
+        <v>311</v>
       </c>
       <c r="C98">
         <v>117</v>
@@ -4200,7 +4223,7 @@
         <v>15</v>
       </c>
       <c r="H104" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
     </row>
     <row r="105" spans="1:9" x14ac:dyDescent="0.25">
@@ -4234,19 +4257,19 @@
         <v>104</v>
       </c>
       <c r="B106" t="s">
-        <v>320</v>
+        <v>342</v>
       </c>
       <c r="C106">
-        <v>42</v>
+        <v>70</v>
       </c>
       <c r="D106">
-        <v>0.4</v>
+        <v>0.1</v>
       </c>
       <c r="E106">
-        <v>7.6</v>
+        <v>14.6</v>
       </c>
       <c r="F106">
-        <v>0.6</v>
+        <v>2</v>
       </c>
       <c r="G106" t="s">
         <v>15</v>
@@ -4260,25 +4283,25 @@
         <v>105</v>
       </c>
       <c r="B107" t="s">
-        <v>186</v>
+        <v>319</v>
       </c>
       <c r="C107">
-        <v>303</v>
+        <v>42</v>
       </c>
       <c r="D107">
-        <v>20.8</v>
+        <v>0.4</v>
       </c>
       <c r="E107">
-        <v>14.5</v>
+        <v>7.6</v>
       </c>
       <c r="F107">
-        <v>14.3</v>
+        <v>0.6</v>
       </c>
       <c r="G107" t="s">
         <v>15</v>
       </c>
       <c r="H107" t="s">
-        <v>139</v>
+        <v>41</v>
       </c>
     </row>
     <row r="108" spans="1:9" x14ac:dyDescent="0.25">
@@ -4286,28 +4309,25 @@
         <v>106</v>
       </c>
       <c r="B108" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="C108">
-        <v>117</v>
+        <v>303</v>
       </c>
       <c r="D108">
-        <v>0.4</v>
+        <v>20.8</v>
       </c>
       <c r="E108">
-        <v>26</v>
+        <v>14.5</v>
       </c>
       <c r="F108">
-        <v>2</v>
+        <v>14.3</v>
       </c>
       <c r="G108" t="s">
         <v>15</v>
       </c>
       <c r="H108" t="s">
-        <v>59</v>
-      </c>
-      <c r="I108">
-        <v>1.1399999999999999</v>
+        <v>139</v>
       </c>
     </row>
     <row r="109" spans="1:9" x14ac:dyDescent="0.25">
@@ -4315,25 +4335,28 @@
         <v>107</v>
       </c>
       <c r="B109" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="C109">
-        <v>62</v>
+        <v>117</v>
       </c>
       <c r="D109">
         <v>0.4</v>
       </c>
       <c r="E109">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F109">
-        <v>0.8</v>
+        <v>2</v>
       </c>
       <c r="G109" t="s">
         <v>15</v>
       </c>
       <c r="H109" t="s">
-        <v>29</v>
+        <v>59</v>
+      </c>
+      <c r="I109">
+        <v>1.1399999999999999</v>
       </c>
     </row>
     <row r="110" spans="1:9" x14ac:dyDescent="0.25">
@@ -4341,25 +4364,25 @@
         <v>108</v>
       </c>
       <c r="B110" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="C110">
-        <v>332</v>
+        <v>62</v>
       </c>
       <c r="D110">
-        <v>1.7</v>
+        <v>0.4</v>
       </c>
       <c r="E110">
-        <v>61.1</v>
+        <v>13</v>
       </c>
       <c r="F110">
-        <v>12</v>
+        <v>0.8</v>
       </c>
       <c r="G110" t="s">
         <v>15</v>
       </c>
       <c r="H110" t="s">
-        <v>190</v>
+        <v>29</v>
       </c>
     </row>
     <row r="111" spans="1:9" x14ac:dyDescent="0.25">
@@ -4367,25 +4390,25 @@
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>191</v>
+        <v>189</v>
       </c>
       <c r="C111">
-        <v>137</v>
+        <v>332</v>
       </c>
       <c r="D111">
-        <v>0.5</v>
+        <v>1.7</v>
       </c>
       <c r="E111">
-        <v>24.5</v>
+        <v>61.1</v>
       </c>
       <c r="F111">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="G111" t="s">
         <v>15</v>
       </c>
       <c r="H111" t="s">
-        <v>41</v>
+        <v>190</v>
       </c>
     </row>
     <row r="112" spans="1:9" x14ac:dyDescent="0.25">
@@ -4393,25 +4416,25 @@
         <v>110</v>
       </c>
       <c r="B112" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="C112">
-        <v>442</v>
+        <v>137</v>
       </c>
       <c r="D112">
-        <v>17.399999999999999</v>
+        <v>0.5</v>
       </c>
       <c r="E112">
-        <v>58.8</v>
+        <v>24.5</v>
       </c>
       <c r="F112">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G112" t="s">
         <v>15</v>
       </c>
       <c r="H112" t="s">
-        <v>106</v>
+        <v>41</v>
       </c>
     </row>
     <row r="113" spans="1:9" x14ac:dyDescent="0.25">
@@ -4419,25 +4442,25 @@
         <v>111</v>
       </c>
       <c r="B113" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="C113">
-        <v>223</v>
+        <v>442</v>
       </c>
       <c r="D113">
-        <v>15.6</v>
+        <v>17.399999999999999</v>
       </c>
       <c r="E113">
-        <v>0.7</v>
+        <v>58.8</v>
       </c>
       <c r="F113">
-        <v>19.8</v>
+        <v>9</v>
       </c>
       <c r="G113" t="s">
         <v>15</v>
       </c>
       <c r="H113" t="s">
-        <v>70</v>
+        <v>106</v>
       </c>
     </row>
     <row r="114" spans="1:9" x14ac:dyDescent="0.25">
@@ -4445,25 +4468,25 @@
         <v>112</v>
       </c>
       <c r="B114" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="C114">
-        <v>214</v>
+        <v>223</v>
       </c>
       <c r="D114">
-        <v>21.3</v>
+        <v>15.6</v>
       </c>
       <c r="E114">
-        <v>3.1</v>
+        <v>0.7</v>
       </c>
       <c r="F114">
-        <v>2.4</v>
+        <v>19.8</v>
       </c>
       <c r="G114" t="s">
         <v>15</v>
       </c>
       <c r="H114" t="s">
-        <v>57</v>
+        <v>70</v>
       </c>
     </row>
     <row r="115" spans="1:9" x14ac:dyDescent="0.25">
@@ -4471,28 +4494,25 @@
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="C115">
-        <v>246</v>
+        <v>214</v>
       </c>
       <c r="D115">
-        <v>0.5</v>
+        <v>21.3</v>
       </c>
       <c r="E115">
-        <v>58.7</v>
+        <v>3.1</v>
       </c>
       <c r="F115">
-        <v>0.5</v>
+        <v>2.4</v>
       </c>
       <c r="G115" t="s">
         <v>15</v>
       </c>
       <c r="H115" t="s">
-        <v>116</v>
-      </c>
-      <c r="I115">
-        <v>1.4</v>
+        <v>57</v>
       </c>
     </row>
     <row r="116" spans="1:9" x14ac:dyDescent="0.25">
@@ -4500,25 +4520,28 @@
         <v>114</v>
       </c>
       <c r="B116" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="C116">
-        <v>14</v>
+        <v>246</v>
       </c>
       <c r="D116">
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="E116">
-        <v>1.1000000000000001</v>
+        <v>58.7</v>
       </c>
       <c r="F116">
-        <v>1.3</v>
+        <v>0.5</v>
       </c>
       <c r="G116" t="s">
         <v>15</v>
       </c>
       <c r="H116" t="s">
-        <v>41</v>
+        <v>116</v>
+      </c>
+      <c r="I116">
+        <v>1.4</v>
       </c>
     </row>
     <row r="117" spans="1:9" x14ac:dyDescent="0.25">
@@ -4526,19 +4549,19 @@
         <v>115</v>
       </c>
       <c r="B117" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="C117">
-        <v>28</v>
+        <v>14</v>
       </c>
       <c r="D117">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E117">
-        <v>4.5999999999999996</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F117">
-        <v>1.1000000000000001</v>
+        <v>1.3</v>
       </c>
       <c r="G117" t="s">
         <v>15</v>
@@ -4552,25 +4575,25 @@
         <v>116</v>
       </c>
       <c r="B118" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="C118">
-        <v>615</v>
+        <v>28</v>
       </c>
       <c r="D118">
-        <v>49.1</v>
+        <v>0.1</v>
       </c>
       <c r="E118">
-        <v>4.7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="F118">
-        <v>35.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G118" t="s">
         <v>15</v>
       </c>
       <c r="H118" t="s">
-        <v>57</v>
+        <v>41</v>
       </c>
     </row>
     <row r="119" spans="1:9" x14ac:dyDescent="0.25">
@@ -4578,25 +4601,25 @@
         <v>117</v>
       </c>
       <c r="B119" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="C119">
-        <v>167</v>
+        <v>615</v>
       </c>
       <c r="D119">
-        <v>8.1999999999999993</v>
+        <v>49.1</v>
       </c>
       <c r="E119">
-        <v>0</v>
+        <v>4.7</v>
       </c>
       <c r="F119">
-        <v>23.2</v>
+        <v>35.6</v>
       </c>
       <c r="G119" t="s">
         <v>15</v>
       </c>
       <c r="H119" t="s">
-        <v>115</v>
+        <v>57</v>
       </c>
     </row>
     <row r="120" spans="1:9" x14ac:dyDescent="0.25">
@@ -4604,28 +4627,25 @@
         <v>118</v>
       </c>
       <c r="B120" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="C120">
-        <v>47</v>
+        <v>167</v>
       </c>
       <c r="D120">
-        <v>2.8</v>
+        <v>8.1999999999999993</v>
       </c>
       <c r="E120">
-        <v>3.2</v>
+        <v>0</v>
       </c>
       <c r="F120">
-        <v>2.2000000000000002</v>
+        <v>23.2</v>
       </c>
       <c r="G120" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H120" t="s">
-        <v>332</v>
-      </c>
-      <c r="I120">
-        <v>0.88</v>
+        <v>115</v>
       </c>
     </row>
     <row r="121" spans="1:9" x14ac:dyDescent="0.25">
@@ -4633,25 +4653,28 @@
         <v>119</v>
       </c>
       <c r="B121" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="C121">
-        <v>444</v>
+        <v>47</v>
       </c>
       <c r="D121">
-        <v>18.899999999999999</v>
+        <v>2.8</v>
       </c>
       <c r="E121">
-        <v>60.2</v>
+        <v>3.2</v>
       </c>
       <c r="F121">
-        <v>6.5</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G121" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H121" t="s">
-        <v>61</v>
+        <v>331</v>
+      </c>
+      <c r="I121">
+        <v>0.88</v>
       </c>
     </row>
     <row r="122" spans="1:9" x14ac:dyDescent="0.25">
@@ -4659,25 +4682,25 @@
         <v>120</v>
       </c>
       <c r="B122" t="s">
-        <v>203</v>
+        <v>201</v>
       </c>
       <c r="C122">
-        <v>134</v>
+        <v>444</v>
       </c>
       <c r="D122">
-        <v>0.6</v>
+        <v>18.899999999999999</v>
       </c>
       <c r="E122">
-        <v>19</v>
+        <v>60.2</v>
       </c>
       <c r="F122">
-        <v>11</v>
+        <v>6.5</v>
       </c>
       <c r="G122" t="s">
         <v>15</v>
       </c>
       <c r="H122" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="123" spans="1:9" x14ac:dyDescent="0.25">
@@ -4685,25 +4708,25 @@
         <v>121</v>
       </c>
       <c r="B123" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="C123">
-        <v>244</v>
+        <v>134</v>
       </c>
       <c r="D123">
-        <v>21.8</v>
+        <v>0.6</v>
       </c>
       <c r="E123">
-        <v>0.5</v>
+        <v>19</v>
       </c>
       <c r="F123">
-        <v>11.5</v>
+        <v>11</v>
       </c>
       <c r="G123" t="s">
         <v>15</v>
       </c>
       <c r="H123" t="s">
-        <v>44</v>
+        <v>71</v>
       </c>
     </row>
     <row r="124" spans="1:9" x14ac:dyDescent="0.25">
@@ -4711,25 +4734,25 @@
         <v>122</v>
       </c>
       <c r="B124" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="C124">
-        <v>93</v>
+        <v>244</v>
       </c>
       <c r="D124">
-        <v>1.2</v>
+        <v>21.8</v>
       </c>
       <c r="E124">
-        <v>15.7</v>
+        <v>0.5</v>
       </c>
       <c r="F124">
-        <v>3.3</v>
+        <v>11.5</v>
       </c>
       <c r="G124" t="s">
         <v>15</v>
       </c>
       <c r="H124" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
     </row>
     <row r="125" spans="1:9" x14ac:dyDescent="0.25">
@@ -4737,25 +4760,25 @@
         <v>123</v>
       </c>
       <c r="B125" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="C125">
-        <v>47</v>
+        <v>93</v>
       </c>
       <c r="D125">
-        <v>0.2</v>
+        <v>1.2</v>
       </c>
       <c r="E125">
-        <v>9.1999999999999993</v>
+        <v>15.7</v>
       </c>
       <c r="F125">
-        <v>0.8</v>
+        <v>3.3</v>
       </c>
       <c r="G125" t="s">
         <v>15</v>
       </c>
       <c r="H125" t="s">
-        <v>29</v>
+        <v>41</v>
       </c>
     </row>
     <row r="126" spans="1:9" x14ac:dyDescent="0.25">
@@ -4763,25 +4786,25 @@
         <v>124</v>
       </c>
       <c r="B126" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="C126">
-        <v>624</v>
+        <v>47</v>
       </c>
       <c r="D126">
-        <v>52.1</v>
+        <v>0.2</v>
       </c>
       <c r="E126">
-        <v>7.8</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="F126">
-        <v>25.6</v>
+        <v>0.8</v>
       </c>
       <c r="G126" t="s">
         <v>15</v>
       </c>
       <c r="H126" t="s">
-        <v>57</v>
+        <v>29</v>
       </c>
     </row>
     <row r="127" spans="1:9" x14ac:dyDescent="0.25">
@@ -4789,16 +4812,16 @@
         <v>125</v>
       </c>
       <c r="B127" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C127">
-        <v>649</v>
+        <v>624</v>
       </c>
       <c r="D127">
-        <v>55.2</v>
+        <v>52.1</v>
       </c>
       <c r="E127">
-        <v>7.2</v>
+        <v>7.8</v>
       </c>
       <c r="F127">
         <v>25.6</v>
@@ -4807,7 +4830,7 @@
         <v>15</v>
       </c>
       <c r="H127" t="s">
-        <v>129</v>
+        <v>57</v>
       </c>
     </row>
     <row r="128" spans="1:9" x14ac:dyDescent="0.25">
@@ -4815,25 +4838,25 @@
         <v>126</v>
       </c>
       <c r="B128" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="C128">
-        <v>68</v>
+        <v>649</v>
       </c>
       <c r="D128">
-        <v>0.6</v>
+        <v>55.2</v>
       </c>
       <c r="E128">
-        <v>14.3</v>
+        <v>7.2</v>
       </c>
       <c r="F128">
-        <v>0.6</v>
+        <v>25.6</v>
       </c>
       <c r="G128" t="s">
         <v>15</v>
       </c>
       <c r="H128" t="s">
-        <v>29</v>
+        <v>129</v>
       </c>
     </row>
     <row r="129" spans="1:9" x14ac:dyDescent="0.25">
@@ -4841,25 +4864,25 @@
         <v>127</v>
       </c>
       <c r="B129" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="C129">
-        <v>23</v>
+        <v>68</v>
       </c>
       <c r="D129">
-        <v>0.2</v>
+        <v>0.6</v>
       </c>
       <c r="E129">
-        <v>2.7</v>
+        <v>14.3</v>
       </c>
       <c r="F129">
-        <v>2.1</v>
+        <v>0.6</v>
       </c>
       <c r="G129" t="s">
         <v>15</v>
       </c>
       <c r="H129" t="s">
-        <v>41</v>
+        <v>29</v>
       </c>
     </row>
     <row r="130" spans="1:9" x14ac:dyDescent="0.25">
@@ -4867,25 +4890,25 @@
         <v>128</v>
       </c>
       <c r="B130" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="C130">
-        <v>357</v>
+        <v>23</v>
       </c>
       <c r="D130">
-        <v>39</v>
+        <v>0.2</v>
       </c>
       <c r="E130">
-        <v>1.1000000000000001</v>
+        <v>2.7</v>
       </c>
       <c r="F130">
-        <v>0.3</v>
+        <v>2.1</v>
       </c>
       <c r="G130" t="s">
         <v>15</v>
       </c>
       <c r="H130" t="s">
-        <v>333</v>
+        <v>41</v>
       </c>
     </row>
     <row r="131" spans="1:9" x14ac:dyDescent="0.25">
@@ -4893,25 +4916,25 @@
         <v>129</v>
       </c>
       <c r="B131" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="C131">
-        <v>356</v>
+        <v>357</v>
       </c>
       <c r="D131">
-        <v>17.100000000000001</v>
+        <v>39</v>
       </c>
       <c r="E131">
-        <v>42.6</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="F131">
-        <v>7.4</v>
+        <v>0.3</v>
       </c>
       <c r="G131" t="s">
         <v>15</v>
       </c>
       <c r="H131" t="s">
-        <v>88</v>
+        <v>332</v>
       </c>
     </row>
     <row r="132" spans="1:9" x14ac:dyDescent="0.25">
@@ -4919,25 +4942,25 @@
         <v>130</v>
       </c>
       <c r="B132" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="C132">
-        <v>474</v>
+        <v>356</v>
       </c>
       <c r="D132">
-        <v>17.600000000000001</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="E132">
-        <v>68.599999999999994</v>
+        <v>42.6</v>
       </c>
       <c r="F132">
-        <v>8</v>
+        <v>7.4</v>
       </c>
       <c r="G132" t="s">
         <v>15</v>
       </c>
       <c r="H132" t="s">
-        <v>214</v>
+        <v>88</v>
       </c>
     </row>
     <row r="133" spans="1:9" x14ac:dyDescent="0.25">
@@ -4945,28 +4968,25 @@
         <v>131</v>
       </c>
       <c r="B133" t="s">
-        <v>215</v>
+        <v>213</v>
       </c>
       <c r="C133">
-        <v>742</v>
+        <v>474</v>
       </c>
       <c r="D133">
-        <v>81.7</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="E133">
-        <v>0.5</v>
+        <v>68.599999999999994</v>
       </c>
       <c r="F133">
-        <v>1.1000000000000001</v>
+        <v>8</v>
       </c>
       <c r="G133" t="s">
         <v>15</v>
       </c>
       <c r="H133" t="s">
-        <v>216</v>
-      </c>
-      <c r="I133">
-        <v>0.9</v>
+        <v>214</v>
       </c>
     </row>
     <row r="134" spans="1:9" x14ac:dyDescent="0.25">
@@ -4974,25 +4994,28 @@
         <v>132</v>
       </c>
       <c r="B134" t="s">
-        <v>217</v>
+        <v>215</v>
       </c>
       <c r="C134">
-        <v>343</v>
+        <v>742</v>
       </c>
       <c r="D134">
-        <v>1.4</v>
+        <v>81.7</v>
       </c>
       <c r="E134">
-        <v>67.8</v>
+        <v>0.5</v>
       </c>
       <c r="F134">
-        <v>12.4</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G134" t="s">
         <v>15</v>
       </c>
       <c r="H134" t="s">
-        <v>81</v>
+        <v>216</v>
+      </c>
+      <c r="I134">
+        <v>0.9</v>
       </c>
     </row>
     <row r="135" spans="1:9" x14ac:dyDescent="0.25">
@@ -5000,28 +5023,25 @@
         <v>133</v>
       </c>
       <c r="B135" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="C135">
-        <v>59</v>
+        <v>343</v>
       </c>
       <c r="D135">
-        <v>2.9</v>
+        <v>1.4</v>
       </c>
       <c r="E135">
-        <v>4.8</v>
+        <v>67.8</v>
       </c>
       <c r="F135">
-        <v>3.2</v>
+        <v>12.4</v>
       </c>
       <c r="G135" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H135" t="s">
-        <v>163</v>
-      </c>
-      <c r="I135">
-        <v>1</v>
+        <v>81</v>
       </c>
     </row>
     <row r="136" spans="1:9" x14ac:dyDescent="0.25">
@@ -5029,25 +5049,28 @@
         <v>134</v>
       </c>
       <c r="B136" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="C136">
-        <v>537</v>
+        <v>59</v>
       </c>
       <c r="D136">
-        <v>31.1</v>
+        <v>2.9</v>
       </c>
       <c r="E136">
-        <v>56.9</v>
+        <v>4.8</v>
       </c>
       <c r="F136">
-        <v>6.5</v>
+        <v>3.2</v>
       </c>
       <c r="G136" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H136" t="s">
-        <v>74</v>
+        <v>163</v>
+      </c>
+      <c r="I136">
+        <v>1</v>
       </c>
     </row>
     <row r="137" spans="1:9" x14ac:dyDescent="0.25">
@@ -5055,19 +5078,19 @@
         <v>135</v>
       </c>
       <c r="B137" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="C137">
-        <v>570</v>
+        <v>537</v>
       </c>
       <c r="D137">
-        <v>38.200000000000003</v>
+        <v>31.1</v>
       </c>
       <c r="E137">
-        <v>46.1</v>
+        <v>56.9</v>
       </c>
       <c r="F137">
-        <v>8.8000000000000007</v>
+        <v>6.5</v>
       </c>
       <c r="G137" t="s">
         <v>15</v>
@@ -5081,28 +5104,25 @@
         <v>136</v>
       </c>
       <c r="B138" t="s">
-        <v>314</v>
+        <v>220</v>
       </c>
       <c r="C138">
-        <v>0</v>
+        <v>570</v>
       </c>
       <c r="D138">
-        <v>0</v>
+        <v>38.200000000000003</v>
       </c>
       <c r="E138">
-        <v>0</v>
+        <v>46.1</v>
       </c>
       <c r="F138">
-        <v>0</v>
+        <v>8.8000000000000007</v>
       </c>
       <c r="G138" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H138" t="s">
-        <v>313</v>
-      </c>
-      <c r="I138">
-        <v>1</v>
+        <v>74</v>
       </c>
     </row>
     <row r="139" spans="1:9" x14ac:dyDescent="0.25">
@@ -5110,7 +5130,7 @@
         <v>137</v>
       </c>
       <c r="B139" t="s">
-        <v>315</v>
+        <v>313</v>
       </c>
       <c r="C139">
         <v>0</v>
@@ -5128,7 +5148,7 @@
         <v>21</v>
       </c>
       <c r="H139" t="s">
-        <v>313</v>
+        <v>312</v>
       </c>
       <c r="I139">
         <v>1</v>
@@ -5139,25 +5159,28 @@
         <v>138</v>
       </c>
       <c r="B140" t="s">
-        <v>221</v>
+        <v>314</v>
       </c>
       <c r="C140">
-        <v>314</v>
+        <v>0</v>
       </c>
       <c r="D140">
-        <v>27.3</v>
+        <v>0</v>
       </c>
       <c r="E140">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="F140">
-        <v>16.100000000000001</v>
+        <v>0</v>
       </c>
       <c r="G140" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H140" t="s">
-        <v>44</v>
+        <v>312</v>
+      </c>
+      <c r="I140">
+        <v>1</v>
       </c>
     </row>
     <row r="141" spans="1:9" x14ac:dyDescent="0.25">
@@ -5165,25 +5188,25 @@
         <v>139</v>
       </c>
       <c r="B141" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="C141">
-        <v>256</v>
+        <v>314</v>
       </c>
       <c r="D141">
-        <v>19.5</v>
+        <v>27.3</v>
       </c>
       <c r="E141">
-        <v>0.7</v>
+        <v>0.8</v>
       </c>
       <c r="F141">
-        <v>19.5</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="G141" t="s">
         <v>15</v>
       </c>
       <c r="H141" t="s">
-        <v>334</v>
+        <v>44</v>
       </c>
     </row>
     <row r="142" spans="1:9" x14ac:dyDescent="0.25">
@@ -5191,25 +5214,25 @@
         <v>140</v>
       </c>
       <c r="B142" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="C142">
-        <v>365</v>
+        <v>256</v>
       </c>
       <c r="D142">
-        <v>5.6</v>
+        <v>19.5</v>
       </c>
       <c r="E142">
-        <v>62.2</v>
+        <v>0.7</v>
       </c>
       <c r="F142">
-        <v>11.4</v>
+        <v>19.5</v>
       </c>
       <c r="G142" t="s">
         <v>15</v>
       </c>
       <c r="H142" t="s">
-        <v>106</v>
+        <v>333</v>
       </c>
     </row>
     <row r="143" spans="1:9" x14ac:dyDescent="0.25">
@@ -5217,25 +5240,25 @@
         <v>141</v>
       </c>
       <c r="B143" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="C143">
-        <v>125</v>
+        <v>365</v>
       </c>
       <c r="D143">
-        <v>1.8</v>
+        <v>5.6</v>
       </c>
       <c r="E143">
-        <v>16.100000000000001</v>
+        <v>62.2</v>
       </c>
       <c r="F143">
-        <v>10.8</v>
+        <v>11.4</v>
       </c>
       <c r="G143" t="s">
         <v>15</v>
       </c>
       <c r="H143" t="s">
-        <v>50</v>
+        <v>106</v>
       </c>
     </row>
     <row r="144" spans="1:9" x14ac:dyDescent="0.25">
@@ -5243,25 +5266,25 @@
         <v>142</v>
       </c>
       <c r="B144" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="C144">
-        <v>55</v>
+        <v>125</v>
       </c>
       <c r="D144">
-        <v>0.3</v>
+        <v>1.8</v>
       </c>
       <c r="E144">
-        <v>11.3</v>
+        <v>16.100000000000001</v>
       </c>
       <c r="F144">
-        <v>1</v>
+        <v>10.8</v>
       </c>
       <c r="G144" t="s">
         <v>15</v>
       </c>
       <c r="H144" t="s">
-        <v>29</v>
+        <v>50</v>
       </c>
     </row>
     <row r="145" spans="1:9" x14ac:dyDescent="0.25">
@@ -5269,25 +5292,25 @@
         <v>143</v>
       </c>
       <c r="B145" t="s">
-        <v>321</v>
+        <v>225</v>
       </c>
       <c r="C145">
-        <v>127</v>
+        <v>55</v>
       </c>
       <c r="D145">
-        <v>5</v>
+        <v>0.3</v>
       </c>
       <c r="E145">
-        <v>18.100000000000001</v>
+        <v>11.3</v>
       </c>
       <c r="F145">
-        <v>1.8</v>
+        <v>1</v>
       </c>
       <c r="G145" t="s">
         <v>15</v>
       </c>
       <c r="H145" t="s">
-        <v>177</v>
+        <v>29</v>
       </c>
     </row>
     <row r="146" spans="1:9" x14ac:dyDescent="0.25">
@@ -5295,25 +5318,25 @@
         <v>144</v>
       </c>
       <c r="B146" t="s">
-        <v>226</v>
+        <v>320</v>
       </c>
       <c r="C146">
-        <v>176</v>
+        <v>127</v>
       </c>
       <c r="D146">
-        <v>17.2</v>
+        <v>5</v>
       </c>
       <c r="E146">
-        <v>0.8</v>
+        <v>18.100000000000001</v>
       </c>
       <c r="F146">
-        <v>1.4</v>
+        <v>1.8</v>
       </c>
       <c r="G146" t="s">
         <v>15</v>
       </c>
       <c r="H146" t="s">
-        <v>57</v>
+        <v>177</v>
       </c>
     </row>
     <row r="147" spans="1:9" x14ac:dyDescent="0.25">
@@ -5321,28 +5344,25 @@
         <v>145</v>
       </c>
       <c r="B147" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="C147">
-        <v>810</v>
+        <v>176</v>
       </c>
       <c r="D147">
-        <v>90</v>
+        <v>17.2</v>
       </c>
       <c r="E147">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="F147">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="G147" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H147" t="s">
-        <v>58</v>
-      </c>
-      <c r="I147">
-        <v>0.9</v>
+        <v>57</v>
       </c>
     </row>
     <row r="148" spans="1:9" x14ac:dyDescent="0.25">
@@ -5350,25 +5370,28 @@
         <v>146</v>
       </c>
       <c r="B148" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="C148">
-        <v>45</v>
+        <v>810</v>
       </c>
       <c r="D148">
-        <v>0.2</v>
+        <v>90</v>
       </c>
       <c r="E148">
-        <v>8</v>
+        <v>0</v>
       </c>
       <c r="F148">
-        <v>0.8</v>
+        <v>0</v>
       </c>
       <c r="G148" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H148" t="s">
-        <v>29</v>
+        <v>58</v>
+      </c>
+      <c r="I148">
+        <v>0.9</v>
       </c>
     </row>
     <row r="149" spans="1:9" x14ac:dyDescent="0.25">
@@ -5376,28 +5399,25 @@
         <v>147</v>
       </c>
       <c r="B149" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="C149">
-        <v>44</v>
+        <v>45</v>
       </c>
       <c r="D149">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E149">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="F149">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G149" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H149" t="s">
-        <v>328</v>
-      </c>
-      <c r="I149">
-        <v>1.04</v>
+        <v>29</v>
       </c>
     </row>
     <row r="150" spans="1:9" x14ac:dyDescent="0.25">
@@ -5405,25 +5425,28 @@
         <v>148</v>
       </c>
       <c r="B150" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="C150">
-        <v>358</v>
+        <v>44</v>
       </c>
       <c r="D150">
-        <v>13</v>
+        <v>0.1</v>
       </c>
       <c r="E150">
-        <v>34.9</v>
+        <v>10</v>
       </c>
       <c r="F150">
-        <v>14.8</v>
+        <v>0.6</v>
       </c>
       <c r="G150" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H150" t="s">
-        <v>48</v>
+        <v>327</v>
+      </c>
+      <c r="I150">
+        <v>1.04</v>
       </c>
     </row>
     <row r="151" spans="1:9" x14ac:dyDescent="0.25">
@@ -5431,25 +5454,25 @@
         <v>149</v>
       </c>
       <c r="B151" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="C151">
-        <v>698</v>
+        <v>358</v>
       </c>
       <c r="D151">
-        <v>66.5</v>
+        <v>13</v>
       </c>
       <c r="E151">
-        <v>4.2</v>
+        <v>34.9</v>
       </c>
       <c r="F151">
-        <v>17</v>
+        <v>14.8</v>
       </c>
       <c r="G151" t="s">
         <v>15</v>
       </c>
       <c r="H151" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
     </row>
     <row r="152" spans="1:9" x14ac:dyDescent="0.25">
@@ -5457,25 +5480,25 @@
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="C152">
-        <v>401</v>
+        <v>698</v>
       </c>
       <c r="D152">
-        <v>31</v>
+        <v>66.5</v>
       </c>
       <c r="E152">
-        <v>0.3</v>
+        <v>4.2</v>
       </c>
       <c r="F152">
-        <v>30.5</v>
+        <v>17</v>
       </c>
       <c r="G152" t="s">
         <v>15</v>
       </c>
       <c r="H152" t="s">
-        <v>37</v>
+        <v>57</v>
       </c>
     </row>
     <row r="153" spans="1:9" x14ac:dyDescent="0.25">
@@ -5483,25 +5506,25 @@
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="C153">
-        <v>430</v>
+        <v>401</v>
       </c>
       <c r="D153">
-        <v>42.5</v>
+        <v>31</v>
       </c>
       <c r="E153">
-        <v>6.6</v>
+        <v>0.3</v>
       </c>
       <c r="F153">
-        <v>3.9</v>
+        <v>30.5</v>
       </c>
       <c r="G153" t="s">
         <v>15</v>
       </c>
       <c r="H153" t="s">
-        <v>59</v>
+        <v>37</v>
       </c>
     </row>
     <row r="154" spans="1:9" x14ac:dyDescent="0.25">
@@ -5509,19 +5532,19 @@
         <v>152</v>
       </c>
       <c r="B154" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="C154">
-        <v>398</v>
+        <v>430</v>
       </c>
       <c r="D154">
-        <v>35.799999999999997</v>
+        <v>42.5</v>
       </c>
       <c r="E154">
-        <v>10.8</v>
+        <v>6.6</v>
       </c>
       <c r="F154">
-        <v>5.7</v>
+        <v>3.9</v>
       </c>
       <c r="G154" t="s">
         <v>15</v>
@@ -5535,25 +5558,25 @@
         <v>153</v>
       </c>
       <c r="B155" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="C155">
-        <v>58</v>
+        <v>398</v>
       </c>
       <c r="D155">
-        <v>0.5</v>
+        <v>35.799999999999997</v>
       </c>
       <c r="E155">
-        <v>7.4</v>
+        <v>10.8</v>
       </c>
       <c r="F155">
-        <v>3.9</v>
+        <v>5.7</v>
       </c>
       <c r="G155" t="s">
         <v>15</v>
       </c>
       <c r="H155" t="s">
-        <v>53</v>
+        <v>59</v>
       </c>
     </row>
     <row r="156" spans="1:9" x14ac:dyDescent="0.25">
@@ -5561,25 +5584,25 @@
         <v>154</v>
       </c>
       <c r="B156" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="C156">
-        <v>43</v>
+        <v>58</v>
       </c>
       <c r="D156">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E156">
-        <v>8.9</v>
+        <v>7.4</v>
       </c>
       <c r="F156">
-        <v>0.8</v>
+        <v>3.9</v>
       </c>
       <c r="G156" t="s">
         <v>15</v>
       </c>
       <c r="H156" t="s">
-        <v>29</v>
+        <v>53</v>
       </c>
     </row>
     <row r="157" spans="1:9" x14ac:dyDescent="0.25">
@@ -5587,19 +5610,19 @@
         <v>155</v>
       </c>
       <c r="B157" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="C157">
-        <v>48</v>
+        <v>43</v>
       </c>
       <c r="D157">
-        <v>0.2</v>
+        <v>0.1</v>
       </c>
       <c r="E157">
-        <v>10.199999999999999</v>
+        <v>8.9</v>
       </c>
       <c r="F157">
-        <v>0.6</v>
+        <v>0.8</v>
       </c>
       <c r="G157" t="s">
         <v>15</v>
@@ -5613,25 +5636,25 @@
         <v>156</v>
       </c>
       <c r="B158" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="C158">
+        <v>48</v>
+      </c>
+      <c r="D158">
+        <v>0.2</v>
+      </c>
+      <c r="E158">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="F158">
+        <v>0.6</v>
+      </c>
+      <c r="G158" t="s">
+        <v>15</v>
+      </c>
+      <c r="H158" t="s">
         <v>29</v>
-      </c>
-      <c r="D158">
-        <v>0.4</v>
-      </c>
-      <c r="E158">
-        <v>0.6</v>
-      </c>
-      <c r="F158">
-        <v>3.5</v>
-      </c>
-      <c r="G158" t="s">
-        <v>15</v>
-      </c>
-      <c r="H158" t="s">
-        <v>95</v>
       </c>
     </row>
     <row r="159" spans="1:9" x14ac:dyDescent="0.25">
@@ -5639,25 +5662,25 @@
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="C159">
-        <v>594</v>
+        <v>29</v>
       </c>
       <c r="D159">
-        <v>45.4</v>
+        <v>0.4</v>
       </c>
       <c r="E159">
-        <v>17.600000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="F159">
-        <v>23.8</v>
+        <v>3.5</v>
       </c>
       <c r="G159" t="s">
         <v>15</v>
       </c>
       <c r="H159" t="s">
-        <v>57</v>
+        <v>95</v>
       </c>
     </row>
     <row r="160" spans="1:9" x14ac:dyDescent="0.25">
@@ -5665,25 +5688,25 @@
         <v>158</v>
       </c>
       <c r="B160" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="C160">
-        <v>226</v>
+        <v>594</v>
       </c>
       <c r="D160">
-        <v>7.6</v>
+        <v>45.4</v>
       </c>
       <c r="E160">
-        <v>26.5</v>
+        <v>17.600000000000001</v>
       </c>
       <c r="F160">
-        <v>12</v>
+        <v>23.8</v>
       </c>
       <c r="G160" t="s">
         <v>15</v>
       </c>
       <c r="H160" t="s">
-        <v>91</v>
+        <v>57</v>
       </c>
     </row>
     <row r="161" spans="1:9" x14ac:dyDescent="0.25">
@@ -5691,19 +5714,19 @@
         <v>159</v>
       </c>
       <c r="B161" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="C161">
-        <v>195</v>
+        <v>226</v>
       </c>
       <c r="D161">
-        <v>6.3</v>
+        <v>7.6</v>
       </c>
       <c r="E161">
-        <v>24.2</v>
+        <v>26.5</v>
       </c>
       <c r="F161">
-        <v>9.5</v>
+        <v>12</v>
       </c>
       <c r="G161" t="s">
         <v>15</v>
@@ -5717,19 +5740,19 @@
         <v>160</v>
       </c>
       <c r="B162" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="C162">
-        <v>238</v>
+        <v>195</v>
       </c>
       <c r="D162">
-        <v>8.4</v>
+        <v>6.3</v>
       </c>
       <c r="E162">
-        <v>29.9</v>
+        <v>24.2</v>
       </c>
       <c r="F162">
-        <v>9.9</v>
+        <v>9.5</v>
       </c>
       <c r="G162" t="s">
         <v>15</v>
@@ -5743,19 +5766,19 @@
         <v>161</v>
       </c>
       <c r="B163" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="C163">
-        <v>204</v>
+        <v>238</v>
       </c>
       <c r="D163">
-        <v>6.9</v>
+        <v>8.4</v>
       </c>
       <c r="E163">
-        <v>23.9</v>
+        <v>29.9</v>
       </c>
       <c r="F163">
-        <v>10.7</v>
+        <v>9.9</v>
       </c>
       <c r="G163" t="s">
         <v>15</v>
@@ -5769,19 +5792,19 @@
         <v>162</v>
       </c>
       <c r="B164" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="C164">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="D164">
-        <v>6.4</v>
+        <v>6.9</v>
       </c>
       <c r="E164">
-        <v>28.7</v>
+        <v>23.9</v>
       </c>
       <c r="F164">
-        <v>10.6</v>
+        <v>10.7</v>
       </c>
       <c r="G164" t="s">
         <v>15</v>
@@ -5795,19 +5818,19 @@
         <v>163</v>
       </c>
       <c r="B165" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="C165">
-        <v>297</v>
+        <v>218</v>
       </c>
       <c r="D165">
+        <v>6.4</v>
+      </c>
+      <c r="E165">
+        <v>28.7</v>
+      </c>
+      <c r="F165">
         <v>10.6</v>
-      </c>
-      <c r="E165">
-        <v>37.200000000000003</v>
-      </c>
-      <c r="F165">
-        <v>12.3</v>
       </c>
       <c r="G165" t="s">
         <v>15</v>
@@ -5821,25 +5844,25 @@
         <v>164</v>
       </c>
       <c r="B166" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="C166">
-        <v>232</v>
+        <v>297</v>
       </c>
       <c r="D166">
-        <v>9.1</v>
+        <v>10.6</v>
       </c>
       <c r="E166">
-        <v>33</v>
+        <v>37.200000000000003</v>
       </c>
       <c r="F166">
-        <v>3.3</v>
+        <v>12.3</v>
       </c>
       <c r="G166" t="s">
         <v>15</v>
       </c>
       <c r="H166" t="s">
-        <v>177</v>
+        <v>91</v>
       </c>
     </row>
     <row r="167" spans="1:9" x14ac:dyDescent="0.25">
@@ -5847,19 +5870,19 @@
         <v>165</v>
       </c>
       <c r="B167" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="C167">
-        <v>286</v>
+        <v>232</v>
       </c>
       <c r="D167">
-        <v>15.4</v>
+        <v>9.1</v>
       </c>
       <c r="E167">
-        <v>32.4</v>
+        <v>33</v>
       </c>
       <c r="F167">
-        <v>3.2</v>
+        <v>3.3</v>
       </c>
       <c r="G167" t="s">
         <v>15</v>
@@ -5873,25 +5896,25 @@
         <v>166</v>
       </c>
       <c r="B168" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="C168">
-        <v>367</v>
+        <v>286</v>
       </c>
       <c r="D168">
-        <v>4.2</v>
+        <v>15.4</v>
       </c>
       <c r="E168">
-        <v>62.9</v>
+        <v>32.4</v>
       </c>
       <c r="F168">
-        <v>12</v>
+        <v>3.2</v>
       </c>
       <c r="G168" t="s">
         <v>15</v>
       </c>
       <c r="H168" t="s">
-        <v>127</v>
+        <v>177</v>
       </c>
     </row>
     <row r="169" spans="1:9" x14ac:dyDescent="0.25">
@@ -5899,25 +5922,25 @@
         <v>167</v>
       </c>
       <c r="B169" t="s">
-        <v>322</v>
+        <v>248</v>
       </c>
       <c r="C169">
-        <v>107</v>
+        <v>367</v>
       </c>
       <c r="D169">
-        <v>1</v>
+        <v>4.2</v>
       </c>
       <c r="E169">
-        <v>0</v>
+        <v>62.9</v>
       </c>
       <c r="F169">
-        <v>24.6</v>
+        <v>12</v>
       </c>
       <c r="G169" t="s">
         <v>15</v>
       </c>
       <c r="H169" t="s">
-        <v>152</v>
+        <v>127</v>
       </c>
     </row>
     <row r="170" spans="1:9" x14ac:dyDescent="0.25">
@@ -5925,19 +5948,19 @@
         <v>168</v>
       </c>
       <c r="B170" t="s">
-        <v>323</v>
+        <v>321</v>
       </c>
       <c r="C170">
-        <v>128</v>
+        <v>107</v>
       </c>
       <c r="D170">
-        <v>0.8</v>
+        <v>1</v>
       </c>
       <c r="E170">
         <v>0</v>
       </c>
       <c r="F170">
-        <v>30.1</v>
+        <v>24.6</v>
       </c>
       <c r="G170" t="s">
         <v>15</v>
@@ -5951,19 +5974,19 @@
         <v>169</v>
       </c>
       <c r="B171" t="s">
-        <v>324</v>
+        <v>322</v>
       </c>
       <c r="C171">
-        <v>163</v>
+        <v>128</v>
       </c>
       <c r="D171">
-        <v>10.199999999999999</v>
+        <v>0.8</v>
       </c>
       <c r="E171">
         <v>0</v>
       </c>
       <c r="F171">
-        <v>17.899999999999999</v>
+        <v>30.1</v>
       </c>
       <c r="G171" t="s">
         <v>15</v>
@@ -5977,25 +6000,25 @@
         <v>170</v>
       </c>
       <c r="B172" t="s">
-        <v>249</v>
+        <v>323</v>
       </c>
       <c r="C172">
-        <v>102</v>
+        <v>163</v>
       </c>
       <c r="D172">
-        <v>2.1</v>
+        <v>10.199999999999999</v>
       </c>
       <c r="E172">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="F172">
-        <v>2.8</v>
+        <v>17.899999999999999</v>
       </c>
       <c r="G172" t="s">
         <v>15</v>
       </c>
       <c r="H172" t="s">
-        <v>202</v>
+        <v>152</v>
       </c>
     </row>
     <row r="173" spans="1:9" x14ac:dyDescent="0.25">
@@ -6003,25 +6026,25 @@
         <v>171</v>
       </c>
       <c r="B173" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="C173">
-        <v>61</v>
+        <v>102</v>
       </c>
       <c r="D173">
-        <v>0.2</v>
+        <v>2.1</v>
       </c>
       <c r="E173">
-        <v>4.2</v>
+        <v>18</v>
       </c>
       <c r="F173">
-        <v>10.6</v>
+        <v>2.8</v>
       </c>
       <c r="G173" t="s">
         <v>15</v>
       </c>
       <c r="H173" t="s">
-        <v>66</v>
+        <v>202</v>
       </c>
     </row>
     <row r="174" spans="1:9" x14ac:dyDescent="0.25">
@@ -6029,25 +6052,25 @@
         <v>172</v>
       </c>
       <c r="B174" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="C174">
-        <v>17</v>
+        <v>61</v>
       </c>
       <c r="D174">
-        <v>0.1</v>
+        <v>0.2</v>
       </c>
       <c r="E174">
-        <v>2.1</v>
+        <v>4.2</v>
       </c>
       <c r="F174">
-        <v>1.1000000000000001</v>
+        <v>10.6</v>
       </c>
       <c r="G174" t="s">
         <v>15</v>
       </c>
       <c r="H174" t="s">
-        <v>41</v>
+        <v>66</v>
       </c>
     </row>
     <row r="175" spans="1:9" x14ac:dyDescent="0.25">
@@ -6055,28 +6078,25 @@
         <v>173</v>
       </c>
       <c r="B175" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="C175">
-        <v>810</v>
+        <v>17</v>
       </c>
       <c r="D175">
-        <v>90</v>
+        <v>0.1</v>
       </c>
       <c r="E175">
-        <v>0</v>
+        <v>2.1</v>
       </c>
       <c r="F175">
-        <v>0</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="G175" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H175" t="s">
-        <v>58</v>
-      </c>
-      <c r="I175">
-        <v>0.9</v>
+        <v>41</v>
       </c>
     </row>
     <row r="176" spans="1:9" x14ac:dyDescent="0.25">
@@ -6084,25 +6104,28 @@
         <v>174</v>
       </c>
       <c r="B176" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="C176">
-        <v>45</v>
+        <v>810</v>
       </c>
       <c r="D176">
-        <v>2.2000000000000002</v>
+        <v>90</v>
       </c>
       <c r="E176">
-        <v>4</v>
+        <v>0</v>
       </c>
       <c r="F176">
-        <v>1.4</v>
+        <v>0</v>
       </c>
       <c r="G176" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H176" t="s">
-        <v>39</v>
+        <v>58</v>
+      </c>
+      <c r="I176">
+        <v>0.9</v>
       </c>
     </row>
     <row r="177" spans="1:9" x14ac:dyDescent="0.25">
@@ -6110,25 +6133,25 @@
         <v>175</v>
       </c>
       <c r="B177" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="C177">
-        <v>406</v>
+        <v>45</v>
       </c>
       <c r="D177">
-        <v>32.1</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="E177">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="F177">
-        <v>29.3</v>
+        <v>1.4</v>
       </c>
       <c r="G177" t="s">
         <v>15</v>
       </c>
       <c r="H177" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
     </row>
     <row r="178" spans="1:9" x14ac:dyDescent="0.25">
@@ -6136,25 +6159,25 @@
         <v>176</v>
       </c>
       <c r="B178" t="s">
-        <v>256</v>
+        <v>254</v>
       </c>
       <c r="C178">
-        <v>126</v>
+        <v>406</v>
       </c>
       <c r="D178">
-        <v>1</v>
+        <v>32.1</v>
       </c>
       <c r="E178">
-        <v>25.7</v>
+        <v>0</v>
       </c>
       <c r="F178">
-        <v>2.7</v>
+        <v>29.3</v>
       </c>
       <c r="G178" t="s">
         <v>15</v>
       </c>
       <c r="H178" t="s">
-        <v>255</v>
+        <v>37</v>
       </c>
     </row>
     <row r="179" spans="1:9" x14ac:dyDescent="0.25">
@@ -6162,25 +6185,25 @@
         <v>177</v>
       </c>
       <c r="B179" t="s">
-        <v>338</v>
+        <v>256</v>
       </c>
       <c r="C179">
-        <v>162</v>
+        <v>126</v>
       </c>
       <c r="D179">
-        <v>4.5999999999999996</v>
+        <v>1</v>
       </c>
       <c r="E179">
-        <v>0</v>
+        <v>25.7</v>
       </c>
       <c r="F179">
-        <v>30.2</v>
+        <v>2.7</v>
       </c>
       <c r="G179" t="s">
         <v>15</v>
       </c>
       <c r="H179" t="s">
-        <v>161</v>
+        <v>255</v>
       </c>
     </row>
     <row r="180" spans="1:9" x14ac:dyDescent="0.25">
@@ -6188,19 +6211,19 @@
         <v>178</v>
       </c>
       <c r="B180" t="s">
-        <v>257</v>
+        <v>337</v>
       </c>
       <c r="C180">
-        <v>133</v>
+        <v>162</v>
       </c>
       <c r="D180">
-        <v>4.5</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E180">
         <v>0</v>
       </c>
       <c r="F180">
-        <v>23.2</v>
+        <v>30.2</v>
       </c>
       <c r="G180" t="s">
         <v>15</v>
@@ -6214,19 +6237,19 @@
         <v>179</v>
       </c>
       <c r="B181" t="s">
-        <v>339</v>
+        <v>257</v>
       </c>
       <c r="C181">
-        <v>128</v>
+        <v>133</v>
       </c>
       <c r="D181">
-        <v>2</v>
+        <v>4.5</v>
       </c>
       <c r="E181">
         <v>0</v>
       </c>
       <c r="F181">
-        <v>27.7</v>
+        <v>23.2</v>
       </c>
       <c r="G181" t="s">
         <v>15</v>
@@ -6240,10 +6263,10 @@
         <v>180</v>
       </c>
       <c r="B182" t="s">
-        <v>258</v>
+        <v>338</v>
       </c>
       <c r="C182">
-        <v>105</v>
+        <v>128</v>
       </c>
       <c r="D182">
         <v>2</v>
@@ -6252,7 +6275,7 @@
         <v>0</v>
       </c>
       <c r="F182">
-        <v>21.9</v>
+        <v>27.7</v>
       </c>
       <c r="G182" t="s">
         <v>15</v>
@@ -6266,19 +6289,19 @@
         <v>181</v>
       </c>
       <c r="B183" t="s">
-        <v>325</v>
+        <v>258</v>
       </c>
       <c r="C183">
-        <v>211</v>
+        <v>105</v>
       </c>
       <c r="D183">
-        <v>8.9</v>
+        <v>2</v>
       </c>
       <c r="E183">
         <v>0</v>
       </c>
       <c r="F183">
-        <v>32.6</v>
+        <v>21.9</v>
       </c>
       <c r="G183" t="s">
         <v>15</v>
@@ -6292,19 +6315,19 @@
         <v>182</v>
       </c>
       <c r="B184" t="s">
-        <v>326</v>
+        <v>324</v>
       </c>
       <c r="C184">
-        <v>154</v>
+        <v>211</v>
       </c>
       <c r="D184">
-        <v>7.5</v>
+        <v>8.9</v>
       </c>
       <c r="E184">
         <v>0</v>
       </c>
       <c r="F184">
-        <v>21.6</v>
+        <v>32.6</v>
       </c>
       <c r="G184" t="s">
         <v>15</v>
@@ -6318,25 +6341,25 @@
         <v>183</v>
       </c>
       <c r="B185" t="s">
-        <v>259</v>
+        <v>325</v>
       </c>
       <c r="C185">
-        <v>321</v>
+        <v>154</v>
       </c>
       <c r="D185">
-        <v>0.9</v>
+        <v>7.5</v>
       </c>
       <c r="E185">
-        <v>73.2</v>
+        <v>0</v>
       </c>
       <c r="F185">
-        <v>3</v>
+        <v>21.6</v>
       </c>
       <c r="G185" t="s">
         <v>15</v>
       </c>
       <c r="H185" t="s">
-        <v>32</v>
+        <v>161</v>
       </c>
     </row>
     <row r="186" spans="1:9" x14ac:dyDescent="0.25">
@@ -6344,25 +6367,25 @@
         <v>184</v>
       </c>
       <c r="B186" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="C186">
-        <v>150</v>
+        <v>321</v>
       </c>
       <c r="D186">
-        <v>5.7</v>
+        <v>0.9</v>
       </c>
       <c r="E186">
-        <v>20.7</v>
+        <v>73.2</v>
       </c>
       <c r="F186">
-        <v>2.6</v>
+        <v>3</v>
       </c>
       <c r="G186" t="s">
         <v>15</v>
       </c>
       <c r="H186" t="s">
-        <v>177</v>
+        <v>32</v>
       </c>
     </row>
     <row r="187" spans="1:9" x14ac:dyDescent="0.25">
@@ -6370,16 +6393,16 @@
         <v>185</v>
       </c>
       <c r="B187" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="C187">
-        <v>28</v>
+        <v>150</v>
       </c>
       <c r="D187">
-        <v>0.7</v>
+        <v>5.7</v>
       </c>
       <c r="E187">
-        <v>2.1</v>
+        <v>20.7</v>
       </c>
       <c r="F187">
         <v>2.6</v>
@@ -6388,7 +6411,7 @@
         <v>15</v>
       </c>
       <c r="H187" t="s">
-        <v>41</v>
+        <v>177</v>
       </c>
     </row>
     <row r="188" spans="1:9" x14ac:dyDescent="0.25">
@@ -6396,25 +6419,25 @@
         <v>186</v>
       </c>
       <c r="B188" t="s">
-        <v>262</v>
+        <v>341</v>
       </c>
       <c r="C188">
-        <v>147</v>
+        <v>28</v>
       </c>
       <c r="D188">
-        <v>10.8</v>
+        <v>0.2</v>
       </c>
       <c r="E188">
+        <v>4.9000000000000004</v>
+      </c>
+      <c r="F188">
         <v>1.3</v>
       </c>
-      <c r="F188">
-        <v>11.2</v>
-      </c>
       <c r="G188" t="s">
         <v>15</v>
       </c>
       <c r="H188" t="s">
-        <v>24</v>
+        <v>41</v>
       </c>
     </row>
     <row r="189" spans="1:9" x14ac:dyDescent="0.25">
@@ -6422,25 +6445,25 @@
         <v>187</v>
       </c>
       <c r="B189" t="s">
-        <v>263</v>
+        <v>261</v>
       </c>
       <c r="C189">
-        <v>422</v>
+        <v>28</v>
       </c>
       <c r="D189">
-        <v>37.1</v>
+        <v>0.7</v>
       </c>
       <c r="E189">
-        <v>3</v>
+        <v>2.1</v>
       </c>
       <c r="F189">
-        <v>22</v>
+        <v>2.6</v>
       </c>
       <c r="G189" t="s">
         <v>15</v>
       </c>
       <c r="H189" t="s">
-        <v>56</v>
+        <v>41</v>
       </c>
     </row>
     <row r="190" spans="1:9" x14ac:dyDescent="0.25">
@@ -6448,28 +6471,25 @@
         <v>188</v>
       </c>
       <c r="B190" t="s">
-        <v>264</v>
+        <v>262</v>
       </c>
       <c r="C190">
-        <v>464</v>
+        <v>147</v>
       </c>
       <c r="D190">
-        <v>50.7</v>
+        <v>10.8</v>
       </c>
       <c r="E190">
-        <v>1.4</v>
+        <v>1.3</v>
       </c>
       <c r="F190">
-        <v>0.4</v>
+        <v>11.2</v>
       </c>
       <c r="G190" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H190" t="s">
-        <v>131</v>
-      </c>
-      <c r="I190">
-        <v>1.1000000000000001</v>
+        <v>24</v>
       </c>
     </row>
     <row r="191" spans="1:9" x14ac:dyDescent="0.25">
@@ -6477,28 +6497,25 @@
         <v>189</v>
       </c>
       <c r="B191" t="s">
-        <v>265</v>
+        <v>263</v>
       </c>
       <c r="C191">
-        <v>309</v>
+        <v>422</v>
       </c>
       <c r="D191">
-        <v>32.1</v>
+        <v>37.1</v>
       </c>
       <c r="E191">
-        <v>4.9000000000000004</v>
+        <v>3</v>
       </c>
       <c r="F191">
-        <v>0.1</v>
+        <v>22</v>
       </c>
       <c r="G191" t="s">
         <v>15</v>
       </c>
       <c r="H191" t="s">
-        <v>131</v>
-      </c>
-      <c r="I191">
-        <v>1.1000000000000001</v>
+        <v>56</v>
       </c>
     </row>
     <row r="192" spans="1:9" x14ac:dyDescent="0.25">
@@ -6506,25 +6523,28 @@
         <v>190</v>
       </c>
       <c r="B192" t="s">
-        <v>266</v>
+        <v>264</v>
       </c>
       <c r="C192">
-        <v>0</v>
+        <v>464</v>
       </c>
       <c r="D192">
-        <v>0</v>
+        <v>50.7</v>
       </c>
       <c r="E192">
-        <v>0</v>
+        <v>1.4</v>
       </c>
       <c r="F192">
-        <v>0</v>
+        <v>0.4</v>
       </c>
       <c r="G192" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H192" t="s">
-        <v>48</v>
+        <v>131</v>
+      </c>
+      <c r="I192">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="193" spans="1:9" x14ac:dyDescent="0.25">
@@ -6532,25 +6552,28 @@
         <v>191</v>
       </c>
       <c r="B193" t="s">
-        <v>267</v>
+        <v>265</v>
       </c>
       <c r="C193">
-        <v>163</v>
+        <v>309</v>
       </c>
       <c r="D193">
-        <v>6.2</v>
+        <v>32.1</v>
       </c>
       <c r="E193">
-        <v>20.100000000000001</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="F193">
-        <v>6</v>
+        <v>0.1</v>
       </c>
       <c r="G193" t="s">
         <v>15</v>
       </c>
       <c r="H193" t="s">
-        <v>114</v>
+        <v>131</v>
+      </c>
+      <c r="I193">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="194" spans="1:9" x14ac:dyDescent="0.25">
@@ -6558,25 +6581,25 @@
         <v>192</v>
       </c>
       <c r="B194" t="s">
-        <v>268</v>
+        <v>266</v>
       </c>
       <c r="C194">
-        <v>131</v>
+        <v>0</v>
       </c>
       <c r="D194">
-        <v>3.7</v>
+        <v>0</v>
       </c>
       <c r="E194">
-        <v>17.3</v>
+        <v>0</v>
       </c>
       <c r="F194">
-        <v>6.3</v>
+        <v>0</v>
       </c>
       <c r="G194" t="s">
         <v>15</v>
       </c>
       <c r="H194" t="s">
-        <v>114</v>
+        <v>48</v>
       </c>
     </row>
     <row r="195" spans="1:9" x14ac:dyDescent="0.25">
@@ -6584,25 +6607,25 @@
         <v>193</v>
       </c>
       <c r="B195" t="s">
-        <v>269</v>
+        <v>267</v>
       </c>
       <c r="C195">
-        <v>19</v>
+        <v>163</v>
       </c>
       <c r="D195">
-        <v>0.3</v>
+        <v>6.2</v>
       </c>
       <c r="E195">
-        <v>1.7</v>
+        <v>20.100000000000001</v>
       </c>
       <c r="F195">
-        <v>1.3</v>
+        <v>6</v>
       </c>
       <c r="G195" t="s">
         <v>15</v>
       </c>
       <c r="H195" t="s">
-        <v>39</v>
+        <v>114</v>
       </c>
     </row>
     <row r="196" spans="1:9" x14ac:dyDescent="0.25">
@@ -6610,28 +6633,25 @@
         <v>194</v>
       </c>
       <c r="B196" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="C196">
-        <v>336</v>
+        <v>131</v>
       </c>
       <c r="D196">
-        <v>35</v>
+        <v>3.7</v>
       </c>
       <c r="E196">
-        <v>2.8</v>
+        <v>17.3</v>
       </c>
       <c r="F196">
-        <v>2.4</v>
+        <v>6.3</v>
       </c>
       <c r="G196" t="s">
         <v>15</v>
       </c>
       <c r="H196" t="s">
-        <v>335</v>
-      </c>
-      <c r="I196">
-        <v>1</v>
+        <v>114</v>
       </c>
     </row>
     <row r="197" spans="1:9" x14ac:dyDescent="0.25">
@@ -6639,25 +6659,25 @@
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="C197">
-        <v>30</v>
+        <v>19</v>
       </c>
       <c r="D197">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="E197">
-        <v>1.9</v>
+        <v>1.7</v>
       </c>
       <c r="F197">
-        <v>3</v>
+        <v>1.3</v>
       </c>
       <c r="G197" t="s">
         <v>15</v>
       </c>
       <c r="H197" t="s">
-        <v>53</v>
+        <v>39</v>
       </c>
     </row>
     <row r="198" spans="1:9" x14ac:dyDescent="0.25">
@@ -6665,25 +6685,28 @@
         <v>196</v>
       </c>
       <c r="B198" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="C198">
-        <v>262</v>
+        <v>336</v>
       </c>
       <c r="D198">
-        <v>11.2</v>
+        <v>35</v>
       </c>
       <c r="E198">
-        <v>25.1</v>
+        <v>2.8</v>
       </c>
       <c r="F198">
-        <v>14.6</v>
+        <v>2.4</v>
       </c>
       <c r="G198" t="s">
         <v>15</v>
       </c>
       <c r="H198" t="s">
-        <v>114</v>
+        <v>334</v>
+      </c>
+      <c r="I198">
+        <v>1</v>
       </c>
     </row>
     <row r="199" spans="1:9" x14ac:dyDescent="0.25">
@@ -6691,25 +6714,25 @@
         <v>197</v>
       </c>
       <c r="B199" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="C199">
-        <v>537</v>
+        <v>30</v>
       </c>
       <c r="D199">
-        <v>31.8</v>
+        <v>0.6</v>
       </c>
       <c r="E199">
-        <v>53.4</v>
+        <v>1.9</v>
       </c>
       <c r="F199">
-        <v>5.7</v>
+        <v>3</v>
       </c>
       <c r="G199" t="s">
         <v>15</v>
       </c>
       <c r="H199" t="s">
-        <v>74</v>
+        <v>53</v>
       </c>
     </row>
     <row r="200" spans="1:9" x14ac:dyDescent="0.25">
@@ -6717,25 +6740,25 @@
         <v>198</v>
       </c>
       <c r="B200" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="C200">
-        <v>567</v>
+        <v>262</v>
       </c>
       <c r="D200">
-        <v>35.200000000000003</v>
+        <v>11.2</v>
       </c>
       <c r="E200">
-        <v>55.8</v>
+        <v>25.1</v>
       </c>
       <c r="F200">
-        <v>6.7</v>
+        <v>14.6</v>
       </c>
       <c r="G200" t="s">
         <v>15</v>
       </c>
       <c r="H200" t="s">
-        <v>74</v>
+        <v>114</v>
       </c>
     </row>
     <row r="201" spans="1:9" x14ac:dyDescent="0.25">
@@ -6743,25 +6766,25 @@
         <v>199</v>
       </c>
       <c r="B201" t="s">
-        <v>275</v>
+        <v>273</v>
       </c>
       <c r="C201">
-        <v>153</v>
+        <v>537</v>
       </c>
       <c r="D201">
-        <v>4</v>
+        <v>31.8</v>
       </c>
       <c r="E201">
-        <v>0</v>
+        <v>53.4</v>
       </c>
       <c r="F201">
-        <v>29.3</v>
+        <v>5.7</v>
       </c>
       <c r="G201" t="s">
         <v>15</v>
       </c>
       <c r="H201" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
     </row>
     <row r="202" spans="1:9" x14ac:dyDescent="0.25">
@@ -6769,25 +6792,25 @@
         <v>200</v>
       </c>
       <c r="B202" t="s">
-        <v>276</v>
+        <v>274</v>
       </c>
       <c r="C202">
-        <v>121</v>
+        <v>567</v>
       </c>
       <c r="D202">
-        <v>3.6</v>
+        <v>35.200000000000003</v>
       </c>
       <c r="E202">
-        <v>0</v>
+        <v>55.8</v>
       </c>
       <c r="F202">
-        <v>22.2</v>
+        <v>6.7</v>
       </c>
       <c r="G202" t="s">
         <v>15</v>
       </c>
       <c r="H202" t="s">
-        <v>104</v>
+        <v>74</v>
       </c>
     </row>
     <row r="203" spans="1:9" x14ac:dyDescent="0.25">
@@ -6795,19 +6818,19 @@
         <v>201</v>
       </c>
       <c r="B203" t="s">
-        <v>277</v>
+        <v>275</v>
       </c>
       <c r="C203">
-        <v>159</v>
+        <v>153</v>
       </c>
       <c r="D203">
-        <v>8.5</v>
+        <v>4</v>
       </c>
       <c r="E203">
         <v>0</v>
       </c>
       <c r="F203">
-        <v>20.5</v>
+        <v>29.3</v>
       </c>
       <c r="G203" t="s">
         <v>15</v>
@@ -6821,25 +6844,25 @@
         <v>202</v>
       </c>
       <c r="B204" t="s">
-        <v>278</v>
+        <v>276</v>
       </c>
       <c r="C204">
-        <v>236</v>
+        <v>121</v>
       </c>
       <c r="D204">
-        <v>18.8</v>
+        <v>3.6</v>
       </c>
       <c r="E204">
-        <v>0.5</v>
+        <v>0</v>
       </c>
       <c r="F204">
-        <v>16.2</v>
+        <v>22.2</v>
       </c>
       <c r="G204" t="s">
         <v>15</v>
       </c>
       <c r="H204" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
     </row>
     <row r="205" spans="1:9" x14ac:dyDescent="0.25">
@@ -6847,25 +6870,25 @@
         <v>203</v>
       </c>
       <c r="B205" t="s">
-        <v>279</v>
+        <v>277</v>
       </c>
       <c r="C205">
-        <v>283</v>
+        <v>159</v>
       </c>
       <c r="D205">
-        <v>22.3</v>
+        <v>8.5</v>
       </c>
       <c r="E205">
-        <v>0.6</v>
+        <v>0</v>
       </c>
       <c r="F205">
-        <v>19.8</v>
+        <v>20.5</v>
       </c>
       <c r="G205" t="s">
         <v>15</v>
       </c>
       <c r="H205" t="s">
-        <v>56</v>
+        <v>104</v>
       </c>
     </row>
     <row r="206" spans="1:9" x14ac:dyDescent="0.25">
@@ -6873,25 +6896,25 @@
         <v>204</v>
       </c>
       <c r="B206" t="s">
-        <v>280</v>
+        <v>278</v>
       </c>
       <c r="C206">
-        <v>80</v>
+        <v>236</v>
       </c>
       <c r="D206">
-        <v>0.3</v>
+        <v>18.8</v>
       </c>
       <c r="E206">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="F206">
-        <v>19.3</v>
+        <v>16.2</v>
       </c>
       <c r="G206" t="s">
         <v>15</v>
       </c>
       <c r="H206" t="s">
-        <v>115</v>
+        <v>56</v>
       </c>
     </row>
     <row r="207" spans="1:9" x14ac:dyDescent="0.25">
@@ -6899,25 +6922,25 @@
         <v>205</v>
       </c>
       <c r="B207" t="s">
-        <v>281</v>
+        <v>279</v>
       </c>
       <c r="C207">
-        <v>85</v>
+        <v>283</v>
       </c>
       <c r="D207">
-        <v>1.1000000000000001</v>
+        <v>22.3</v>
       </c>
       <c r="E207">
-        <v>0</v>
+        <v>0.6</v>
       </c>
       <c r="F207">
-        <v>18.7</v>
+        <v>19.8</v>
       </c>
       <c r="G207" t="s">
         <v>15</v>
       </c>
       <c r="H207" t="s">
-        <v>115</v>
+        <v>56</v>
       </c>
     </row>
     <row r="208" spans="1:9" x14ac:dyDescent="0.25">
@@ -6925,25 +6948,25 @@
         <v>206</v>
       </c>
       <c r="B208" t="s">
-        <v>283</v>
+        <v>280</v>
       </c>
       <c r="C208">
-        <v>124</v>
+        <v>80</v>
       </c>
       <c r="D208">
-        <v>7.7</v>
+        <v>0.3</v>
       </c>
       <c r="E208">
-        <v>3.8</v>
+        <v>0</v>
       </c>
       <c r="F208">
-        <v>7.1</v>
+        <v>19.3</v>
       </c>
       <c r="G208" t="s">
         <v>15</v>
       </c>
       <c r="H208" t="s">
-        <v>59</v>
+        <v>115</v>
       </c>
     </row>
     <row r="209" spans="1:9" x14ac:dyDescent="0.25">
@@ -6951,25 +6974,25 @@
         <v>207</v>
       </c>
       <c r="B209" t="s">
-        <v>284</v>
+        <v>281</v>
       </c>
       <c r="C209">
-        <v>621</v>
+        <v>85</v>
       </c>
       <c r="D209">
-        <v>54.5</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E209">
-        <v>3.6</v>
+        <v>0</v>
       </c>
       <c r="F209">
-        <v>25.1</v>
+        <v>18.7</v>
       </c>
       <c r="G209" t="s">
         <v>15</v>
       </c>
       <c r="H209" t="s">
-        <v>57</v>
+        <v>115</v>
       </c>
     </row>
     <row r="210" spans="1:9" x14ac:dyDescent="0.25">
@@ -6977,28 +7000,25 @@
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>285</v>
+        <v>283</v>
       </c>
       <c r="C210">
-        <v>810</v>
+        <v>124</v>
       </c>
       <c r="D210">
-        <v>90</v>
+        <v>7.7</v>
       </c>
       <c r="E210">
-        <v>0</v>
+        <v>3.8</v>
       </c>
       <c r="F210">
-        <v>0</v>
+        <v>7.1</v>
       </c>
       <c r="G210" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H210" t="s">
-        <v>58</v>
-      </c>
-      <c r="I210">
-        <v>0.9</v>
+        <v>59</v>
       </c>
     </row>
     <row r="211" spans="1:9" x14ac:dyDescent="0.25">
@@ -7006,25 +7026,25 @@
         <v>209</v>
       </c>
       <c r="B211" t="s">
-        <v>286</v>
+        <v>284</v>
       </c>
       <c r="C211">
-        <v>26</v>
+        <v>621</v>
       </c>
       <c r="D211">
-        <v>0.2</v>
+        <v>54.5</v>
       </c>
       <c r="E211">
-        <v>3.1</v>
+        <v>3.6</v>
       </c>
       <c r="F211">
-        <v>2.1</v>
+        <v>25.1</v>
       </c>
       <c r="G211" t="s">
         <v>15</v>
       </c>
       <c r="H211" t="s">
-        <v>39</v>
+        <v>57</v>
       </c>
     </row>
     <row r="212" spans="1:9" x14ac:dyDescent="0.25">
@@ -7032,25 +7052,28 @@
         <v>210</v>
       </c>
       <c r="B212" t="s">
-        <v>287</v>
+        <v>285</v>
       </c>
       <c r="C212">
-        <v>27</v>
+        <v>810</v>
       </c>
       <c r="D212">
-        <v>0.2</v>
+        <v>90</v>
       </c>
       <c r="E212">
-        <v>3.3</v>
+        <v>0</v>
       </c>
       <c r="F212">
-        <v>2.2000000000000002</v>
+        <v>0</v>
       </c>
       <c r="G212" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H212" t="s">
-        <v>41</v>
+        <v>58</v>
+      </c>
+      <c r="I212">
+        <v>0.9</v>
       </c>
     </row>
     <row r="213" spans="1:9" x14ac:dyDescent="0.25">
@@ -7058,25 +7081,25 @@
         <v>211</v>
       </c>
       <c r="B213" t="s">
-        <v>288</v>
+        <v>286</v>
       </c>
       <c r="C213">
-        <v>46</v>
+        <v>26</v>
       </c>
       <c r="D213">
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="E213">
-        <v>0.6</v>
+        <v>3.1</v>
       </c>
       <c r="F213">
-        <v>6.1</v>
+        <v>2.1</v>
       </c>
       <c r="G213" t="s">
         <v>15</v>
       </c>
       <c r="H213" t="s">
-        <v>95</v>
+        <v>39</v>
       </c>
     </row>
     <row r="214" spans="1:9" x14ac:dyDescent="0.25">
@@ -7084,25 +7107,25 @@
         <v>212</v>
       </c>
       <c r="B214" t="s">
-        <v>289</v>
+        <v>287</v>
       </c>
       <c r="C214">
-        <v>39</v>
+        <v>27</v>
       </c>
       <c r="D214">
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="E214">
-        <v>0.5</v>
+        <v>3.3</v>
       </c>
       <c r="F214">
-        <v>5.4</v>
+        <v>2.2000000000000002</v>
       </c>
       <c r="G214" t="s">
         <v>15</v>
       </c>
       <c r="H214" t="s">
-        <v>95</v>
+        <v>41</v>
       </c>
     </row>
     <row r="215" spans="1:9" x14ac:dyDescent="0.25">
@@ -7110,25 +7133,25 @@
         <v>213</v>
       </c>
       <c r="B215" t="s">
-        <v>290</v>
+        <v>288</v>
       </c>
       <c r="C215">
-        <v>81</v>
+        <v>46</v>
       </c>
       <c r="D215">
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="E215">
-        <v>17.100000000000001</v>
+        <v>0.6</v>
       </c>
       <c r="F215">
-        <v>1.6</v>
+        <v>6.1</v>
       </c>
       <c r="G215" t="s">
         <v>15</v>
       </c>
       <c r="H215" t="s">
-        <v>177</v>
+        <v>95</v>
       </c>
     </row>
     <row r="216" spans="1:9" x14ac:dyDescent="0.25">
@@ -7136,25 +7159,25 @@
         <v>214</v>
       </c>
       <c r="B216" t="s">
-        <v>291</v>
+        <v>289</v>
       </c>
       <c r="C216">
-        <v>81</v>
+        <v>39</v>
       </c>
       <c r="D216">
-        <v>0.1</v>
+        <v>0.4</v>
       </c>
       <c r="E216">
-        <v>17.100000000000001</v>
+        <v>0.5</v>
       </c>
       <c r="F216">
-        <v>1.6</v>
+        <v>5.4</v>
       </c>
       <c r="G216" t="s">
         <v>15</v>
       </c>
       <c r="H216" t="s">
-        <v>177</v>
+        <v>95</v>
       </c>
     </row>
     <row r="217" spans="1:9" x14ac:dyDescent="0.25">
@@ -7162,25 +7185,25 @@
         <v>215</v>
       </c>
       <c r="B217" t="s">
-        <v>292</v>
+        <v>290</v>
       </c>
       <c r="C217">
-        <v>149</v>
+        <v>81</v>
       </c>
       <c r="D217">
-        <v>6.2</v>
+        <v>0.1</v>
       </c>
       <c r="E217">
-        <v>0</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="F217">
-        <v>23.4</v>
+        <v>1.6</v>
       </c>
       <c r="G217" t="s">
         <v>15</v>
       </c>
       <c r="H217" t="s">
-        <v>115</v>
+        <v>177</v>
       </c>
     </row>
     <row r="218" spans="1:9" x14ac:dyDescent="0.25">
@@ -7188,25 +7211,25 @@
         <v>216</v>
       </c>
       <c r="B218" t="s">
-        <v>293</v>
+        <v>291</v>
       </c>
       <c r="C218">
-        <v>316</v>
+        <v>81</v>
       </c>
       <c r="D218">
-        <v>10.4</v>
+        <v>0.1</v>
       </c>
       <c r="E218">
-        <v>45.7</v>
+        <v>17.100000000000001</v>
       </c>
       <c r="F218">
-        <v>8.9</v>
+        <v>1.6</v>
       </c>
       <c r="G218" t="s">
         <v>15</v>
       </c>
       <c r="H218" t="s">
-        <v>55</v>
+        <v>177</v>
       </c>
     </row>
     <row r="219" spans="1:9" x14ac:dyDescent="0.25">
@@ -7214,25 +7237,25 @@
         <v>217</v>
       </c>
       <c r="B219" t="s">
-        <v>294</v>
+        <v>292</v>
       </c>
       <c r="C219">
-        <v>271</v>
+        <v>149</v>
       </c>
       <c r="D219">
-        <v>4.9000000000000004</v>
+        <v>6.2</v>
       </c>
       <c r="E219">
-        <v>43.7</v>
+        <v>0</v>
       </c>
       <c r="F219">
-        <v>9.3000000000000007</v>
+        <v>23.4</v>
       </c>
       <c r="G219" t="s">
         <v>15</v>
       </c>
       <c r="H219" t="s">
-        <v>55</v>
+        <v>115</v>
       </c>
     </row>
     <row r="220" spans="1:9" x14ac:dyDescent="0.25">
@@ -7240,25 +7263,25 @@
         <v>218</v>
       </c>
       <c r="B220" t="s">
-        <v>295</v>
+        <v>293</v>
       </c>
       <c r="C220">
-        <v>21</v>
+        <v>316</v>
       </c>
       <c r="D220">
-        <v>0.3</v>
+        <v>10.4</v>
       </c>
       <c r="E220">
-        <v>3.3</v>
+        <v>45.7</v>
       </c>
       <c r="F220">
-        <v>0.9</v>
+        <v>8.9</v>
       </c>
       <c r="G220" t="s">
         <v>15</v>
       </c>
       <c r="H220" t="s">
-        <v>41</v>
+        <v>55</v>
       </c>
     </row>
     <row r="221" spans="1:9" x14ac:dyDescent="0.25">
@@ -7266,25 +7289,25 @@
         <v>219</v>
       </c>
       <c r="B221" t="s">
-        <v>296</v>
+        <v>294</v>
       </c>
       <c r="C221">
-        <v>69</v>
+        <v>271</v>
       </c>
       <c r="D221">
-        <v>2.1</v>
+        <v>4.9000000000000004</v>
       </c>
       <c r="E221">
-        <v>9.6999999999999993</v>
+        <v>43.7</v>
       </c>
       <c r="F221">
-        <v>1.8</v>
+        <v>9.3000000000000007</v>
       </c>
       <c r="G221" t="s">
         <v>15</v>
       </c>
       <c r="H221" t="s">
-        <v>59</v>
+        <v>55</v>
       </c>
     </row>
     <row r="222" spans="1:9" x14ac:dyDescent="0.25">
@@ -7292,28 +7315,25 @@
         <v>220</v>
       </c>
       <c r="B222" t="s">
-        <v>297</v>
+        <v>295</v>
       </c>
       <c r="C222">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="D222">
-        <v>1.1000000000000001</v>
+        <v>0.3</v>
       </c>
       <c r="E222">
-        <v>6.6</v>
+        <v>3.3</v>
       </c>
       <c r="F222">
-        <v>1</v>
+        <v>0.9</v>
       </c>
       <c r="G222" t="s">
         <v>15</v>
       </c>
       <c r="H222" t="s">
-        <v>73</v>
-      </c>
-      <c r="I222">
-        <v>1</v>
+        <v>41</v>
       </c>
     </row>
     <row r="223" spans="1:9" x14ac:dyDescent="0.25">
@@ -7321,25 +7341,25 @@
         <v>221</v>
       </c>
       <c r="B223" t="s">
-        <v>316</v>
+        <v>296</v>
       </c>
       <c r="C223">
-        <v>391</v>
+        <v>69</v>
       </c>
       <c r="D223">
-        <v>0.2</v>
+        <v>2.1</v>
       </c>
       <c r="E223">
-        <v>96.7</v>
+        <v>9.6999999999999993</v>
       </c>
       <c r="F223">
-        <v>0.2</v>
+        <v>1.8</v>
       </c>
       <c r="G223" t="s">
         <v>15</v>
       </c>
       <c r="H223" t="s">
-        <v>19</v>
+        <v>59</v>
       </c>
     </row>
     <row r="224" spans="1:9" x14ac:dyDescent="0.25">
@@ -7347,25 +7367,28 @@
         <v>222</v>
       </c>
       <c r="B224" t="s">
-        <v>298</v>
+        <v>297</v>
       </c>
       <c r="C224">
-        <v>92</v>
+        <v>42</v>
       </c>
       <c r="D224">
-        <v>2.2999999999999998</v>
+        <v>1.1000000000000001</v>
       </c>
       <c r="E224">
-        <v>1.6</v>
+        <v>6.6</v>
       </c>
       <c r="F224">
-        <v>13.4</v>
+        <v>1</v>
       </c>
       <c r="G224" t="s">
         <v>15</v>
       </c>
       <c r="H224" t="s">
-        <v>282</v>
+        <v>73</v>
+      </c>
+      <c r="I224">
+        <v>1</v>
       </c>
     </row>
     <row r="225" spans="1:9" x14ac:dyDescent="0.25">
@@ -7373,28 +7396,25 @@
         <v>223</v>
       </c>
       <c r="B225" t="s">
-        <v>299</v>
+        <v>315</v>
       </c>
       <c r="C225">
-        <v>255</v>
+        <v>391</v>
       </c>
       <c r="D225">
-        <v>25.2</v>
+        <v>0.2</v>
       </c>
       <c r="E225">
-        <v>2.1</v>
+        <v>96.7</v>
       </c>
       <c r="F225">
-        <v>4.5999999999999996</v>
+        <v>0.2</v>
       </c>
       <c r="G225" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H225" t="s">
-        <v>131</v>
-      </c>
-      <c r="I225">
-        <v>1.1000000000000001</v>
+        <v>19</v>
       </c>
     </row>
     <row r="226" spans="1:9" x14ac:dyDescent="0.25">
@@ -7402,28 +7422,25 @@
         <v>224</v>
       </c>
       <c r="B226" t="s">
-        <v>300</v>
+        <v>298</v>
       </c>
       <c r="C226">
-        <v>68</v>
+        <v>92</v>
       </c>
       <c r="D226">
-        <v>4</v>
+        <v>2.2999999999999998</v>
       </c>
       <c r="E226">
-        <v>4.7</v>
+        <v>1.6</v>
       </c>
       <c r="F226">
-        <v>3.2</v>
+        <v>13.4</v>
       </c>
       <c r="G226" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H226" t="s">
-        <v>163</v>
-      </c>
-      <c r="I226">
-        <v>1</v>
+        <v>282</v>
       </c>
     </row>
     <row r="227" spans="1:9" x14ac:dyDescent="0.25">
@@ -7431,25 +7448,28 @@
         <v>225</v>
       </c>
       <c r="B227" t="s">
-        <v>301</v>
+        <v>299</v>
       </c>
       <c r="C227">
-        <v>37</v>
+        <v>255</v>
       </c>
       <c r="D227">
-        <v>0.2</v>
+        <v>25.2</v>
       </c>
       <c r="E227">
-        <v>8.3000000000000007</v>
+        <v>2.1</v>
       </c>
       <c r="F227">
-        <v>0.7</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="G227" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H227" t="s">
-        <v>29</v>
+        <v>131</v>
+      </c>
+      <c r="I227">
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="228" spans="1:9" x14ac:dyDescent="0.25">
@@ -7457,25 +7477,28 @@
         <v>226</v>
       </c>
       <c r="B228" t="s">
-        <v>302</v>
+        <v>300</v>
       </c>
       <c r="C228">
-        <v>242</v>
+        <v>68</v>
       </c>
       <c r="D228">
-        <v>0.8</v>
+        <v>4</v>
       </c>
       <c r="E228">
-        <v>48.9</v>
+        <v>4.7</v>
       </c>
       <c r="F228">
-        <v>8.5</v>
+        <v>3.2</v>
       </c>
       <c r="G228" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H228" t="s">
-        <v>55</v>
+        <v>163</v>
+      </c>
+      <c r="I228">
+        <v>1</v>
       </c>
     </row>
     <row r="229" spans="1:9" x14ac:dyDescent="0.25">
@@ -7483,25 +7506,25 @@
         <v>227</v>
       </c>
       <c r="B229" t="s">
-        <v>303</v>
+        <v>343</v>
       </c>
       <c r="C229">
-        <v>242</v>
+        <v>691</v>
       </c>
       <c r="D229">
-        <v>20.399999999999999</v>
+        <v>63</v>
       </c>
       <c r="E229">
-        <v>0.6</v>
+        <v>11</v>
       </c>
       <c r="F229">
-        <v>13.9</v>
+        <v>17</v>
       </c>
       <c r="G229" t="s">
         <v>15</v>
       </c>
       <c r="H229" t="s">
-        <v>44</v>
+        <v>57</v>
       </c>
     </row>
     <row r="230" spans="1:9" x14ac:dyDescent="0.25">
@@ -7509,28 +7532,25 @@
         <v>228</v>
       </c>
       <c r="B230" t="s">
-        <v>317</v>
+        <v>301</v>
       </c>
       <c r="C230">
-        <v>96</v>
+        <v>37</v>
       </c>
       <c r="D230">
-        <v>0.8</v>
+        <v>0.2</v>
       </c>
       <c r="E230">
-        <v>21.5</v>
+        <v>8.3000000000000007</v>
       </c>
       <c r="F230">
-        <v>0.8</v>
+        <v>0.7</v>
       </c>
       <c r="G230" t="s">
-        <v>21</v>
+        <v>15</v>
       </c>
       <c r="H230" t="s">
-        <v>59</v>
-      </c>
-      <c r="I230">
-        <v>1</v>
+        <v>29</v>
       </c>
     </row>
     <row r="231" spans="1:9" x14ac:dyDescent="0.25">
@@ -7538,25 +7558,25 @@
         <v>229</v>
       </c>
       <c r="B231" t="s">
-        <v>304</v>
+        <v>302</v>
       </c>
       <c r="C231">
-        <v>505</v>
+        <v>242</v>
       </c>
       <c r="D231">
-        <v>25.9</v>
+        <v>0.8</v>
       </c>
       <c r="E231">
-        <v>50.9</v>
+        <v>48.9</v>
       </c>
       <c r="F231">
-        <v>14.2</v>
+        <v>8.5</v>
       </c>
       <c r="G231" t="s">
         <v>15</v>
       </c>
       <c r="H231" t="s">
-        <v>26</v>
+        <v>55</v>
       </c>
     </row>
     <row r="232" spans="1:9" x14ac:dyDescent="0.25">
@@ -7564,25 +7584,25 @@
         <v>230</v>
       </c>
       <c r="B232" t="s">
-        <v>305</v>
+        <v>339</v>
       </c>
       <c r="C232">
-        <v>23</v>
+        <v>286</v>
       </c>
       <c r="D232">
-        <v>0.5</v>
+        <v>25</v>
       </c>
       <c r="E232">
-        <v>2.9</v>
+        <v>1</v>
       </c>
       <c r="F232">
-        <v>0.8</v>
+        <v>14</v>
       </c>
       <c r="G232" t="s">
         <v>15</v>
       </c>
       <c r="H232" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
     </row>
     <row r="233" spans="1:9" x14ac:dyDescent="0.25">
@@ -7590,25 +7610,25 @@
         <v>231</v>
       </c>
       <c r="B233" t="s">
-        <v>306</v>
+        <v>316</v>
       </c>
       <c r="C233">
-        <v>28</v>
+        <v>96</v>
       </c>
       <c r="D233">
-        <v>0.2</v>
+        <v>0.8</v>
       </c>
       <c r="E233">
-        <v>2.5</v>
+        <v>21.5</v>
       </c>
       <c r="F233">
-        <v>0.4</v>
+        <v>0.8</v>
       </c>
       <c r="G233" t="s">
         <v>21</v>
       </c>
       <c r="H233" t="s">
-        <v>328</v>
+        <v>59</v>
       </c>
       <c r="I233">
         <v>1</v>
@@ -7619,25 +7639,25 @@
         <v>232</v>
       </c>
       <c r="B234" t="s">
-        <v>307</v>
+        <v>303</v>
       </c>
       <c r="C234">
-        <v>390</v>
+        <v>505</v>
       </c>
       <c r="D234">
-        <v>0</v>
+        <v>25.9</v>
       </c>
       <c r="E234">
-        <v>97.6</v>
+        <v>50.9</v>
       </c>
       <c r="F234">
-        <v>0</v>
+        <v>14.2</v>
       </c>
       <c r="G234" t="s">
         <v>15</v>
       </c>
       <c r="H234" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
     </row>
     <row r="235" spans="1:9" x14ac:dyDescent="0.25">
@@ -7645,25 +7665,25 @@
         <v>233</v>
       </c>
       <c r="B235" t="s">
-        <v>308</v>
+        <v>304</v>
       </c>
       <c r="C235">
-        <v>400</v>
+        <v>23</v>
       </c>
       <c r="D235">
-        <v>0</v>
+        <v>0.5</v>
       </c>
       <c r="E235">
-        <v>100</v>
+        <v>2.9</v>
       </c>
       <c r="F235">
-        <v>0</v>
+        <v>0.8</v>
       </c>
       <c r="G235" t="s">
         <v>15</v>
       </c>
       <c r="H235" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
     </row>
     <row r="236" spans="1:9" x14ac:dyDescent="0.25">
@@ -7671,25 +7691,28 @@
         <v>234</v>
       </c>
       <c r="B236" t="s">
-        <v>309</v>
+        <v>305</v>
       </c>
       <c r="C236">
-        <v>421</v>
+        <v>28</v>
       </c>
       <c r="D236">
-        <v>7.8</v>
+        <v>0.2</v>
       </c>
       <c r="E236">
-        <v>74.599999999999994</v>
+        <v>2.5</v>
       </c>
       <c r="F236">
-        <v>11.6</v>
+        <v>0.4</v>
       </c>
       <c r="G236" t="s">
-        <v>15</v>
+        <v>21</v>
       </c>
       <c r="H236" t="s">
-        <v>190</v>
+        <v>327</v>
+      </c>
+      <c r="I236">
+        <v>1</v>
       </c>
     </row>
     <row r="237" spans="1:9" x14ac:dyDescent="0.25">
@@ -7697,25 +7720,25 @@
         <v>235</v>
       </c>
       <c r="B237" t="s">
-        <v>310</v>
+        <v>340</v>
       </c>
       <c r="C237">
-        <v>413</v>
+        <v>19</v>
       </c>
       <c r="D237">
-        <v>9.1</v>
+        <v>0.4</v>
       </c>
       <c r="E237">
-        <v>61.2</v>
+        <v>2</v>
       </c>
       <c r="F237">
-        <v>17.5</v>
+        <v>1.6</v>
       </c>
       <c r="G237" t="s">
         <v>15</v>
       </c>
       <c r="H237" t="s">
-        <v>190</v>
+        <v>41</v>
       </c>
     </row>
     <row r="238" spans="1:9" x14ac:dyDescent="0.25">
@@ -7723,24 +7746,128 @@
         <v>236</v>
       </c>
       <c r="B238" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="C238">
+        <v>390</v>
+      </c>
+      <c r="D238">
+        <v>0</v>
+      </c>
+      <c r="E238">
+        <v>97.6</v>
+      </c>
+      <c r="F238">
+        <v>0</v>
+      </c>
+      <c r="G238" t="s">
+        <v>15</v>
+      </c>
+      <c r="H238" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A239">
+        <v>237</v>
+      </c>
+      <c r="B239" t="s">
+        <v>307</v>
+      </c>
+      <c r="C239">
+        <v>400</v>
+      </c>
+      <c r="D239">
+        <v>0</v>
+      </c>
+      <c r="E239">
+        <v>100</v>
+      </c>
+      <c r="F239">
+        <v>0</v>
+      </c>
+      <c r="G239" t="s">
+        <v>15</v>
+      </c>
+      <c r="H239" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A240">
+        <v>238</v>
+      </c>
+      <c r="B240" t="s">
+        <v>308</v>
+      </c>
+      <c r="C240">
+        <v>421</v>
+      </c>
+      <c r="D240">
+        <v>7.8</v>
+      </c>
+      <c r="E240">
+        <v>74.599999999999994</v>
+      </c>
+      <c r="F240">
+        <v>11.6</v>
+      </c>
+      <c r="G240" t="s">
+        <v>15</v>
+      </c>
+      <c r="H240" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A241">
+        <v>239</v>
+      </c>
+      <c r="B241" t="s">
+        <v>309</v>
+      </c>
+      <c r="C241">
+        <v>413</v>
+      </c>
+      <c r="D241">
+        <v>9.1</v>
+      </c>
+      <c r="E241">
+        <v>61.2</v>
+      </c>
+      <c r="F241">
+        <v>17.5</v>
+      </c>
+      <c r="G241" t="s">
+        <v>15</v>
+      </c>
+      <c r="H241" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A242">
+        <v>240</v>
+      </c>
+      <c r="B242" t="s">
+        <v>310</v>
+      </c>
+      <c r="C242">
         <v>39</v>
       </c>
-      <c r="D238">
+      <c r="D242">
         <v>0.6</v>
       </c>
-      <c r="E238">
+      <c r="E242">
         <v>6.3</v>
       </c>
-      <c r="F238">
+      <c r="F242">
         <v>1.1000000000000001</v>
       </c>
-      <c r="G238" t="s">
-        <v>15</v>
-      </c>
-      <c r="H238" t="s">
+      <c r="G242" t="s">
+        <v>15</v>
+      </c>
+      <c r="H242" t="s">
         <v>41</v>
       </c>
     </row>

</xml_diff>

<commit_message>
fixed typo in database and updated all IDs
</commit_message>
<xml_diff>
--- a/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
+++ b/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\NutriLearnVR\NutriLearnVR\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A23CF9D-9767-4276-B854-E043542B5D6D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9230EDA-AB3A-4FCA-855B-7454D1EF9C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5175" windowWidth="29040" windowHeight="15720" xr2:uid="{8C58FACA-B588-4A2F-A614-585794A6AB4A}"/>
   </bookViews>
@@ -1448,8 +1448,8 @@
   <dimension ref="A1:I253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A240" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A225" sqref="A225"/>
+      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3813,7 +3813,7 @@
         <v>334</v>
       </c>
       <c r="C90">
-        <v>46.1</v>
+        <v>46</v>
       </c>
       <c r="D90">
         <v>1.5</v>

</xml_diff>

<commit_message>
updated database for new scoring system using NutriScore values and more nutrient information
</commit_message>
<xml_diff>
--- a/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
+++ b/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\NutriLearnVR\NutriLearnVR\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9230EDA-AB3A-4FCA-855B-7454D1EF9C74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405CE51E-3F4F-4220-A0C9-481DF1B60309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="38280" yWindow="5175" windowWidth="29040" windowHeight="15720" xr2:uid="{8C58FACA-B588-4A2F-A614-585794A6AB4A}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8C58FACA-B588-4A2F-A614-585794A6AB4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Generische Lebensmittel" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="765" uniqueCount="343">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="346">
   <si>
     <t>ID</t>
   </si>
@@ -1022,9 +1022,6 @@
     <t>Zucchini, roh</t>
   </si>
   <si>
-    <t>rote Zwiebel, roh</t>
-  </si>
-  <si>
     <t>Kartoffel, roh</t>
   </si>
   <si>
@@ -1068,6 +1065,18 @@
   </si>
   <si>
     <t>Spiegelei</t>
+  </si>
+  <si>
+    <t>NutriScore-Wert</t>
+  </si>
+  <si>
+    <t>Rote Zwiebel, roh</t>
+  </si>
+  <si>
+    <t>gesättigte Fettsäuren</t>
+  </si>
+  <si>
+    <t>Zucker</t>
   </si>
 </sst>
 </file>
@@ -1445,11 +1454,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB881A-4068-4DEA-B356-9AC1A56CFC86}">
-  <dimension ref="A1:I253"/>
+  <dimension ref="A1:L253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A222" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="C91" sqref="C91"/>
+      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J91" sqref="J91"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1457,11 +1466,11 @@
     <col min="1" max="1" width="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="78.28515625" bestFit="1" customWidth="1"/>
     <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="166.140625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="32.140625" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" s="3" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" s="3" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1489,8 +1498,17 @@
       <c r="I1" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J1" s="1" t="s">
+        <v>344</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>345</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>342</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1516,7 +1534,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1545,7 +1563,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1571,7 +1589,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1597,7 +1615,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1626,7 +1644,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1651,8 +1669,17 @@
       <c r="H7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J7">
+        <v>0.1</v>
+      </c>
+      <c r="K7">
+        <v>11.5</v>
+      </c>
+      <c r="L7">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1678,7 +1705,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1704,7 +1731,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1733,7 +1760,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1759,7 +1786,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1785,7 +1812,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1811,7 +1838,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1836,8 +1863,17 @@
       <c r="H14" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J14">
+        <v>9.1</v>
+      </c>
+      <c r="K14">
+        <v>0.7</v>
+      </c>
+      <c r="L14">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1862,8 +1898,17 @@
       <c r="H15" t="s">
         <v>312</v>
       </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J15">
+        <v>2.8</v>
+      </c>
+      <c r="K15">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="L15">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1889,7 +1934,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1914,8 +1959,17 @@
       <c r="H17" t="s">
         <v>39</v>
       </c>
-    </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J17">
+        <v>0</v>
+      </c>
+      <c r="K17">
+        <v>15</v>
+      </c>
+      <c r="L17">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -1940,8 +1994,17 @@
       <c r="H18" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J18">
+        <v>0.1</v>
+      </c>
+      <c r="K18">
+        <v>15.6</v>
+      </c>
+      <c r="L18">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -1967,7 +2030,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -1993,7 +2056,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2019,7 +2082,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2044,8 +2107,17 @@
       <c r="H22" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J22">
+        <v>0.1</v>
+      </c>
+      <c r="K22">
+        <v>9</v>
+      </c>
+      <c r="L22">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2074,7 +2146,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2100,7 +2172,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2126,7 +2198,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2152,7 +2224,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2177,8 +2249,17 @@
       <c r="H27" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J27">
+        <v>0.1</v>
+      </c>
+      <c r="K27">
+        <v>3.3</v>
+      </c>
+      <c r="L27">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2206,13 +2287,22 @@
       <c r="I28">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J28">
+        <v>64.900000000000006</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
       <c r="B29" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="C29">
         <v>298</v>
@@ -2232,8 +2322,17 @@
       <c r="H29" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J29">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="K29">
+        <v>0.2</v>
+      </c>
+      <c r="L29">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2259,7 +2358,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2285,7 +2384,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2310,8 +2409,17 @@
       <c r="H32" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J32">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="K32">
+        <v>1.3</v>
+      </c>
+      <c r="L32">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2337,12 +2445,12 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
       <c r="B34" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="C34">
         <v>754</v>
@@ -2362,8 +2470,17 @@
       <c r="H34" t="s">
         <v>72</v>
       </c>
-    </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J34">
+        <v>53.8</v>
+      </c>
+      <c r="K34">
+        <v>0.1</v>
+      </c>
+      <c r="L34">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2392,7 +2509,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2417,8 +2534,17 @@
       <c r="H36" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J36">
+        <v>6.5</v>
+      </c>
+      <c r="K36">
+        <v>2.9</v>
+      </c>
+      <c r="L36">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2443,8 +2569,17 @@
       <c r="H37" t="s">
         <v>64</v>
       </c>
-    </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J37">
+        <v>13.9</v>
+      </c>
+      <c r="K37">
+        <v>0</v>
+      </c>
+      <c r="L37">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2470,7 +2605,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2496,7 +2631,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2521,8 +2656,17 @@
       <c r="H40" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J40">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K40">
+        <v>3.1</v>
+      </c>
+      <c r="L40">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2547,8 +2691,17 @@
       <c r="H41" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J41">
+        <v>0.1</v>
+      </c>
+      <c r="K41">
+        <v>0.12</v>
+      </c>
+      <c r="L41">
+        <v>-2</v>
+      </c>
+    </row>
+    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2573,8 +2726,17 @@
       <c r="H42" t="s">
         <v>81</v>
       </c>
-    </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J42">
+        <v>0</v>
+      </c>
+      <c r="K42">
+        <v>0.3</v>
+      </c>
+      <c r="L42">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2600,7 +2762,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2626,7 +2788,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2652,7 +2814,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2678,7 +2840,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2704,7 +2866,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2729,8 +2891,17 @@
       <c r="H48" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J48">
+        <v>0.1</v>
+      </c>
+      <c r="K48">
+        <v>7.2</v>
+      </c>
+      <c r="L48">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2756,12 +2927,12 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
       <c r="B50" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="C50">
         <v>244</v>
@@ -2781,8 +2952,17 @@
       <c r="H50" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J50">
+        <v>8.6999999999999993</v>
+      </c>
+      <c r="K50">
+        <v>2.2999999999999998</v>
+      </c>
+      <c r="L50">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2807,8 +2987,17 @@
       <c r="H51" t="s">
         <v>96</v>
       </c>
-    </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J51">
+        <v>9.3000000000000007</v>
+      </c>
+      <c r="K51">
+        <v>26.4</v>
+      </c>
+      <c r="L51">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -2834,7 +3023,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -2860,7 +3049,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -2885,8 +3074,17 @@
       <c r="H54" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J54">
+        <v>6.6</v>
+      </c>
+      <c r="K54">
+        <v>2.9</v>
+      </c>
+      <c r="L54">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -2912,7 +3110,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -2938,7 +3136,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -2964,7 +3162,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -2990,7 +3188,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -3019,7 +3217,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -3045,7 +3243,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3071,7 +3269,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -3097,7 +3295,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3123,7 +3321,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3149,7 +3347,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3175,7 +3373,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3200,8 +3398,17 @@
       <c r="H66" t="s">
         <v>115</v>
       </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J66">
+        <v>8.6</v>
+      </c>
+      <c r="K66">
+        <v>4.2</v>
+      </c>
+      <c r="L66">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3227,7 +3434,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3253,7 +3460,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3279,7 +3486,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3305,7 +3512,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3331,7 +3538,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3357,7 +3564,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3383,7 +3590,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -3409,7 +3616,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -3435,7 +3642,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -3461,7 +3668,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -3490,7 +3697,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -3519,7 +3726,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -3545,7 +3752,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -3571,7 +3778,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -3597,7 +3804,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -3623,7 +3830,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -3649,7 +3856,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -3675,7 +3882,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -3701,12 +3908,12 @@
         <v>143</v>
       </c>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
       <c r="B86" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="C86">
         <v>26</v>
@@ -3726,8 +3933,17 @@
       <c r="H86" t="s">
         <v>30</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J86">
+        <v>0.1</v>
+      </c>
+      <c r="K86">
+        <v>3.3</v>
+      </c>
+      <c r="L86">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -3753,7 +3969,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -3778,8 +3994,17 @@
       <c r="H88" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J88">
+        <v>0.04</v>
+      </c>
+      <c r="K88">
+        <v>1.7</v>
+      </c>
+      <c r="L88">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -3804,13 +4029,22 @@
       <c r="H89" t="s">
         <v>141</v>
       </c>
-    </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J89">
+        <v>1</v>
+      </c>
+      <c r="K89">
+        <v>1</v>
+      </c>
+      <c r="L89">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
       <c r="B90" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="C90">
         <v>46</v>
@@ -3833,8 +4067,17 @@
       <c r="I90">
         <v>1</v>
       </c>
-    </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J90">
+        <v>0.3</v>
+      </c>
+      <c r="K90">
+        <v>3.4</v>
+      </c>
+      <c r="L90">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -3860,7 +4103,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -3885,8 +4128,17 @@
       <c r="H92" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J92">
+        <v>4.2</v>
+      </c>
+      <c r="K92">
+        <v>3</v>
+      </c>
+      <c r="L92">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -3914,8 +4166,17 @@
       <c r="I93">
         <v>1.3</v>
       </c>
-    </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J93">
+        <v>10.7</v>
+      </c>
+      <c r="K93">
+        <v>55.9</v>
+      </c>
+      <c r="L93">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -3941,7 +4202,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -3967,7 +4228,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -3993,7 +4254,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -4019,7 +4280,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -4047,8 +4308,17 @@
       <c r="I98">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J98">
+        <v>0</v>
+      </c>
+      <c r="K98">
+        <v>76</v>
+      </c>
+      <c r="L98">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -4074,7 +4344,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -4100,7 +4370,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -4125,8 +4395,17 @@
       <c r="H101" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J101">
+        <v>3.3</v>
+      </c>
+      <c r="K101">
+        <v>0.5</v>
+      </c>
+      <c r="L101">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
@@ -4152,7 +4431,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
@@ -4178,7 +4457,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>102</v>
       </c>
@@ -4207,7 +4486,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>103</v>
       </c>
@@ -4236,7 +4515,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>104</v>
       </c>
@@ -4265,7 +4544,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105</v>
       </c>
@@ -4294,7 +4573,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
       </c>
@@ -4320,7 +4599,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
@@ -4346,7 +4625,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>108</v>
       </c>
@@ -4372,12 +4651,12 @@
         <v>88</v>
       </c>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>109</v>
       </c>
       <c r="B111" t="s">
-        <v>328</v>
+        <v>327</v>
       </c>
       <c r="C111">
         <v>70</v>
@@ -4397,8 +4676,17 @@
       <c r="H111" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J111">
+        <v>0</v>
+      </c>
+      <c r="K111">
+        <v>0.7</v>
+      </c>
+      <c r="L111">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>110</v>
       </c>
@@ -4423,8 +4711,17 @@
       <c r="H112" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J112">
+        <v>0.1</v>
+      </c>
+      <c r="K112">
+        <v>6</v>
+      </c>
+      <c r="L112">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>111</v>
       </c>
@@ -4450,7 +4747,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>112</v>
       </c>
@@ -4479,12 +4776,12 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>113</v>
       </c>
       <c r="B115" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="C115">
         <v>573</v>
@@ -4504,8 +4801,17 @@
       <c r="H115" t="s">
         <v>143</v>
       </c>
-    </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J115">
+        <v>21.4</v>
+      </c>
+      <c r="K115">
+        <v>39.6</v>
+      </c>
+      <c r="L115">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>114</v>
       </c>
@@ -4531,7 +4837,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>115</v>
       </c>
@@ -4556,8 +4862,17 @@
       <c r="H117" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J117">
+        <v>0.3</v>
+      </c>
+      <c r="K117">
+        <v>3.3</v>
+      </c>
+      <c r="L117">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>116</v>
       </c>
@@ -4582,8 +4897,17 @@
       <c r="H118" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J118">
+        <v>0.1</v>
+      </c>
+      <c r="K118">
+        <v>22.5</v>
+      </c>
+      <c r="L118">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>117</v>
       </c>
@@ -4608,8 +4932,17 @@
       <c r="H119" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J119">
+        <v>5.2</v>
+      </c>
+      <c r="K119">
+        <v>19.8</v>
+      </c>
+      <c r="L119">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>118</v>
       </c>
@@ -4635,7 +4968,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>119</v>
       </c>
@@ -4661,7 +4994,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>120</v>
       </c>
@@ -4689,8 +5022,17 @@
       <c r="I122">
         <v>1.4</v>
       </c>
-    </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J122">
+        <v>0.05</v>
+      </c>
+      <c r="K122">
+        <v>58.7</v>
+      </c>
+      <c r="L122">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>121</v>
       </c>
@@ -4716,7 +5058,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>122</v>
       </c>
@@ -4742,7 +5084,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>123</v>
       </c>
@@ -4768,7 +5110,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>124</v>
       </c>
@@ -4794,7 +5136,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>125</v>
       </c>
@@ -4823,7 +5165,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>126</v>
       </c>
@@ -4849,7 +5191,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="129" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>127</v>
       </c>
@@ -4875,7 +5217,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="130" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>128</v>
       </c>
@@ -4901,7 +5243,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="131" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>129</v>
       </c>
@@ -4926,8 +5268,17 @@
       <c r="H131" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="132" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J131">
+        <v>0.2</v>
+      </c>
+      <c r="K131">
+        <v>3.4</v>
+      </c>
+      <c r="L131">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>130</v>
       </c>
@@ -4952,8 +5303,17 @@
       <c r="H132" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="133" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J132">
+        <v>0.01</v>
+      </c>
+      <c r="K132">
+        <v>8.6</v>
+      </c>
+      <c r="L132">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>131</v>
       </c>
@@ -4978,8 +5338,17 @@
       <c r="H133" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="134" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J133">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K133">
+        <v>6.6</v>
+      </c>
+      <c r="L133">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>132</v>
       </c>
@@ -5005,7 +5374,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="135" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>133</v>
       </c>
@@ -5031,7 +5400,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="136" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>134</v>
       </c>
@@ -5057,7 +5426,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="137" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>135</v>
       </c>
@@ -5083,7 +5452,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="138" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>136</v>
       </c>
@@ -5109,7 +5478,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="139" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>137</v>
       </c>
@@ -5135,7 +5504,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="140" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>138</v>
       </c>
@@ -5163,8 +5532,17 @@
       <c r="I140">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="141" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J140">
+        <v>5.3</v>
+      </c>
+      <c r="K140">
+        <v>1.5</v>
+      </c>
+      <c r="L140">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>139</v>
       </c>
@@ -5189,8 +5567,17 @@
       <c r="H141" t="s">
         <v>69</v>
       </c>
-    </row>
-    <row r="142" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J141">
+        <v>0.3</v>
+      </c>
+      <c r="K141">
+        <v>0.4</v>
+      </c>
+      <c r="L141">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>140</v>
       </c>
@@ -5219,7 +5606,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>141</v>
       </c>
@@ -5245,7 +5632,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="144" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>142</v>
       </c>
@@ -5271,7 +5658,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="145" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>143</v>
       </c>
@@ -5300,7 +5687,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>144</v>
       </c>
@@ -5329,7 +5716,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>145</v>
       </c>
@@ -5355,7 +5742,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="148" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>146</v>
       </c>
@@ -5381,7 +5768,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="149" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>147</v>
       </c>
@@ -5407,7 +5794,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="150" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>148</v>
       </c>
@@ -5433,7 +5820,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="151" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>149</v>
       </c>
@@ -5459,12 +5846,12 @@
         <v>20</v>
       </c>
     </row>
-    <row r="152" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>150</v>
       </c>
       <c r="B152" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="C152">
         <v>159</v>
@@ -5482,15 +5869,24 @@
         <v>9</v>
       </c>
       <c r="H152" t="s">
-        <v>337</v>
-      </c>
-    </row>
-    <row r="153" spans="1:9" x14ac:dyDescent="0.25">
+        <v>336</v>
+      </c>
+      <c r="J152">
+        <v>0.2</v>
+      </c>
+      <c r="K152">
+        <v>0.6</v>
+      </c>
+      <c r="L152">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>151</v>
       </c>
       <c r="B153" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="C153">
         <v>545</v>
@@ -5510,8 +5906,17 @@
       <c r="H153" t="s">
         <v>188</v>
       </c>
-    </row>
-    <row r="154" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J153">
+        <v>10.7</v>
+      </c>
+      <c r="K153">
+        <v>55.9</v>
+      </c>
+      <c r="L153">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>152</v>
       </c>
@@ -5537,7 +5942,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="155" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>153</v>
       </c>
@@ -5563,7 +5968,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="156" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>154</v>
       </c>
@@ -5591,8 +5996,17 @@
       <c r="I156">
         <v>0.9</v>
       </c>
-    </row>
-    <row r="157" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J156">
+        <v>10.7</v>
+      </c>
+      <c r="K156">
+        <v>0</v>
+      </c>
+      <c r="L156">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>155</v>
       </c>
@@ -5617,8 +6031,17 @@
       <c r="H157" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="158" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J157">
+        <v>0</v>
+      </c>
+      <c r="K157">
+        <v>7.6</v>
+      </c>
+      <c r="L157">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>156</v>
       </c>
@@ -5646,13 +6069,22 @@
       <c r="I158">
         <v>1.04</v>
       </c>
-    </row>
-    <row r="159" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J158">
+        <v>0.1</v>
+      </c>
+      <c r="K158">
+        <v>10</v>
+      </c>
+      <c r="L158">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>157</v>
       </c>
       <c r="B159" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="C159">
         <v>20</v>
@@ -5670,10 +6102,19 @@
         <v>9</v>
       </c>
       <c r="H159" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="160" spans="1:9" x14ac:dyDescent="0.25">
+        <v>339</v>
+      </c>
+      <c r="J159">
+        <v>0</v>
+      </c>
+      <c r="K159">
+        <v>5</v>
+      </c>
+      <c r="L159">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>158</v>
       </c>
@@ -5699,7 +6140,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="161" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>159</v>
       </c>
@@ -5725,7 +6166,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="162" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>160</v>
       </c>
@@ -5751,7 +6192,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="163" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>161</v>
       </c>
@@ -5777,7 +6218,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="164" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>162</v>
       </c>
@@ -5803,7 +6244,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="165" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>163</v>
       </c>
@@ -5829,7 +6270,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="166" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>164</v>
       </c>
@@ -5855,7 +6296,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>165</v>
       </c>
@@ -5880,8 +6321,17 @@
       <c r="H167" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="168" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J167">
+        <v>0</v>
+      </c>
+      <c r="K167">
+        <v>8.8000000000000007</v>
+      </c>
+      <c r="L167">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>166</v>
       </c>
@@ -5907,7 +6357,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="169" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>167</v>
       </c>
@@ -5933,7 +6383,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="170" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>168</v>
       </c>
@@ -5959,7 +6409,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="171" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>169</v>
       </c>
@@ -5985,7 +6435,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="172" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>170</v>
       </c>
@@ -6011,7 +6461,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="173" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>171</v>
       </c>
@@ -6037,7 +6487,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="174" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>172</v>
       </c>
@@ -6063,7 +6513,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="175" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>173</v>
       </c>
@@ -6089,7 +6539,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="176" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>174</v>
       </c>
@@ -6115,7 +6565,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="177" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>175</v>
       </c>
@@ -6141,7 +6591,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="178" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>176</v>
       </c>
@@ -6167,7 +6617,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="179" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>177</v>
       </c>
@@ -6192,8 +6642,17 @@
       <c r="H179" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="180" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J179">
+        <v>0.3</v>
+      </c>
+      <c r="K179">
+        <v>0</v>
+      </c>
+      <c r="L179">
+        <v>-4</v>
+      </c>
+    </row>
+    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>178</v>
       </c>
@@ -6219,7 +6678,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="181" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>179</v>
       </c>
@@ -6244,8 +6703,17 @@
       <c r="H181" t="s">
         <v>138</v>
       </c>
-    </row>
-    <row r="182" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J181">
+        <v>3.2</v>
+      </c>
+      <c r="K181">
+        <v>0</v>
+      </c>
+      <c r="L181">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>180</v>
       </c>
@@ -6271,7 +6739,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="183" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>181</v>
       </c>
@@ -6297,7 +6765,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="184" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>182</v>
       </c>
@@ -6322,8 +6790,17 @@
       <c r="H184" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="185" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J184">
+        <v>0</v>
+      </c>
+      <c r="K184">
+        <v>2.1</v>
+      </c>
+      <c r="L184">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>183</v>
       </c>
@@ -6352,7 +6829,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="186" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>184</v>
       </c>
@@ -6378,7 +6855,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="187" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>185</v>
       </c>
@@ -6404,7 +6881,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="188" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>186</v>
       </c>
@@ -6430,7 +6907,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="189" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>187</v>
       </c>
@@ -6456,7 +6933,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="190" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>188</v>
       </c>
@@ -6482,7 +6959,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="191" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>189</v>
       </c>
@@ -6508,7 +6985,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="192" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>190</v>
       </c>
@@ -6534,7 +7011,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="193" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>191</v>
       </c>
@@ -6560,7 +7037,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="194" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>192</v>
       </c>
@@ -6585,8 +7062,17 @@
       <c r="H194" t="s">
         <v>147</v>
       </c>
-    </row>
-    <row r="195" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J194">
+        <v>6.3</v>
+      </c>
+      <c r="K194">
+        <v>0.5</v>
+      </c>
+      <c r="L194">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>193</v>
       </c>
@@ -6612,7 +7098,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>194</v>
       </c>
@@ -6638,12 +7124,12 @@
         <v>163</v>
       </c>
     </row>
-    <row r="197" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>195</v>
       </c>
       <c r="B197" t="s">
-        <v>327</v>
+        <v>343</v>
       </c>
       <c r="C197">
         <v>28</v>
@@ -6663,8 +7149,17 @@
       <c r="H197" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="198" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J197">
+        <v>0.2</v>
+      </c>
+      <c r="K197">
+        <v>4.8</v>
+      </c>
+      <c r="L197">
+        <v>-5</v>
+      </c>
+    </row>
+    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>196</v>
       </c>
@@ -6690,7 +7185,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="199" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>197</v>
       </c>
@@ -6716,7 +7211,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="200" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>198</v>
       </c>
@@ -6741,8 +7236,17 @@
       <c r="H200" t="s">
         <v>46</v>
       </c>
-    </row>
-    <row r="201" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J200">
+        <v>11.3</v>
+      </c>
+      <c r="K200">
+        <v>1</v>
+      </c>
+      <c r="L200">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>199</v>
       </c>
@@ -6771,7 +7275,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="202" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>200</v>
       </c>
@@ -6800,7 +7304,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="203" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>201</v>
       </c>
@@ -6826,7 +7330,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="204" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>202</v>
       </c>
@@ -6852,7 +7356,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="205" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>203</v>
       </c>
@@ -6878,7 +7382,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="206" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>204</v>
       </c>
@@ -6904,7 +7408,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="207" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>205</v>
       </c>
@@ -6932,8 +7436,17 @@
       <c r="I207">
         <v>1</v>
       </c>
-    </row>
-    <row r="208" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J207">
+        <v>15.8</v>
+      </c>
+      <c r="K207">
+        <v>2.4</v>
+      </c>
+      <c r="L207">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>206</v>
       </c>
@@ -6959,7 +7472,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="209" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>207</v>
       </c>
@@ -6985,12 +7498,12 @@
         <v>100</v>
       </c>
     </row>
-    <row r="210" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>208</v>
       </c>
       <c r="B210" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="C210">
         <v>409</v>
@@ -7011,7 +7524,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="211" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>209</v>
       </c>
@@ -7037,7 +7550,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="212" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>210</v>
       </c>
@@ -7063,7 +7576,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="213" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>211</v>
       </c>
@@ -7089,7 +7602,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="214" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>212</v>
       </c>
@@ -7115,7 +7628,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="215" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>213</v>
       </c>
@@ -7141,7 +7654,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="216" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>214</v>
       </c>
@@ -7167,7 +7680,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="217" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>215</v>
       </c>
@@ -7193,7 +7706,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="218" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>216</v>
       </c>
@@ -7219,7 +7732,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="219" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>217</v>
       </c>
@@ -7245,7 +7758,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="220" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>218</v>
       </c>
@@ -7271,7 +7784,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="221" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>219</v>
       </c>
@@ -7296,8 +7809,17 @@
       <c r="H221" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="222" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J221">
+        <v>5.4</v>
+      </c>
+      <c r="K221">
+        <v>3.4</v>
+      </c>
+      <c r="L221">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>220</v>
       </c>
@@ -7326,7 +7848,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="223" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>221</v>
       </c>
@@ -7352,7 +7874,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="224" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>222</v>
       </c>
@@ -7378,12 +7900,12 @@
         <v>32</v>
       </c>
     </row>
-    <row r="225" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>223</v>
       </c>
       <c r="B225" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="C225">
         <v>223</v>
@@ -7403,8 +7925,17 @@
       <c r="H225" t="s">
         <v>160</v>
       </c>
-    </row>
-    <row r="226" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J225">
+        <v>8.1999999999999993</v>
+      </c>
+      <c r="K225">
+        <v>1</v>
+      </c>
+      <c r="L225">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>224</v>
       </c>
@@ -7430,7 +7961,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="227" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>225</v>
       </c>
@@ -7456,7 +7987,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="228" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>226</v>
       </c>
@@ -7482,7 +8013,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="229" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>227</v>
       </c>
@@ -7508,7 +8039,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="230" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>228</v>
       </c>
@@ -7533,8 +8064,17 @@
       <c r="H230" t="s">
         <v>101</v>
       </c>
-    </row>
-    <row r="231" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J230">
+        <v>1.8</v>
+      </c>
+      <c r="K230">
+        <v>0</v>
+      </c>
+      <c r="L230">
+        <v>-3</v>
+      </c>
+    </row>
+    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>229</v>
       </c>
@@ -7559,8 +8099,17 @@
       <c r="H231" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="232" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J231">
+        <v>6</v>
+      </c>
+      <c r="K231">
+        <v>2.7</v>
+      </c>
+      <c r="L231">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>230</v>
       </c>
@@ -7586,7 +8135,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="233" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>231</v>
       </c>
@@ -7611,8 +8160,17 @@
       <c r="H233" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="234" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J233">
+        <v>0.1</v>
+      </c>
+      <c r="K233">
+        <v>3.2</v>
+      </c>
+      <c r="L233">
+        <v>-6</v>
+      </c>
+    </row>
+    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>232</v>
       </c>
@@ -7638,7 +8196,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="235" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>233</v>
       </c>
@@ -7667,7 +8225,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>234</v>
       </c>
@@ -7693,7 +8251,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>235</v>
       </c>
@@ -7719,7 +8277,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="238" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>236</v>
       </c>
@@ -7748,7 +8306,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="239" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>237</v>
       </c>
@@ -7777,12 +8335,12 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>238</v>
       </c>
       <c r="B240" t="s">
-        <v>329</v>
+        <v>328</v>
       </c>
       <c r="C240">
         <v>691</v>
@@ -7802,8 +8360,17 @@
       <c r="H240" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="241" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J240">
+        <v>6.9</v>
+      </c>
+      <c r="K240">
+        <v>3.5</v>
+      </c>
+      <c r="L240">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>239</v>
       </c>
@@ -7829,7 +8396,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="242" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>240</v>
       </c>
@@ -7854,8 +8421,17 @@
       <c r="H242" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="243" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J242">
+        <v>7.8</v>
+      </c>
+      <c r="K242">
+        <v>0.2</v>
+      </c>
+      <c r="L242">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>241</v>
       </c>
@@ -7880,8 +8456,17 @@
       <c r="H243" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="244" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J243">
+        <v>7.8</v>
+      </c>
+      <c r="K243">
+        <v>0.6</v>
+      </c>
+      <c r="L243">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>242</v>
       </c>
@@ -7910,7 +8495,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>243</v>
       </c>
@@ -7936,7 +8521,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="246" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>244</v>
       </c>
@@ -7961,8 +8546,17 @@
       <c r="H246" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="247" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J246">
+        <v>0.1</v>
+      </c>
+      <c r="K246">
+        <v>2.5</v>
+      </c>
+      <c r="L246">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>245</v>
       </c>
@@ -7991,7 +8585,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>246</v>
       </c>
@@ -8016,8 +8610,17 @@
       <c r="H248" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="249" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J248">
+        <v>0</v>
+      </c>
+      <c r="K248">
+        <v>1.9</v>
+      </c>
+      <c r="L248">
+        <v>-7</v>
+      </c>
+    </row>
+    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>247</v>
       </c>
@@ -8042,8 +8645,17 @@
       <c r="H249" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="250" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J249">
+        <v>0</v>
+      </c>
+      <c r="K249">
+        <v>97.6</v>
+      </c>
+      <c r="L249">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>248</v>
       </c>
@@ -8069,7 +8681,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="251" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>249</v>
       </c>
@@ -8094,8 +8706,17 @@
       <c r="H251" t="s">
         <v>176</v>
       </c>
-    </row>
-    <row r="252" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="J251">
+        <v>1</v>
+      </c>
+      <c r="K251">
+        <v>14.2</v>
+      </c>
+      <c r="L251">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>250</v>
       </c>
@@ -8121,7 +8742,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="253" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>251</v>
       </c>
@@ -8145,6 +8766,15 @@
       </c>
       <c r="H253" t="s">
         <v>32</v>
+      </c>
+      <c r="J253">
+        <v>0.2</v>
+      </c>
+      <c r="K253">
+        <v>4.8</v>
+      </c>
+      <c r="L253">
+        <v>-5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
updated database with own food product categories for new score
</commit_message>
<xml_diff>
--- a/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
+++ b/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\NutriLearnVR\NutriLearnVR\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{405CE51E-3F4F-4220-A0C9-481DF1B60309}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2A35BD-9D57-4774-860C-17B0036E902F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8C58FACA-B588-4A2F-A614-585794A6AB4A}"/>
   </bookViews>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="768" uniqueCount="346">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="356">
   <si>
     <t>ID</t>
   </si>
@@ -1077,6 +1077,36 @@
   </si>
   <si>
     <t>Zucker</t>
+  </si>
+  <si>
+    <t>Obst/Gemüse</t>
+  </si>
+  <si>
+    <t>Tierprodukte</t>
+  </si>
+  <si>
+    <t>Sonstiges</t>
+  </si>
+  <si>
+    <t>Milchprodukte</t>
+  </si>
+  <si>
+    <t>Vollkornprodukte</t>
+  </si>
+  <si>
+    <t>Gerichte</t>
+  </si>
+  <si>
+    <t>Backwaren</t>
+  </si>
+  <si>
+    <t>Nüsse</t>
+  </si>
+  <si>
+    <t>Kategorie NutriLearnVR</t>
+  </si>
+  <si>
+    <t>Gericht</t>
   </si>
 </sst>
 </file>
@@ -1454,11 +1484,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{05FB881A-4068-4DEA-B356-9AC1A56CFC86}">
-  <dimension ref="A1:L253"/>
+  <dimension ref="A1:M253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A79" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J91" sqref="J91"/>
+      <pane ySplit="1" topLeftCell="A220" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="M253" sqref="M253"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1468,9 +1498,10 @@
     <col min="7" max="7" width="22.5703125" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="32.140625" customWidth="1"/>
     <col min="9" max="9" width="19.28515625" customWidth="1"/>
+    <col min="13" max="13" width="16.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="3" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" s="3" customFormat="1" ht="141.75" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -1507,8 +1538,11 @@
       <c r="L1" s="1" t="s">
         <v>342</v>
       </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M1" s="1" t="s">
+        <v>354</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -1534,7 +1568,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1</v>
       </c>
@@ -1563,7 +1597,7 @@
         <v>1.32</v>
       </c>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>2</v>
       </c>
@@ -1589,7 +1623,7 @@
         <v>15</v>
       </c>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>3</v>
       </c>
@@ -1615,7 +1649,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>4</v>
       </c>
@@ -1644,7 +1678,7 @@
         <v>1.05</v>
       </c>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>5</v>
       </c>
@@ -1678,8 +1712,11 @@
       <c r="L7">
         <v>-4</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M7" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>6</v>
       </c>
@@ -1705,7 +1742,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>7</v>
       </c>
@@ -1731,7 +1768,7 @@
         <v>18</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>8</v>
       </c>
@@ -1760,7 +1797,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>9</v>
       </c>
@@ -1786,7 +1823,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>10</v>
       </c>
@@ -1812,7 +1849,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>11</v>
       </c>
@@ -1838,7 +1875,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>12</v>
       </c>
@@ -1872,8 +1909,11 @@
       <c r="L14">
         <v>12</v>
       </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M14" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>13</v>
       </c>
@@ -1907,8 +1947,11 @@
       <c r="L15">
         <v>-2</v>
       </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M15" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>14</v>
       </c>
@@ -1934,7 +1977,7 @@
         <v>314</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>15</v>
       </c>
@@ -1968,8 +2011,11 @@
       <c r="L17">
         <v>4</v>
       </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>16</v>
       </c>
@@ -2003,8 +2049,11 @@
       <c r="L18">
         <v>-3</v>
       </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>17</v>
       </c>
@@ -2030,7 +2079,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>18</v>
       </c>
@@ -2056,7 +2105,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>19</v>
       </c>
@@ -2082,7 +2131,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>20</v>
       </c>
@@ -2116,8 +2165,11 @@
       <c r="L22">
         <v>-7</v>
       </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>21</v>
       </c>
@@ -2146,7 +2198,7 @@
         <v>1.04</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>22</v>
       </c>
@@ -2172,7 +2224,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>23</v>
       </c>
@@ -2198,7 +2250,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>24</v>
       </c>
@@ -2224,7 +2276,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>25</v>
       </c>
@@ -2258,8 +2310,11 @@
       <c r="L27">
         <v>-6</v>
       </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>26</v>
       </c>
@@ -2296,8 +2351,11 @@
       <c r="L28">
         <v>20</v>
       </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M28" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>27</v>
       </c>
@@ -2331,8 +2389,11 @@
       <c r="L29">
         <v>11</v>
       </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M29" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>28</v>
       </c>
@@ -2358,7 +2419,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>29</v>
       </c>
@@ -2384,7 +2445,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>30</v>
       </c>
@@ -2418,8 +2479,11 @@
       <c r="L32">
         <v>8</v>
       </c>
-    </row>
-    <row r="33" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M32" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>31</v>
       </c>
@@ -2445,7 +2509,7 @@
         <v>69</v>
       </c>
     </row>
-    <row r="34" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>32</v>
       </c>
@@ -2479,8 +2543,11 @@
       <c r="L34">
         <v>19</v>
       </c>
-    </row>
-    <row r="35" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M34" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>33</v>
       </c>
@@ -2509,7 +2576,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>34</v>
       </c>
@@ -2543,8 +2610,11 @@
       <c r="L36">
         <v>14</v>
       </c>
-    </row>
-    <row r="37" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M36" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>35</v>
       </c>
@@ -2578,8 +2648,11 @@
       <c r="L37">
         <v>14</v>
       </c>
-    </row>
-    <row r="38" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M37" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>36</v>
       </c>
@@ -2605,7 +2678,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="39" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>37</v>
       </c>
@@ -2631,7 +2704,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="40" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>38</v>
       </c>
@@ -2665,8 +2738,11 @@
       <c r="L40">
         <v>2</v>
       </c>
-    </row>
-    <row r="41" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M40" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>39</v>
       </c>
@@ -2700,8 +2776,11 @@
       <c r="L41">
         <v>-2</v>
       </c>
-    </row>
-    <row r="42" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M41" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>40</v>
       </c>
@@ -2735,8 +2814,11 @@
       <c r="L42">
         <v>-5</v>
       </c>
-    </row>
-    <row r="43" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M42" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>41</v>
       </c>
@@ -2762,7 +2844,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="44" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>42</v>
       </c>
@@ -2788,7 +2870,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="45" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>43</v>
       </c>
@@ -2814,7 +2896,7 @@
         <v>61</v>
       </c>
     </row>
-    <row r="46" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>44</v>
       </c>
@@ -2840,7 +2922,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="47" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>45</v>
       </c>
@@ -2866,7 +2948,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="48" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>46</v>
       </c>
@@ -2900,8 +2982,11 @@
       <c r="L48">
         <v>8</v>
       </c>
-    </row>
-    <row r="49" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M48" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>47</v>
       </c>
@@ -2927,7 +3012,7 @@
         <v>94</v>
       </c>
     </row>
-    <row r="50" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>48</v>
       </c>
@@ -2961,8 +3046,11 @@
       <c r="L50">
         <v>14</v>
       </c>
-    </row>
-    <row r="51" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M50" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>49</v>
       </c>
@@ -2996,8 +3084,11 @@
       <c r="L51">
         <v>18</v>
       </c>
-    </row>
-    <row r="52" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M51" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>50</v>
       </c>
@@ -3023,7 +3114,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="53" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>51</v>
       </c>
@@ -3049,7 +3140,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="54" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>52</v>
       </c>
@@ -3083,8 +3174,11 @@
       <c r="L54">
         <v>4</v>
       </c>
-    </row>
-    <row r="55" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M54" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>53</v>
       </c>
@@ -3110,7 +3204,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="56" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>54</v>
       </c>
@@ -3136,7 +3230,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="57" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>55</v>
       </c>
@@ -3162,7 +3256,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="58" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>56</v>
       </c>
@@ -3188,7 +3282,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="59" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>57</v>
       </c>
@@ -3217,7 +3311,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="60" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>58</v>
       </c>
@@ -3243,7 +3337,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="61" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>59</v>
       </c>
@@ -3269,7 +3363,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="62" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>60</v>
       </c>
@@ -3295,7 +3389,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="63" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>61</v>
       </c>
@@ -3321,7 +3415,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="64" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>62</v>
       </c>
@@ -3347,7 +3441,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="65" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>63</v>
       </c>
@@ -3373,7 +3467,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="66" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>64</v>
       </c>
@@ -3407,8 +3501,11 @@
       <c r="L66">
         <v>15</v>
       </c>
-    </row>
-    <row r="67" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M66" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="67" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>65</v>
       </c>
@@ -3434,7 +3531,7 @@
         <v>102</v>
       </c>
     </row>
-    <row r="68" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>66</v>
       </c>
@@ -3460,7 +3557,7 @@
         <v>119</v>
       </c>
     </row>
-    <row r="69" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>67</v>
       </c>
@@ -3486,7 +3583,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="70" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>68</v>
       </c>
@@ -3512,7 +3609,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="71" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>69</v>
       </c>
@@ -3538,7 +3635,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="72" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>70</v>
       </c>
@@ -3564,7 +3661,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="73" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>71</v>
       </c>
@@ -3590,7 +3687,7 @@
         <v>321</v>
       </c>
     </row>
-    <row r="74" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>72</v>
       </c>
@@ -3616,7 +3713,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="75" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="75" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>73</v>
       </c>
@@ -3642,7 +3739,7 @@
         <v>103</v>
       </c>
     </row>
-    <row r="76" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="76" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>74</v>
       </c>
@@ -3668,7 +3765,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="77" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>75</v>
       </c>
@@ -3697,7 +3794,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="78" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>76</v>
       </c>
@@ -3726,7 +3823,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="79" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>77</v>
       </c>
@@ -3752,7 +3849,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="80" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="80" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>78</v>
       </c>
@@ -3778,7 +3875,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="81" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="81" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>79</v>
       </c>
@@ -3804,7 +3901,7 @@
         <v>135</v>
       </c>
     </row>
-    <row r="82" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="82" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>80</v>
       </c>
@@ -3830,7 +3927,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="83" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>81</v>
       </c>
@@ -3856,7 +3953,7 @@
         <v>322</v>
       </c>
     </row>
-    <row r="84" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>82</v>
       </c>
@@ -3882,7 +3979,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="85" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="85" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>83</v>
       </c>
@@ -3908,7 +4005,7 @@
         <v>143</v>
       </c>
     </row>
-    <row r="86" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="86" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>84</v>
       </c>
@@ -3942,8 +4039,11 @@
       <c r="L86">
         <v>-6</v>
       </c>
-    </row>
-    <row r="87" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M86" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="87" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>85</v>
       </c>
@@ -3969,7 +4069,7 @@
         <v>145</v>
       </c>
     </row>
-    <row r="88" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="88" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>86</v>
       </c>
@@ -4003,8 +4103,11 @@
       <c r="L88">
         <v>-5</v>
       </c>
-    </row>
-    <row r="89" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M88" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="89" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>87</v>
       </c>
@@ -4038,8 +4141,11 @@
       <c r="L89">
         <v>-6</v>
       </c>
-    </row>
-    <row r="90" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M89" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="90" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>88</v>
       </c>
@@ -4076,8 +4182,11 @@
       <c r="L90">
         <v>12</v>
       </c>
-    </row>
-    <row r="91" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M90" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="91" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>89</v>
       </c>
@@ -4103,7 +4212,7 @@
         <v>70</v>
       </c>
     </row>
-    <row r="92" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="92" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>90</v>
       </c>
@@ -4137,8 +4246,11 @@
       <c r="L92">
         <v>-3</v>
       </c>
-    </row>
-    <row r="93" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M92" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="93" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>91</v>
       </c>
@@ -4175,8 +4287,11 @@
       <c r="L93">
         <v>23</v>
       </c>
-    </row>
-    <row r="94" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M93" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="94" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>92</v>
       </c>
@@ -4202,7 +4317,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="95" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="95" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>93</v>
       </c>
@@ -4228,7 +4343,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="96" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="96" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>94</v>
       </c>
@@ -4254,7 +4369,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="97" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>95</v>
       </c>
@@ -4280,7 +4395,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="98" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>96</v>
       </c>
@@ -4317,8 +4432,11 @@
       <c r="L98">
         <v>13</v>
       </c>
-    </row>
-    <row r="99" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M98" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="99" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>97</v>
       </c>
@@ -4344,7 +4462,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="100" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="100" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>98</v>
       </c>
@@ -4370,7 +4488,7 @@
         <v>160</v>
       </c>
     </row>
-    <row r="101" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>99</v>
       </c>
@@ -4404,8 +4522,11 @@
       <c r="L101">
         <v>0</v>
       </c>
-    </row>
-    <row r="102" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M101" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="102" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>100</v>
       </c>
@@ -4431,7 +4552,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="103" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>101</v>
       </c>
@@ -4457,7 +4578,7 @@
         <v>165</v>
       </c>
     </row>
-    <row r="104" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>102</v>
       </c>
@@ -4486,7 +4607,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="105" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>103</v>
       </c>
@@ -4515,7 +4636,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="106" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>104</v>
       </c>
@@ -4544,7 +4665,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="107" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>105</v>
       </c>
@@ -4573,7 +4694,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="108" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>106</v>
       </c>
@@ -4599,7 +4720,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="109" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>107</v>
       </c>
@@ -4625,7 +4746,7 @@
         <v>316</v>
       </c>
     </row>
-    <row r="110" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="110" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>108</v>
       </c>
@@ -4651,7 +4772,7 @@
         <v>88</v>
       </c>
     </row>
-    <row r="111" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="111" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>109</v>
       </c>
@@ -4685,8 +4806,11 @@
       <c r="L111">
         <v>-3</v>
       </c>
-    </row>
-    <row r="112" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M111" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="112" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>110</v>
       </c>
@@ -4720,8 +4844,11 @@
       <c r="L112">
         <v>-6</v>
       </c>
-    </row>
-    <row r="113" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M112" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="113" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>111</v>
       </c>
@@ -4747,7 +4874,7 @@
         <v>125</v>
       </c>
     </row>
-    <row r="114" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="114" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>112</v>
       </c>
@@ -4776,7 +4903,7 @@
         <v>1.1399999999999999</v>
       </c>
     </row>
-    <row r="115" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="115" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>113</v>
       </c>
@@ -4810,8 +4937,11 @@
       <c r="L115">
         <v>24</v>
       </c>
-    </row>
-    <row r="116" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M115" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="116" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>114</v>
       </c>
@@ -4837,7 +4967,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="117" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="117" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>115</v>
       </c>
@@ -4871,8 +5001,11 @@
       <c r="L117">
         <v>0</v>
       </c>
-    </row>
-    <row r="118" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M117" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="118" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>116</v>
       </c>
@@ -4906,8 +5039,11 @@
       <c r="L118">
         <v>1</v>
       </c>
-    </row>
-    <row r="119" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M118" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="119" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>117</v>
       </c>
@@ -4941,8 +5077,11 @@
       <c r="L119">
         <v>10</v>
       </c>
-    </row>
-    <row r="120" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M119" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="120" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>118</v>
       </c>
@@ -4968,7 +5107,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="121" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="121" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>119</v>
       </c>
@@ -4994,7 +5133,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="122" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="122" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>120</v>
       </c>
@@ -5031,8 +5170,11 @@
       <c r="L122">
         <v>10</v>
       </c>
-    </row>
-    <row r="123" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M122" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="123" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>121</v>
       </c>
@@ -5058,7 +5200,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="124" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="124" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>122</v>
       </c>
@@ -5084,7 +5226,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="125" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="125" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>123</v>
       </c>
@@ -5110,7 +5252,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="126" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="126" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>124</v>
       </c>
@@ -5136,7 +5278,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="127" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="127" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>125</v>
       </c>
@@ -5165,7 +5307,7 @@
         <v>0.88</v>
       </c>
     </row>
-    <row r="128" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="128" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>126</v>
       </c>
@@ -5191,7 +5333,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="129" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="129" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>127</v>
       </c>
@@ -5217,7 +5359,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="130" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="130" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>128</v>
       </c>
@@ -5243,7 +5385,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="131" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="131" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>129</v>
       </c>
@@ -5277,8 +5419,11 @@
       <c r="L131">
         <v>-5</v>
       </c>
-    </row>
-    <row r="132" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M131" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="132" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>130</v>
       </c>
@@ -5312,8 +5457,11 @@
       <c r="L132">
         <v>-5</v>
       </c>
-    </row>
-    <row r="133" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M132" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="133" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>131</v>
       </c>
@@ -5347,8 +5495,11 @@
       <c r="L133">
         <v>-3</v>
       </c>
-    </row>
-    <row r="134" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M133" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="134" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>132</v>
       </c>
@@ -5374,7 +5525,7 @@
         <v>115</v>
       </c>
     </row>
-    <row r="135" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>133</v>
       </c>
@@ -5400,7 +5551,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="136" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="136" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>134</v>
       </c>
@@ -5426,7 +5577,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="137" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="137" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>135</v>
       </c>
@@ -5452,7 +5603,7 @@
         <v>318</v>
       </c>
     </row>
-    <row r="138" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="138" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>136</v>
       </c>
@@ -5478,7 +5629,7 @@
         <v>74</v>
       </c>
     </row>
-    <row r="139" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="139" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>137</v>
       </c>
@@ -5504,7 +5655,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="140" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="140" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>138</v>
       </c>
@@ -5541,8 +5692,11 @@
       <c r="L140">
         <v>14</v>
       </c>
-    </row>
-    <row r="141" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M140" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="141" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>139</v>
       </c>
@@ -5576,8 +5730,11 @@
       <c r="L141">
         <v>-5</v>
       </c>
-    </row>
-    <row r="142" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M141" t="s">
+        <v>350</v>
+      </c>
+    </row>
+    <row r="142" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>140</v>
       </c>
@@ -5606,7 +5763,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="143" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="143" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>141</v>
       </c>
@@ -5632,7 +5789,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="144" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="144" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>142</v>
       </c>
@@ -5658,7 +5815,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="145" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>143</v>
       </c>
@@ -5687,7 +5844,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="146" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>144</v>
       </c>
@@ -5716,7 +5873,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="147" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>145</v>
       </c>
@@ -5742,7 +5899,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="148" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>146</v>
       </c>
@@ -5768,7 +5925,7 @@
         <v>319</v>
       </c>
     </row>
-    <row r="149" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>147</v>
       </c>
@@ -5794,7 +5951,7 @@
         <v>92</v>
       </c>
     </row>
-    <row r="150" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="150" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>148</v>
       </c>
@@ -5820,7 +5977,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="151" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="151" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>149</v>
       </c>
@@ -5846,7 +6003,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="152" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="152" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>150</v>
       </c>
@@ -5880,8 +6037,11 @@
       <c r="L152">
         <v>-3</v>
       </c>
-    </row>
-    <row r="153" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M152" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="153" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>151</v>
       </c>
@@ -5915,8 +6075,11 @@
       <c r="L153">
         <v>23</v>
       </c>
-    </row>
-    <row r="154" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M153" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="154" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>152</v>
       </c>
@@ -5942,7 +6105,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="155" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="155" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>153</v>
       </c>
@@ -5968,7 +6131,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="156" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="156" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>154</v>
       </c>
@@ -6005,8 +6168,11 @@
       <c r="L156">
         <v>6</v>
       </c>
-    </row>
-    <row r="157" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M156" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="157" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>155</v>
       </c>
@@ -6040,8 +6206,11 @@
       <c r="L157">
         <v>-6</v>
       </c>
-    </row>
-    <row r="158" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M157" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="158" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>156</v>
       </c>
@@ -6078,8 +6247,11 @@
       <c r="L158">
         <v>14</v>
       </c>
-    </row>
-    <row r="159" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M158" t="s">
+        <v>348</v>
+      </c>
+    </row>
+    <row r="159" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>157</v>
       </c>
@@ -6113,8 +6285,11 @@
       <c r="L159">
         <v>-5</v>
       </c>
-    </row>
-    <row r="160" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M159" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="160" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>158</v>
       </c>
@@ -6140,7 +6315,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="161" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="161" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>159</v>
       </c>
@@ -6166,7 +6341,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="162" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="162" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>160</v>
       </c>
@@ -6192,7 +6367,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="163" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="163" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>161</v>
       </c>
@@ -6218,7 +6393,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="164" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="164" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>162</v>
       </c>
@@ -6244,7 +6419,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="165" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="165" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>163</v>
       </c>
@@ -6270,7 +6445,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="166" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="166" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>164</v>
       </c>
@@ -6296,7 +6471,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="167" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="167" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>165</v>
       </c>
@@ -6330,8 +6505,11 @@
       <c r="L167">
         <v>-5</v>
       </c>
-    </row>
-    <row r="168" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M167" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="168" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>166</v>
       </c>
@@ -6357,7 +6535,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="169" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="169" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>167</v>
       </c>
@@ -6383,7 +6561,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="170" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="170" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>168</v>
       </c>
@@ -6409,7 +6587,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="171" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="171" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>169</v>
       </c>
@@ -6435,7 +6613,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="172" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="172" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>170</v>
       </c>
@@ -6461,7 +6639,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="173" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="173" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>171</v>
       </c>
@@ -6487,7 +6665,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="174" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="174" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>172</v>
       </c>
@@ -6513,7 +6691,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="175" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="175" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>173</v>
       </c>
@@ -6539,7 +6717,7 @@
         <v>77</v>
       </c>
     </row>
-    <row r="176" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="176" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>174</v>
       </c>
@@ -6565,7 +6743,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="177" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="177" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>175</v>
       </c>
@@ -6591,7 +6769,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="178" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="178" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>176</v>
       </c>
@@ -6617,7 +6795,7 @@
         <v>113</v>
       </c>
     </row>
-    <row r="179" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="179" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>177</v>
       </c>
@@ -6651,8 +6829,11 @@
       <c r="L179">
         <v>-4</v>
       </c>
-    </row>
-    <row r="180" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M179" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="180" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>178</v>
       </c>
@@ -6678,7 +6859,7 @@
         <v>138</v>
       </c>
     </row>
-    <row r="181" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="181" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>179</v>
       </c>
@@ -6712,8 +6893,11 @@
       <c r="L181">
         <v>0</v>
       </c>
-    </row>
-    <row r="182" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M181" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="182" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>180</v>
       </c>
@@ -6739,7 +6923,7 @@
         <v>188</v>
       </c>
     </row>
-    <row r="183" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="183" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>181</v>
       </c>
@@ -6765,7 +6949,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="184" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="184" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>182</v>
       </c>
@@ -6799,8 +6983,11 @@
       <c r="L184">
         <v>-6</v>
       </c>
-    </row>
-    <row r="185" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M184" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="185" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>183</v>
       </c>
@@ -6829,7 +7016,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="186" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="186" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>184</v>
       </c>
@@ -6855,7 +7042,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="187" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="187" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>185</v>
       </c>
@@ -6881,7 +7068,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="188" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="188" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>186</v>
       </c>
@@ -6907,7 +7094,7 @@
         <v>241</v>
       </c>
     </row>
-    <row r="189" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>187</v>
       </c>
@@ -6933,7 +7120,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="190" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="190" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>188</v>
       </c>
@@ -6959,7 +7146,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="191" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="191" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>189</v>
       </c>
@@ -6985,7 +7172,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="192" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="192" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>190</v>
       </c>
@@ -7011,7 +7198,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="193" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="193" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>191</v>
       </c>
@@ -7037,7 +7224,7 @@
         <v>147</v>
       </c>
     </row>
-    <row r="194" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="194" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>192</v>
       </c>
@@ -7071,8 +7258,11 @@
       <c r="L194">
         <v>3</v>
       </c>
-    </row>
-    <row r="195" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M194" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="195" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>193</v>
       </c>
@@ -7098,7 +7288,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="196" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="196" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>194</v>
       </c>
@@ -7124,7 +7314,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="197" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="197" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>195</v>
       </c>
@@ -7158,8 +7348,11 @@
       <c r="L197">
         <v>-5</v>
       </c>
-    </row>
-    <row r="198" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M197" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="198" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>196</v>
       </c>
@@ -7185,7 +7378,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="199" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="199" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>197</v>
       </c>
@@ -7211,7 +7404,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="200" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="200" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>198</v>
       </c>
@@ -7245,8 +7438,11 @@
       <c r="L200">
         <v>24</v>
       </c>
-    </row>
-    <row r="201" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M200" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="201" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>199</v>
       </c>
@@ -7275,7 +7471,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="202" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="202" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>200</v>
       </c>
@@ -7304,7 +7500,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="203" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="203" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>201</v>
       </c>
@@ -7330,7 +7526,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="204" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="204" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>202</v>
       </c>
@@ -7356,7 +7552,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="205" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="205" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>203</v>
       </c>
@@ -7382,7 +7578,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="206" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="206" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>204</v>
       </c>
@@ -7408,7 +7604,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="207" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="207" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>205</v>
       </c>
@@ -7445,8 +7641,11 @@
       <c r="L207">
         <v>13</v>
       </c>
-    </row>
-    <row r="208" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M207" t="s">
+        <v>349</v>
+      </c>
+    </row>
+    <row r="208" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>206</v>
       </c>
@@ -7472,7 +7671,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="209" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="209" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>207</v>
       </c>
@@ -7498,7 +7697,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="210" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="210" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>208</v>
       </c>
@@ -7524,7 +7723,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="211" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="211" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>209</v>
       </c>
@@ -7550,7 +7749,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="212" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="212" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>210</v>
       </c>
@@ -7576,7 +7775,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="213" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="213" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>211</v>
       </c>
@@ -7602,7 +7801,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="214" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="214" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>212</v>
       </c>
@@ -7628,7 +7827,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="215" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="215" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>213</v>
       </c>
@@ -7654,7 +7853,7 @@
         <v>90</v>
       </c>
     </row>
-    <row r="216" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="216" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>214</v>
       </c>
@@ -7680,7 +7879,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="217" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="217" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>215</v>
       </c>
@@ -7706,7 +7905,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="218" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="218" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>216</v>
       </c>
@@ -7732,7 +7931,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="219" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="219" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>217</v>
       </c>
@@ -7758,7 +7957,7 @@
         <v>101</v>
       </c>
     </row>
-    <row r="220" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="220" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>218</v>
       </c>
@@ -7784,7 +7983,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="221" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="221" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>219</v>
       </c>
@@ -7818,8 +8017,11 @@
       <c r="L221">
         <v>7</v>
       </c>
-    </row>
-    <row r="222" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M221" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="222" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>220</v>
       </c>
@@ -7848,7 +8050,7 @@
         <v>0.9</v>
       </c>
     </row>
-    <row r="223" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="223" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>221</v>
       </c>
@@ -7874,7 +8076,7 @@
         <v>30</v>
       </c>
     </row>
-    <row r="224" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="224" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>222</v>
       </c>
@@ -7900,7 +8102,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="225" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="225" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>223</v>
       </c>
@@ -7934,8 +8136,11 @@
       <c r="L225">
         <v>12</v>
       </c>
-    </row>
-    <row r="226" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M225" t="s">
+        <v>351</v>
+      </c>
+    </row>
+    <row r="226" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>224</v>
       </c>
@@ -7961,7 +8166,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="227" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="227" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>225</v>
       </c>
@@ -7987,7 +8192,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="228" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="228" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>226</v>
       </c>
@@ -8013,7 +8218,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="229" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="229" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>227</v>
       </c>
@@ -8039,7 +8244,7 @@
         <v>163</v>
       </c>
     </row>
-    <row r="230" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="230" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>228</v>
       </c>
@@ -8073,8 +8278,11 @@
       <c r="L230">
         <v>-3</v>
       </c>
-    </row>
-    <row r="231" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M230" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="231" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>229</v>
       </c>
@@ -8108,8 +8316,11 @@
       <c r="L231">
         <v>11</v>
       </c>
-    </row>
-    <row r="232" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M231" t="s">
+        <v>355</v>
+      </c>
+    </row>
+    <row r="232" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>230</v>
       </c>
@@ -8135,7 +8346,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="233" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="233" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>231</v>
       </c>
@@ -8169,8 +8380,11 @@
       <c r="L233">
         <v>-6</v>
       </c>
-    </row>
-    <row r="234" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M233" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="234" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>232</v>
       </c>
@@ -8196,7 +8410,7 @@
         <v>49</v>
       </c>
     </row>
-    <row r="235" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="235" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>233</v>
       </c>
@@ -8225,7 +8439,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="236" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="236" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>234</v>
       </c>
@@ -8251,7 +8465,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="237" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="237" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>235</v>
       </c>
@@ -8277,7 +8491,7 @@
         <v>268</v>
       </c>
     </row>
-    <row r="238" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="238" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>236</v>
       </c>
@@ -8306,7 +8520,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="239" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="239" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>237</v>
       </c>
@@ -8335,7 +8549,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="240" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="240" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>238</v>
       </c>
@@ -8369,8 +8583,11 @@
       <c r="L240">
         <v>-1</v>
       </c>
-    </row>
-    <row r="241" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M240" t="s">
+        <v>353</v>
+      </c>
+    </row>
+    <row r="241" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>239</v>
       </c>
@@ -8396,7 +8613,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="242" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="242" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>240</v>
       </c>
@@ -8430,8 +8647,11 @@
       <c r="L242">
         <v>3</v>
       </c>
-    </row>
-    <row r="243" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M242" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="243" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>241</v>
       </c>
@@ -8465,8 +8685,11 @@
       <c r="L243">
         <v>19</v>
       </c>
-    </row>
-    <row r="244" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M243" t="s">
+        <v>347</v>
+      </c>
+    </row>
+    <row r="244" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>242</v>
       </c>
@@ -8495,7 +8718,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="245" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="245" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>243</v>
       </c>
@@ -8521,7 +8744,7 @@
         <v>17</v>
       </c>
     </row>
-    <row r="246" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="246" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>244</v>
       </c>
@@ -8555,8 +8778,11 @@
       <c r="L246">
         <v>-7</v>
       </c>
-    </row>
-    <row r="247" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M246" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="247" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>245</v>
       </c>
@@ -8585,7 +8811,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="248" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="248" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>246</v>
       </c>
@@ -8619,8 +8845,11 @@
       <c r="L248">
         <v>-7</v>
       </c>
-    </row>
-    <row r="249" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M248" t="s">
+        <v>346</v>
+      </c>
+    </row>
+    <row r="249" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>247</v>
       </c>
@@ -8654,8 +8883,11 @@
       <c r="L249">
         <v>14</v>
       </c>
-    </row>
-    <row r="250" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M249" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="250" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>248</v>
       </c>
@@ -8681,7 +8913,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="251" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="251" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>249</v>
       </c>
@@ -8715,8 +8947,11 @@
       <c r="L251">
         <v>10</v>
       </c>
-    </row>
-    <row r="252" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="M251" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="252" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>250</v>
       </c>
@@ -8742,7 +8977,7 @@
         <v>176</v>
       </c>
     </row>
-    <row r="253" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="253" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>251</v>
       </c>
@@ -8775,6 +9010,9 @@
       </c>
       <c r="L253">
         <v>-5</v>
+      </c>
+      <c r="M253" t="s">
+        <v>346</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added last missing food products to compute nutri values and updated db
</commit_message>
<xml_diff>
--- a/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
+++ b/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\NutriLearnVR\NutriLearnVR\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EB2A35BD-9D57-4774-860C-17B0036E902F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DF4839-7936-4AA1-8549-9651ED083412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{8C58FACA-B588-4A2F-A614-585794A6AB4A}"/>
+    <workbookView xWindow="38280" yWindow="5175" windowWidth="29040" windowHeight="15720" xr2:uid="{8C58FACA-B588-4A2F-A614-585794A6AB4A}"/>
   </bookViews>
   <sheets>
     <sheet name="Generische Lebensmittel" sheetId="1" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="837" uniqueCount="356">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="842" uniqueCount="356">
   <si>
     <t>ID</t>
   </si>
@@ -1487,8 +1487,8 @@
   <dimension ref="A1:M253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A220" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="M253" sqref="M253"/>
+      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="J84" sqref="J84"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3952,6 +3952,18 @@
       <c r="H83" t="s">
         <v>322</v>
       </c>
+      <c r="J83">
+        <v>0.1</v>
+      </c>
+      <c r="K83">
+        <v>0.1</v>
+      </c>
+      <c r="L83">
+        <v>-4</v>
+      </c>
+      <c r="M83" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="84" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A84">
@@ -4487,6 +4499,18 @@
       <c r="H100" t="s">
         <v>160</v>
       </c>
+      <c r="J100">
+        <v>3.3</v>
+      </c>
+      <c r="K100">
+        <v>0.5</v>
+      </c>
+      <c r="L100">
+        <v>0</v>
+      </c>
+      <c r="M100" t="s">
+        <v>347</v>
+      </c>
     </row>
     <row r="101" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A101">
@@ -5524,6 +5548,18 @@
       <c r="H134" t="s">
         <v>115</v>
       </c>
+      <c r="J134">
+        <v>4.0999999999999996</v>
+      </c>
+      <c r="K134">
+        <v>6.6</v>
+      </c>
+      <c r="L134">
+        <v>-3</v>
+      </c>
+      <c r="M134" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="135" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A135">
@@ -7093,6 +7129,18 @@
       <c r="H188" t="s">
         <v>241</v>
       </c>
+      <c r="J188">
+        <v>0.3</v>
+      </c>
+      <c r="K188">
+        <v>0.5</v>
+      </c>
+      <c r="L188">
+        <v>-4</v>
+      </c>
+      <c r="M188" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="189" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A189">
@@ -7721,6 +7769,18 @@
       </c>
       <c r="H210" t="s">
         <v>62</v>
+      </c>
+      <c r="J210">
+        <v>10.199999999999999</v>
+      </c>
+      <c r="K210">
+        <v>11.2</v>
+      </c>
+      <c r="L210">
+        <v>21</v>
+      </c>
+      <c r="M210" t="s">
+        <v>349</v>
       </c>
     </row>
     <row r="211" spans="1:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
user test update and disabled console logger after running all tests
</commit_message>
<xml_diff>
--- a/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
+++ b/NutriLearnVR/Assets/FoodProducts_NutriLearn.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27029"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\repos\NutriLearnVR\NutriLearnVR\Assets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7DF4839-7936-4AA1-8549-9651ED083412}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3597BA76-57B5-40C9-956E-8897C917EA17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="5175" windowWidth="29040" windowHeight="15720" xr2:uid="{8C58FACA-B588-4A2F-A614-585794A6AB4A}"/>
   </bookViews>
@@ -1188,9 +1188,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 – 2022-Design">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 – 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1228,7 +1228,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 – 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1334,7 +1334,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 – 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1476,7 +1476,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1487,8 +1487,8 @@
   <dimension ref="A1:M253"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A64" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J84" sqref="J84"/>
+      <pane ySplit="1" topLeftCell="A103" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F116" sqref="F116"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4944,7 +4944,7 @@
         <v>40.1</v>
       </c>
       <c r="F115">
-        <v>734</v>
+        <v>7.3</v>
       </c>
       <c r="G115" t="s">
         <v>9</v>

</xml_diff>